<commit_message>
Update monkeypox data and excess mortality
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZELST007\Desktop\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3AD36E-E4FA-45F0-B0CE-1B577433E763}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C026C5-E721-46D3-A5C3-76979BE71B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,16 +1419,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH107" sqref="AH107"/>
+    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG128" sqref="AG128"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>-16.670000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>-4.58</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>-3.35</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-8.4600000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>-12.77</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>-12.09</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>-2.96</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>29.57</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>96.39</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>136.1</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>108.97</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>82.17</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>60.18</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>27.03</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>13.24</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>18.059999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>12.74</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>-8.02</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>-6.57</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>-3.26</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>-12.96</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>-14.15</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>-0.96</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>-3.81</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>-13.62</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>-10.7</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>-2.34</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>13.39</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>-3.13</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>7.73</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>22.03</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>17.649999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>21.69</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>27.09</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -8749,7 +8749,7 @@
         <v>33.46</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>16.920000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>24.62</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>-2.19</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>6.86</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>-8.99</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>-18.84</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>-13.19</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>-10.11</v>
       </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -10059,7 +10059,7 @@
         <v>-17.760000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -10190,7 +10190,7 @@
         <v>-1.99</v>
       </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -10321,7 +10321,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -10452,7 +10452,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>14.66</v>
       </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>16.29</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>17.89</v>
       </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -11238,7 +11238,7 @@
         <v>-3.24</v>
       </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -11369,7 +11369,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -11500,7 +11500,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -11762,7 +11762,7 @@
         <v>-11.16</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -11893,7 +11893,7 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>16.59</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -12417,7 +12417,7 @@
         <v>13.49</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>9.39</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>-0.93</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -12810,7 +12810,7 @@
         <v>17.54</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -13072,7 +13072,7 @@
         <v>-8.57</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -13334,7 +13334,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>105</v>
       </c>
@@ -13596,7 +13596,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -13727,7 +13727,7 @@
         <v>8.14</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -13858,7 +13858,7 @@
         <v>6.73</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -13989,7 +13989,7 @@
         <v>26.99</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>32.46</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -14382,7 +14382,7 @@
         <v>47.83</v>
       </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -14644,7 +14644,7 @@
         <v>75.849999999999994</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>114</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>69.33</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>115</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>116</v>
       </c>
@@ -15037,7 +15037,7 @@
         <v>45.68</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>117</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>118</v>
       </c>
@@ -15299,7 +15299,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>119</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>131</v>
       </c>
       <c r="S107">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="T107">
         <v>55</v>
@@ -15395,7 +15395,7 @@
       </c>
       <c r="AH107">
         <f t="shared" si="15"/>
-        <v>8.6999999999999993</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="AI107">
         <f t="shared" si="16"/>
@@ -15430,7 +15430,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>120</v>
       </c>
@@ -15561,7 +15561,7 @@
         <v>-10.85</v>
       </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -15692,7 +15692,7 @@
         <v>-9.58</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>122</v>
       </c>
@@ -15748,7 +15748,7 @@
         <v>47</v>
       </c>
       <c r="U110">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="V110">
         <v>217</v>
@@ -15796,7 +15796,7 @@
       </c>
       <c r="AJ110">
         <f t="shared" si="29"/>
-        <v>-8.86</v>
+        <v>-8.6199999999999992</v>
       </c>
       <c r="AK110">
         <f t="shared" si="30"/>
@@ -15823,7 +15823,7 @@
         <v>-4.8899999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -15867,19 +15867,19 @@
         <v>110</v>
       </c>
       <c r="Q111">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="R111">
         <v>122</v>
       </c>
       <c r="S111">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="T111">
         <v>62</v>
       </c>
       <c r="U111">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="V111">
         <v>196</v>
@@ -15911,7 +15911,7 @@
       </c>
       <c r="AF111">
         <f t="shared" si="25"/>
-        <v>-1.42</v>
+        <v>-0.71</v>
       </c>
       <c r="AG111">
         <f t="shared" si="26"/>
@@ -15919,7 +15919,7 @@
       </c>
       <c r="AH111">
         <f t="shared" si="27"/>
-        <v>7.17</v>
+        <v>7.59</v>
       </c>
       <c r="AI111">
         <f t="shared" si="28"/>
@@ -15927,7 +15927,7 @@
       </c>
       <c r="AJ111">
         <f t="shared" si="29"/>
-        <v>-7.66</v>
+        <v>-7.42</v>
       </c>
       <c r="AK111">
         <f t="shared" si="30"/>
@@ -15954,7 +15954,7 @@
         <v>-12.82</v>
       </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>124</v>
       </c>
@@ -16016,10 +16016,10 @@
         <v>242</v>
       </c>
       <c r="W112">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="X112">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="Y112">
         <v>100</v>
@@ -16066,11 +16066,11 @@
       </c>
       <c r="AL112">
         <f t="shared" si="31"/>
-        <v>0.56999999999999995</v>
+        <v>0.76</v>
       </c>
       <c r="AM112">
         <f t="shared" si="32"/>
-        <v>-4.01</v>
+        <v>-3.58</v>
       </c>
       <c r="AN112">
         <f t="shared" si="33"/>
@@ -16085,7 +16085,7 @@
         <v>-12.73</v>
       </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>125</v>
       </c>
@@ -16144,13 +16144,13 @@
         <v>437</v>
       </c>
       <c r="V113">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="W113">
         <v>515</v>
       </c>
       <c r="X113">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="Y113">
         <v>103</v>
@@ -16193,7 +16193,7 @@
       </c>
       <c r="AK113">
         <f t="shared" si="30"/>
-        <v>-8.23</v>
+        <v>-7.79</v>
       </c>
       <c r="AL113">
         <f t="shared" si="31"/>
@@ -16201,7 +16201,7 @@
       </c>
       <c r="AM113">
         <f t="shared" si="32"/>
-        <v>-1.1499999999999999</v>
+        <v>-1.01</v>
       </c>
       <c r="AN113">
         <f t="shared" si="33"/>
@@ -16216,7 +16216,7 @@
         <v>-7.19</v>
       </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -16281,13 +16281,13 @@
         <v>473</v>
       </c>
       <c r="X114">
-        <v>660</v>
+        <v>662</v>
       </c>
       <c r="Y114">
         <v>95</v>
       </c>
       <c r="Z114">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="AA114">
         <v>264</v>
@@ -16332,7 +16332,7 @@
       </c>
       <c r="AM114">
         <f t="shared" si="32"/>
-        <v>-4.07</v>
+        <v>-3.78</v>
       </c>
       <c r="AN114">
         <f t="shared" si="33"/>
@@ -16340,14 +16340,14 @@
       </c>
       <c r="AO114">
         <f t="shared" si="34"/>
-        <v>1.7</v>
+        <v>1.89</v>
       </c>
       <c r="AP114">
         <f t="shared" si="35"/>
         <v>-5.71</v>
       </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -16478,7 +16478,7 @@
         <v>-6.86</v>
       </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>128</v>
       </c>
@@ -16528,7 +16528,7 @@
         <v>101</v>
       </c>
       <c r="S116">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="T116">
         <v>44</v>
@@ -16543,7 +16543,7 @@
         <v>524</v>
       </c>
       <c r="X116">
-        <v>675</v>
+        <v>677</v>
       </c>
       <c r="Y116">
         <v>84</v>
@@ -16552,7 +16552,7 @@
         <v>540</v>
       </c>
       <c r="AA116">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AC116">
         <v>2022</v>
@@ -16574,7 +16574,7 @@
       </c>
       <c r="AH116">
         <f t="shared" si="27"/>
-        <v>7.96</v>
+        <v>8.41</v>
       </c>
       <c r="AI116">
         <f t="shared" si="28"/>
@@ -16594,7 +16594,7 @@
       </c>
       <c r="AM116">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AN116">
         <f t="shared" si="33"/>
@@ -16606,10 +16606,10 @@
       </c>
       <c r="AP116">
         <f t="shared" si="35"/>
-        <v>0.73</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -16653,28 +16653,28 @@
         <v>126</v>
       </c>
       <c r="Q117">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="R117">
         <v>118</v>
       </c>
       <c r="S117">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="T117">
         <v>68</v>
       </c>
       <c r="U117">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="V117">
         <v>236</v>
       </c>
       <c r="W117">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="X117">
-        <v>669</v>
+        <v>673</v>
       </c>
       <c r="Y117">
         <v>113</v>
@@ -16697,7 +16697,7 @@
       </c>
       <c r="AF117">
         <f t="shared" si="25"/>
-        <v>5.71</v>
+        <v>6.43</v>
       </c>
       <c r="AG117">
         <f t="shared" si="26"/>
@@ -16705,7 +16705,7 @@
       </c>
       <c r="AH117">
         <f t="shared" si="27"/>
-        <v>3.15</v>
+        <v>3.6</v>
       </c>
       <c r="AI117">
         <f t="shared" si="28"/>
@@ -16713,7 +16713,7 @@
       </c>
       <c r="AJ117">
         <f t="shared" si="29"/>
-        <v>13.45</v>
+        <v>13.69</v>
       </c>
       <c r="AK117">
         <f t="shared" si="30"/>
@@ -16721,11 +16721,11 @@
       </c>
       <c r="AL117">
         <f t="shared" si="31"/>
-        <v>3.84</v>
+        <v>4.04</v>
       </c>
       <c r="AM117">
         <f t="shared" si="32"/>
-        <v>1.06</v>
+        <v>1.66</v>
       </c>
       <c r="AN117">
         <f t="shared" si="33"/>
@@ -16740,7 +16740,7 @@
         <v>10.45</v>
       </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>130</v>
       </c>
@@ -16787,7 +16787,7 @@
         <v>138</v>
       </c>
       <c r="R118">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="S118">
         <v>205</v>
@@ -16799,22 +16799,22 @@
         <v>458</v>
       </c>
       <c r="V118">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="W118">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="X118">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="Y118">
         <v>82</v>
       </c>
       <c r="Z118">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="AA118">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AC118">
         <v>2022</v>
@@ -16832,7 +16832,7 @@
       </c>
       <c r="AG118">
         <f t="shared" si="26"/>
-        <v>9.26</v>
+        <v>10.19</v>
       </c>
       <c r="AH118">
         <f t="shared" si="27"/>
@@ -16848,15 +16848,15 @@
       </c>
       <c r="AK118">
         <f t="shared" si="30"/>
-        <v>13.95</v>
+        <v>14.42</v>
       </c>
       <c r="AL118">
         <f t="shared" si="31"/>
-        <v>8.9</v>
+        <v>9.52</v>
       </c>
       <c r="AM118">
         <f t="shared" si="32"/>
-        <v>10.63</v>
+        <v>11.25</v>
       </c>
       <c r="AN118">
         <f t="shared" si="33"/>
@@ -16864,14 +16864,14 @@
       </c>
       <c r="AO118">
         <f t="shared" si="34"/>
-        <v>23.73</v>
+        <v>24.14</v>
       </c>
       <c r="AP118">
         <f t="shared" si="35"/>
-        <v>21.92</v>
+        <v>22.31</v>
       </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>131</v>
       </c>
@@ -16921,7 +16921,7 @@
         <v>128</v>
       </c>
       <c r="S119">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="T119">
         <v>79</v>
@@ -16933,16 +16933,16 @@
         <v>237</v>
       </c>
       <c r="W119">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="X119">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="Y119">
         <v>97</v>
       </c>
       <c r="Z119">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AA119">
         <v>250</v>
@@ -16967,7 +16967,7 @@
       </c>
       <c r="AH119">
         <f t="shared" si="27"/>
-        <v>16.670000000000002</v>
+        <v>16.2</v>
       </c>
       <c r="AI119">
         <f t="shared" si="28"/>
@@ -16983,11 +16983,11 @@
       </c>
       <c r="AL119">
         <f t="shared" si="31"/>
-        <v>19.239999999999998</v>
+        <v>19.66</v>
       </c>
       <c r="AM119">
         <f t="shared" si="32"/>
-        <v>13.9</v>
+        <v>14.22</v>
       </c>
       <c r="AN119">
         <f t="shared" si="33"/>
@@ -16995,14 +16995,14 @@
       </c>
       <c r="AO119">
         <f t="shared" si="34"/>
-        <v>4.8</v>
+        <v>5.01</v>
       </c>
       <c r="AP119">
         <f t="shared" si="35"/>
         <v>-0.79</v>
       </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>132</v>
       </c>
@@ -17052,7 +17052,7 @@
         <v>121</v>
       </c>
       <c r="S120">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="T120">
         <v>51</v>
@@ -17064,10 +17064,10 @@
         <v>239</v>
       </c>
       <c r="W120">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="X120">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="Y120">
         <v>97</v>
@@ -17098,7 +17098,7 @@
       </c>
       <c r="AH120">
         <f t="shared" si="27"/>
-        <v>27.23</v>
+        <v>27.7</v>
       </c>
       <c r="AI120">
         <f t="shared" si="28"/>
@@ -17114,11 +17114,11 @@
       </c>
       <c r="AL120">
         <f t="shared" si="31"/>
-        <v>17.53</v>
+        <v>17.75</v>
       </c>
       <c r="AM120">
         <f t="shared" si="32"/>
-        <v>18.34</v>
+        <v>18.510000000000002</v>
       </c>
       <c r="AN120">
         <f t="shared" si="33"/>
@@ -17133,7 +17133,7 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>133</v>
       </c>
@@ -17183,7 +17183,7 @@
         <v>128</v>
       </c>
       <c r="S121">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="T121">
         <v>54</v>
@@ -17195,13 +17195,13 @@
         <v>235</v>
       </c>
       <c r="W121">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="X121">
-        <v>655</v>
+        <v>657</v>
       </c>
       <c r="Y121">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Z121">
         <v>502</v>
@@ -17229,7 +17229,7 @@
       </c>
       <c r="AH121">
         <f t="shared" si="27"/>
-        <v>15.79</v>
+        <v>16.27</v>
       </c>
       <c r="AI121">
         <f t="shared" si="28"/>
@@ -17245,15 +17245,15 @@
       </c>
       <c r="AL121">
         <f t="shared" si="31"/>
-        <v>22.74</v>
+        <v>22.96</v>
       </c>
       <c r="AM121">
         <f t="shared" si="32"/>
-        <v>8.26</v>
+        <v>8.6</v>
       </c>
       <c r="AN121">
         <f t="shared" si="33"/>
-        <v>37.18</v>
+        <v>38.46</v>
       </c>
       <c r="AO121">
         <f t="shared" si="34"/>
@@ -17264,7 +17264,7 @@
         <v>27.85</v>
       </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>134</v>
       </c>
@@ -17320,25 +17320,25 @@
         <v>55</v>
       </c>
       <c r="U122">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="V122">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="W122">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="X122">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="Y122">
         <v>62</v>
       </c>
       <c r="Z122">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="AA122">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="AC122">
         <v>2022</v>
@@ -17368,19 +17368,19 @@
       </c>
       <c r="AJ122">
         <f t="shared" ref="AJ122" si="41">ROUND((U122-G122)/G122*100,2)</f>
-        <v>19.399999999999999</v>
+        <v>19.95</v>
       </c>
       <c r="AK122">
         <f t="shared" ref="AK122" si="42">ROUND((V122-H122)/H122*100,2)</f>
-        <v>-2.0099999999999998</v>
+        <v>-1.51</v>
       </c>
       <c r="AL122">
         <f t="shared" ref="AL122" si="43">ROUND((W122-I122)/I122*100,2)</f>
-        <v>16.809999999999999</v>
+        <v>17.7</v>
       </c>
       <c r="AM122">
         <f t="shared" ref="AM122" si="44">ROUND((X122-J122)/J122*100,2)</f>
-        <v>-3.19</v>
+        <v>-2.35</v>
       </c>
       <c r="AN122">
         <f t="shared" ref="AN122" si="45">ROUND((Y122-K122)/K122*100,2)</f>
@@ -17388,14 +17388,14 @@
       </c>
       <c r="AO122">
         <f t="shared" ref="AO122" si="46">ROUND((Z122-L122)/L122*100,2)</f>
-        <v>5.84</v>
+        <v>6.29</v>
       </c>
       <c r="AP122">
         <f t="shared" ref="AP122" si="47">ROUND((AA122-M122)/M122*100,2)</f>
-        <v>13.73</v>
+        <v>15.02</v>
       </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -17439,34 +17439,34 @@
         <v>109</v>
       </c>
       <c r="Q123">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R123">
         <v>115</v>
       </c>
       <c r="S123">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="T123">
         <v>58</v>
       </c>
       <c r="U123">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="V123">
         <v>214</v>
       </c>
       <c r="W123">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="X123">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="Y123">
         <v>88</v>
       </c>
       <c r="Z123">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="AA123">
         <v>229</v>
@@ -17483,7 +17483,7 @@
       </c>
       <c r="AF123">
         <f t="shared" ref="AF123:AF124" si="49">ROUND((Q123-C123)/C123*100,2)</f>
-        <v>18.850000000000001</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="AG123">
         <f t="shared" ref="AG123:AG124" si="50">ROUND((R123-D123)/D123*100,2)</f>
@@ -17491,7 +17491,7 @@
       </c>
       <c r="AH123">
         <f t="shared" ref="AH123:AH124" si="51">ROUND((S123-E123)/E123*100,2)</f>
-        <v>-0.5</v>
+        <v>1.49</v>
       </c>
       <c r="AI123">
         <f t="shared" ref="AI123:AI124" si="52">ROUND((T123-F123)/F123*100,2)</f>
@@ -17499,7 +17499,7 @@
       </c>
       <c r="AJ123">
         <f t="shared" ref="AJ123:AJ124" si="53">ROUND((U123-G123)/G123*100,2)</f>
-        <v>8.31</v>
+        <v>8.86</v>
       </c>
       <c r="AK123">
         <f t="shared" ref="AK123:AK124" si="54">ROUND((V123-H123)/H123*100,2)</f>
@@ -17507,11 +17507,11 @@
       </c>
       <c r="AL123">
         <f t="shared" ref="AL123:AL124" si="55">ROUND((W123-I123)/I123*100,2)</f>
-        <v>-1.57</v>
+        <v>-0.22</v>
       </c>
       <c r="AM123">
         <f t="shared" ref="AM123:AM124" si="56">ROUND((X123-J123)/J123*100,2)</f>
-        <v>15.48</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="AN123">
         <f t="shared" ref="AN123:AN124" si="57">ROUND((Y123-K123)/K123*100,2)</f>
@@ -17519,14 +17519,14 @@
       </c>
       <c r="AO123">
         <f t="shared" ref="AO123:AO124" si="58">ROUND((Z123-L123)/L123*100,2)</f>
-        <v>2.06</v>
+        <v>2.52</v>
       </c>
       <c r="AP123">
         <f t="shared" ref="AP123:AP124" si="59">ROUND((AA123-M123)/M123*100,2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>136</v>
       </c>
@@ -17567,10 +17567,10 @@
         <v>225</v>
       </c>
       <c r="P124">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q124">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="R124">
         <v>110</v>
@@ -17582,25 +17582,25 @@
         <v>54</v>
       </c>
       <c r="U124">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="V124">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="W124">
-        <v>471</v>
+        <v>484</v>
       </c>
       <c r="X124">
-        <v>625</v>
+        <v>635</v>
       </c>
       <c r="Y124">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Z124">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="AA124">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="AC124">
         <v>2022</v>
@@ -17610,11 +17610,11 @@
       </c>
       <c r="AE124">
         <f t="shared" si="48"/>
-        <v>25.23</v>
+        <v>26.17</v>
       </c>
       <c r="AF124">
         <f t="shared" si="49"/>
-        <v>-1.65</v>
+        <v>-0.83</v>
       </c>
       <c r="AG124">
         <f t="shared" si="50"/>
@@ -17630,34 +17630,34 @@
       </c>
       <c r="AJ124">
         <f t="shared" si="53"/>
-        <v>0.28000000000000003</v>
+        <v>0.84</v>
       </c>
       <c r="AK124">
         <f t="shared" si="54"/>
-        <v>5.15</v>
+        <v>6.7</v>
       </c>
       <c r="AL124">
         <f t="shared" si="55"/>
-        <v>6.32</v>
+        <v>9.26</v>
       </c>
       <c r="AM124">
         <f t="shared" si="56"/>
-        <v>7.39</v>
+        <v>9.11</v>
       </c>
       <c r="AN124">
         <f t="shared" si="57"/>
-        <v>-9.33</v>
+        <v>-8</v>
       </c>
       <c r="AO124">
         <f t="shared" si="58"/>
-        <v>11.63</v>
+        <v>12.33</v>
       </c>
       <c r="AP124">
         <f t="shared" si="59"/>
-        <v>9.33</v>
+        <v>11.56</v>
       </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>137</v>
       </c>
@@ -17698,40 +17698,40 @@
         <v>222</v>
       </c>
       <c r="P125">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="Q125">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="R125">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="S125">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="T125">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="U125">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="V125">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="W125">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="X125">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="Y125">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="Z125">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="AA125">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="AC125">
         <v>2022</v>
@@ -17740,55 +17740,55 @@
         <v>19</v>
       </c>
       <c r="AE125">
-        <f t="shared" ref="AE125" si="60">ROUND((P125-B125)/B125*100,2)</f>
-        <v>21.7</v>
+        <f t="shared" ref="AE125:AE126" si="60">ROUND((P125-B125)/B125*100,2)</f>
+        <v>18.87</v>
       </c>
       <c r="AF125">
-        <f t="shared" ref="AF125" si="61">ROUND((Q125-C125)/C125*100,2)</f>
-        <v>5</v>
+        <f t="shared" ref="AF125:AF126" si="61">ROUND((Q125-C125)/C125*100,2)</f>
+        <v>10</v>
       </c>
       <c r="AG125">
-        <f t="shared" ref="AG125" si="62">ROUND((R125-D125)/D125*100,2)</f>
-        <v>15</v>
+        <f t="shared" ref="AG125:AG126" si="62">ROUND((R125-D125)/D125*100,2)</f>
+        <v>10</v>
       </c>
       <c r="AH125">
-        <f t="shared" ref="AH125" si="63">ROUND((S125-E125)/E125*100,2)</f>
-        <v>3.54</v>
+        <f t="shared" ref="AH125:AH126" si="63">ROUND((S125-E125)/E125*100,2)</f>
+        <v>1.01</v>
       </c>
       <c r="AI125">
-        <f t="shared" ref="AI125" si="64">ROUND((T125-F125)/F125*100,2)</f>
-        <v>18.600000000000001</v>
+        <f t="shared" ref="AI125:AI126" si="64">ROUND((T125-F125)/F125*100,2)</f>
+        <v>25.58</v>
       </c>
       <c r="AJ125">
-        <f t="shared" ref="AJ125" si="65">ROUND((U125-G125)/G125*100,2)</f>
-        <v>15.13</v>
+        <f t="shared" ref="AJ125:AJ126" si="65">ROUND((U125-G125)/G125*100,2)</f>
+        <v>15.97</v>
       </c>
       <c r="AK125">
-        <f t="shared" ref="AK125" si="66">ROUND((V125-H125)/H125*100,2)</f>
-        <v>8.85</v>
+        <f t="shared" ref="AK125:AK126" si="66">ROUND((V125-H125)/H125*100,2)</f>
+        <v>7.81</v>
       </c>
       <c r="AL125">
-        <f t="shared" ref="AL125" si="67">ROUND((W125-I125)/I125*100,2)</f>
-        <v>15.12</v>
+        <f t="shared" ref="AL125:AL126" si="67">ROUND((W125-I125)/I125*100,2)</f>
+        <v>15.8</v>
       </c>
       <c r="AM125">
-        <f t="shared" ref="AM125" si="68">ROUND((X125-J125)/J125*100,2)</f>
+        <f t="shared" ref="AM125:AM126" si="68">ROUND((X125-J125)/J125*100,2)</f>
+        <v>1.04</v>
+      </c>
+      <c r="AN125">
+        <f t="shared" ref="AN125:AN126" si="69">ROUND((Y125-K125)/K125*100,2)</f>
+        <v>22.97</v>
+      </c>
+      <c r="AO125">
+        <f t="shared" ref="AO125:AO126" si="70">ROUND((Z125-L125)/L125*100,2)</f>
+        <v>7.46</v>
+      </c>
+      <c r="AP125">
+        <f t="shared" ref="AP125:AP126" si="71">ROUND((AA125-M125)/M125*100,2)</f>
         <v>2.25</v>
       </c>
-      <c r="AN125">
-        <f t="shared" ref="AN125" si="69">ROUND((Y125-K125)/K125*100,2)</f>
-        <v>29.73</v>
-      </c>
-      <c r="AO125">
-        <f t="shared" ref="AO125" si="70">ROUND((Z125-L125)/L125*100,2)</f>
-        <v>9.32</v>
-      </c>
-      <c r="AP125">
-        <f t="shared" ref="AP125" si="71">ROUND((AA125-M125)/M125*100,2)</f>
-        <v>0.9</v>
-      </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -17828,8 +17828,98 @@
       <c r="M126">
         <v>219</v>
       </c>
+      <c r="P126">
+        <v>100</v>
+      </c>
+      <c r="Q126">
+        <v>152</v>
+      </c>
+      <c r="R126">
+        <v>115</v>
+      </c>
+      <c r="S126">
+        <v>224</v>
+      </c>
+      <c r="T126">
+        <v>53</v>
+      </c>
+      <c r="U126">
+        <v>397</v>
+      </c>
+      <c r="V126">
+        <v>196</v>
+      </c>
+      <c r="W126">
+        <v>454</v>
+      </c>
+      <c r="X126">
+        <v>570</v>
+      </c>
+      <c r="Y126">
+        <v>65</v>
+      </c>
+      <c r="Z126">
+        <v>494</v>
+      </c>
+      <c r="AA126">
+        <v>227</v>
+      </c>
+      <c r="AC126">
+        <v>2022</v>
+      </c>
+      <c r="AD126">
+        <v>20</v>
+      </c>
+      <c r="AE126">
+        <f t="shared" si="60"/>
+        <v>-4.76</v>
+      </c>
+      <c r="AF126">
+        <f t="shared" si="61"/>
+        <v>27.73</v>
+      </c>
+      <c r="AG126">
+        <f t="shared" si="62"/>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="AH126">
+        <f t="shared" si="63"/>
+        <v>14.87</v>
+      </c>
+      <c r="AI126">
+        <f t="shared" si="64"/>
+        <v>26.19</v>
+      </c>
+      <c r="AJ126">
+        <f t="shared" si="65"/>
+        <v>12.78</v>
+      </c>
+      <c r="AK126">
+        <f t="shared" si="66"/>
+        <v>3.16</v>
+      </c>
+      <c r="AL126">
+        <f t="shared" si="67"/>
+        <v>2.95</v>
+      </c>
+      <c r="AM126">
+        <f t="shared" si="68"/>
+        <v>-0.18</v>
+      </c>
+      <c r="AN126">
+        <f t="shared" si="69"/>
+        <v>-12.16</v>
+      </c>
+      <c r="AO126">
+        <f t="shared" si="70"/>
+        <v>15.69</v>
+      </c>
+      <c r="AP126">
+        <f t="shared" si="71"/>
+        <v>3.65</v>
+      </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>139</v>
       </c>
@@ -17869,8 +17959,98 @@
       <c r="M127">
         <v>217</v>
       </c>
+      <c r="P127">
+        <v>108</v>
+      </c>
+      <c r="Q127">
+        <v>120</v>
+      </c>
+      <c r="R127">
+        <v>114</v>
+      </c>
+      <c r="S127">
+        <v>204</v>
+      </c>
+      <c r="T127">
+        <v>60</v>
+      </c>
+      <c r="U127">
+        <v>366</v>
+      </c>
+      <c r="V127">
+        <v>171</v>
+      </c>
+      <c r="W127">
+        <v>430</v>
+      </c>
+      <c r="X127">
+        <v>588</v>
+      </c>
+      <c r="Y127">
+        <v>80</v>
+      </c>
+      <c r="Z127">
+        <v>446</v>
+      </c>
+      <c r="AA127">
+        <v>227</v>
+      </c>
+      <c r="AC127">
+        <v>2022</v>
+      </c>
+      <c r="AD127">
+        <v>21</v>
+      </c>
+      <c r="AE127">
+        <f t="shared" ref="AE127:AE132" si="72">ROUND((P127-B127)/B127*100,2)</f>
+        <v>3.85</v>
+      </c>
+      <c r="AF127">
+        <f t="shared" ref="AF127:AF132" si="73">ROUND((Q127-C127)/C127*100,2)</f>
+        <v>3.45</v>
+      </c>
+      <c r="AG127">
+        <f t="shared" ref="AG127:AG132" si="74">ROUND((R127-D127)/D127*100,2)</f>
+        <v>16.329999999999998</v>
+      </c>
+      <c r="AH127">
+        <f t="shared" ref="AH127:AH132" si="75">ROUND((S127-E127)/E127*100,2)</f>
+        <v>5.7</v>
+      </c>
+      <c r="AI127">
+        <f t="shared" ref="AI127:AI132" si="76">ROUND((T127-F127)/F127*100,2)</f>
+        <v>39.53</v>
+      </c>
+      <c r="AJ127">
+        <f t="shared" ref="AJ127:AJ132" si="77">ROUND((U127-G127)/G127*100,2)</f>
+        <v>4.57</v>
+      </c>
+      <c r="AK127">
+        <f t="shared" ref="AK127:AK132" si="78">ROUND((V127-H127)/H127*100,2)</f>
+        <v>-8.56</v>
+      </c>
+      <c r="AL127">
+        <f t="shared" ref="AL127:AL132" si="79">ROUND((W127-I127)/I127*100,2)</f>
+        <v>-1.6</v>
+      </c>
+      <c r="AM127">
+        <f t="shared" ref="AM127:AM132" si="80">ROUND((X127-J127)/J127*100,2)</f>
+        <v>3.34</v>
+      </c>
+      <c r="AN127">
+        <f t="shared" ref="AN127:AN132" si="81">ROUND((Y127-K127)/K127*100,2)</f>
+        <v>6.67</v>
+      </c>
+      <c r="AO127">
+        <f t="shared" ref="AO127:AO132" si="82">ROUND((Z127-L127)/L127*100,2)</f>
+        <v>5.69</v>
+      </c>
+      <c r="AP127">
+        <f t="shared" ref="AP127:AP132" si="83">ROUND((AA127-M127)/M127*100,2)</f>
+        <v>4.6100000000000003</v>
+      </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>140</v>
       </c>
@@ -17910,8 +18090,98 @@
       <c r="M128">
         <v>215</v>
       </c>
+      <c r="P128">
+        <v>106</v>
+      </c>
+      <c r="Q128">
+        <v>112</v>
+      </c>
+      <c r="R128">
+        <v>109</v>
+      </c>
+      <c r="S128">
+        <v>210</v>
+      </c>
+      <c r="T128">
+        <v>52</v>
+      </c>
+      <c r="U128">
+        <v>352</v>
+      </c>
+      <c r="V128">
+        <v>194</v>
+      </c>
+      <c r="W128">
+        <v>454</v>
+      </c>
+      <c r="X128">
+        <v>623</v>
+      </c>
+      <c r="Y128">
+        <v>88</v>
+      </c>
+      <c r="Z128">
+        <v>446</v>
+      </c>
+      <c r="AA128">
+        <v>205</v>
+      </c>
+      <c r="AC128">
+        <v>2022</v>
+      </c>
+      <c r="AD128">
+        <v>22</v>
+      </c>
+      <c r="AE128">
+        <f t="shared" si="72"/>
+        <v>2.91</v>
+      </c>
+      <c r="AF128">
+        <f t="shared" si="73"/>
+        <v>-3.45</v>
+      </c>
+      <c r="AG128">
+        <f t="shared" si="74"/>
+        <v>13.54</v>
+      </c>
+      <c r="AH128">
+        <f t="shared" si="75"/>
+        <v>8.81</v>
+      </c>
+      <c r="AI128">
+        <f t="shared" si="76"/>
+        <v>23.81</v>
+      </c>
+      <c r="AJ128">
+        <f t="shared" si="77"/>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="AK128">
+        <f t="shared" si="78"/>
+        <v>3.74</v>
+      </c>
+      <c r="AL128">
+        <f t="shared" si="79"/>
+        <v>4.13</v>
+      </c>
+      <c r="AM128">
+        <f t="shared" si="80"/>
+        <v>10.85</v>
+      </c>
+      <c r="AN128">
+        <f t="shared" si="81"/>
+        <v>17.329999999999998</v>
+      </c>
+      <c r="AO128">
+        <f t="shared" si="82"/>
+        <v>6.19</v>
+      </c>
+      <c r="AP128">
+        <f t="shared" si="83"/>
+        <v>-4.6500000000000004</v>
+      </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -17951,8 +18221,98 @@
       <c r="M129">
         <v>215</v>
       </c>
+      <c r="P129">
+        <v>109</v>
+      </c>
+      <c r="Q129">
+        <v>113</v>
+      </c>
+      <c r="R129">
+        <v>90</v>
+      </c>
+      <c r="S129">
+        <v>196</v>
+      </c>
+      <c r="T129">
+        <v>59</v>
+      </c>
+      <c r="U129">
+        <v>394</v>
+      </c>
+      <c r="V129">
+        <v>213</v>
+      </c>
+      <c r="W129">
+        <v>436</v>
+      </c>
+      <c r="X129">
+        <v>588</v>
+      </c>
+      <c r="Y129">
+        <v>73</v>
+      </c>
+      <c r="Z129">
+        <v>454</v>
+      </c>
+      <c r="AA129">
+        <v>206</v>
+      </c>
+      <c r="AC129">
+        <v>2022</v>
+      </c>
+      <c r="AD129">
+        <v>23</v>
+      </c>
+      <c r="AE129">
+        <f t="shared" si="72"/>
+        <v>5.83</v>
+      </c>
+      <c r="AF129">
+        <f t="shared" si="73"/>
+        <v>-1.74</v>
+      </c>
+      <c r="AG129">
+        <f t="shared" si="74"/>
+        <v>-6.25</v>
+      </c>
+      <c r="AH129">
+        <f t="shared" si="75"/>
+        <v>2.62</v>
+      </c>
+      <c r="AI129">
+        <f t="shared" si="76"/>
+        <v>40.479999999999997</v>
+      </c>
+      <c r="AJ129">
+        <f t="shared" si="77"/>
+        <v>14.53</v>
+      </c>
+      <c r="AK129">
+        <f t="shared" si="78"/>
+        <v>15.14</v>
+      </c>
+      <c r="AL129">
+        <f t="shared" si="79"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AM129">
+        <f t="shared" si="80"/>
+        <v>5.19</v>
+      </c>
+      <c r="AN129">
+        <f t="shared" si="81"/>
+        <v>-2.67</v>
+      </c>
+      <c r="AO129">
+        <f t="shared" si="82"/>
+        <v>8.8699999999999992</v>
+      </c>
+      <c r="AP129">
+        <f t="shared" si="83"/>
+        <v>-4.1900000000000004</v>
+      </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>142</v>
       </c>
@@ -17992,8 +18352,98 @@
       <c r="M130">
         <v>215</v>
       </c>
+      <c r="P130">
+        <v>114</v>
+      </c>
+      <c r="Q130">
+        <v>120</v>
+      </c>
+      <c r="R130">
+        <v>118</v>
+      </c>
+      <c r="S130">
+        <v>202</v>
+      </c>
+      <c r="T130">
+        <v>43</v>
+      </c>
+      <c r="U130">
+        <v>367</v>
+      </c>
+      <c r="V130">
+        <v>220</v>
+      </c>
+      <c r="W130">
+        <v>444</v>
+      </c>
+      <c r="X130">
+        <v>602</v>
+      </c>
+      <c r="Y130">
+        <v>65</v>
+      </c>
+      <c r="Z130">
+        <v>465</v>
+      </c>
+      <c r="AA130">
+        <v>225</v>
+      </c>
+      <c r="AC130">
+        <v>2022</v>
+      </c>
+      <c r="AD130">
+        <v>24</v>
+      </c>
+      <c r="AE130">
+        <f t="shared" si="72"/>
+        <v>10.68</v>
+      </c>
+      <c r="AF130">
+        <f t="shared" si="73"/>
+        <v>2.56</v>
+      </c>
+      <c r="AG130">
+        <f t="shared" si="74"/>
+        <v>21.65</v>
+      </c>
+      <c r="AH130">
+        <f t="shared" si="75"/>
+        <v>5.76</v>
+      </c>
+      <c r="AI130">
+        <f t="shared" si="76"/>
+        <v>0</v>
+      </c>
+      <c r="AJ130">
+        <f t="shared" si="77"/>
+        <v>5.76</v>
+      </c>
+      <c r="AK130">
+        <f t="shared" si="78"/>
+        <v>19.57</v>
+      </c>
+      <c r="AL130">
+        <f t="shared" si="79"/>
+        <v>3.26</v>
+      </c>
+      <c r="AM130">
+        <f t="shared" si="80"/>
+        <v>7.5</v>
+      </c>
+      <c r="AN130">
+        <f t="shared" si="81"/>
+        <v>-13.33</v>
+      </c>
+      <c r="AO130">
+        <f t="shared" si="82"/>
+        <v>12.05</v>
+      </c>
+      <c r="AP130">
+        <f t="shared" si="83"/>
+        <v>4.6500000000000004</v>
+      </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -18033,8 +18483,98 @@
       <c r="M131">
         <v>216</v>
       </c>
+      <c r="P131">
+        <v>115</v>
+      </c>
+      <c r="Q131">
+        <v>134</v>
+      </c>
+      <c r="R131">
+        <v>104</v>
+      </c>
+      <c r="S131">
+        <v>220</v>
+      </c>
+      <c r="T131">
+        <v>54</v>
+      </c>
+      <c r="U131">
+        <v>380</v>
+      </c>
+      <c r="V131">
+        <v>208</v>
+      </c>
+      <c r="W131">
+        <v>434</v>
+      </c>
+      <c r="X131">
+        <v>691</v>
+      </c>
+      <c r="Y131">
+        <v>92</v>
+      </c>
+      <c r="Z131">
+        <v>448</v>
+      </c>
+      <c r="AA131">
+        <v>210</v>
+      </c>
+      <c r="AC131">
+        <v>2022</v>
+      </c>
+      <c r="AD131">
+        <v>25</v>
+      </c>
+      <c r="AE131">
+        <f t="shared" si="72"/>
+        <v>9.52</v>
+      </c>
+      <c r="AF131">
+        <f t="shared" si="73"/>
+        <v>15.52</v>
+      </c>
+      <c r="AG131">
+        <f t="shared" si="74"/>
+        <v>7.22</v>
+      </c>
+      <c r="AH131">
+        <f t="shared" si="75"/>
+        <v>15.79</v>
+      </c>
+      <c r="AI131">
+        <f t="shared" si="76"/>
+        <v>25.58</v>
+      </c>
+      <c r="AJ131">
+        <f t="shared" si="77"/>
+        <v>11.76</v>
+      </c>
+      <c r="AK131">
+        <f t="shared" si="78"/>
+        <v>13.66</v>
+      </c>
+      <c r="AL131">
+        <f t="shared" si="79"/>
+        <v>1.4</v>
+      </c>
+      <c r="AM131">
+        <f t="shared" si="80"/>
+        <v>24.06</v>
+      </c>
+      <c r="AN131">
+        <f t="shared" si="81"/>
+        <v>24.32</v>
+      </c>
+      <c r="AO131">
+        <f t="shared" si="82"/>
+        <v>8.2100000000000009</v>
+      </c>
+      <c r="AP131">
+        <f t="shared" si="83"/>
+        <v>-2.78</v>
+      </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>144</v>
       </c>
@@ -18074,8 +18614,98 @@
       <c r="M132">
         <v>216</v>
       </c>
+      <c r="P132">
+        <v>109</v>
+      </c>
+      <c r="Q132">
+        <v>137</v>
+      </c>
+      <c r="R132">
+        <v>123</v>
+      </c>
+      <c r="S132">
+        <v>216</v>
+      </c>
+      <c r="T132">
+        <v>46</v>
+      </c>
+      <c r="U132">
+        <v>368</v>
+      </c>
+      <c r="V132">
+        <v>183</v>
+      </c>
+      <c r="W132">
+        <v>477</v>
+      </c>
+      <c r="X132">
+        <v>582</v>
+      </c>
+      <c r="Y132">
+        <v>72</v>
+      </c>
+      <c r="Z132">
+        <v>472</v>
+      </c>
+      <c r="AA132">
+        <v>261</v>
+      </c>
+      <c r="AC132">
+        <v>2022</v>
+      </c>
+      <c r="AD132">
+        <v>26</v>
+      </c>
+      <c r="AE132">
+        <f t="shared" si="72"/>
+        <v>3.81</v>
+      </c>
+      <c r="AF132">
+        <f t="shared" si="73"/>
+        <v>17.09</v>
+      </c>
+      <c r="AG132">
+        <f t="shared" si="74"/>
+        <v>28.13</v>
+      </c>
+      <c r="AH132">
+        <f t="shared" si="75"/>
+        <v>13.68</v>
+      </c>
+      <c r="AI132">
+        <f t="shared" si="76"/>
+        <v>4.55</v>
+      </c>
+      <c r="AJ132">
+        <f t="shared" si="77"/>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="AK132">
+        <f t="shared" si="78"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AL132">
+        <f t="shared" si="79"/>
+        <v>11.71</v>
+      </c>
+      <c r="AM132">
+        <f t="shared" si="80"/>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="AN132">
+        <f t="shared" si="81"/>
+        <v>-1.37</v>
+      </c>
+      <c r="AO132">
+        <f t="shared" si="82"/>
+        <v>15.12</v>
+      </c>
+      <c r="AP132">
+        <f t="shared" si="83"/>
+        <v>20.83</v>
+      </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>145</v>
       </c>
@@ -18116,7 +18746,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>146</v>
       </c>
@@ -18157,7 +18787,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>147</v>
       </c>
@@ -18198,7 +18828,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -18239,7 +18869,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -18280,7 +18910,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -18321,7 +18951,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -18362,7 +18992,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -18403,7 +19033,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -18444,7 +19074,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -18485,7 +19115,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -18526,7 +19156,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:42" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>156</v>
       </c>
@@ -18567,7 +19197,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>157</v>
       </c>
@@ -18608,7 +19238,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>158</v>
       </c>
@@ -18649,7 +19279,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>159</v>
       </c>
@@ -18690,7 +19320,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>160</v>
       </c>
@@ -18731,7 +19361,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -18772,7 +19402,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>162</v>
       </c>
@@ -18813,7 +19443,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>163</v>
       </c>
@@ -18854,7 +19484,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>164</v>
       </c>
@@ -18895,7 +19525,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>165</v>
       </c>
@@ -18936,7 +19566,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>166</v>
       </c>
@@ -18977,7 +19607,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>167</v>
       </c>
@@ -19018,7 +19648,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>168</v>
       </c>
@@ -19059,7 +19689,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>169</v>
       </c>
@@ -19100,7 +19730,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
[2022-07-26] - Monkeypox update
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZELST007\Desktop\covid-19\data-misc\excess_mortality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C026C5-E721-46D3-A5C3-76979BE71B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5A7C59-DE59-4C3D-8693-319D26519E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="795" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,16 +1419,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG128" sqref="AG128"/>
+    <sheetView tabSelected="1" topLeftCell="H109" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI133" sqref="AI133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>10.76</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>-16.670000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>-4.58</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>-3.35</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>-8.4600000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>-12.77</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>-9.7799999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>-12.09</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>-2.96</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2985,7 +2985,7 @@
         <v>5.66</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>29.57</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>96.39</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>136.1</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>108.97</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -3640,7 +3640,7 @@
         <v>82.17</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>60.18</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -3902,7 +3902,7 @@
         <v>27.03</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>13.24</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>18.059999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>3.74</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>12.74</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>-8.02</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -4688,7 +4688,7 @@
         <v>4.2300000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>-6.57</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -4950,7 +4950,7 @@
         <v>2.82</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>-3.26</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>-12.96</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>0.94</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>-14.15</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>-0.96</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -5998,7 +5998,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -6129,7 +6129,7 @@
         <v>4.8099999999999996</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>-3.81</v>
       </c>
     </row>
-    <row r="38" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>-13.62</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -6522,7 +6522,7 @@
         <v>-10.7</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>-2.34</v>
       </c>
     </row>
-    <row r="41" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>9.1300000000000008</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>2.71</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -7046,7 +7046,7 @@
         <v>13.39</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -7177,7 +7177,7 @@
         <v>-3.13</v>
       </c>
     </row>
-    <row r="45" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -7308,7 +7308,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>58</v>
       </c>
@@ -7439,7 +7439,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>59</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>7.73</v>
       </c>
     </row>
-    <row r="48" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -7832,7 +7832,7 @@
         <v>22.03</v>
       </c>
     </row>
-    <row r="50" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>62</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>17.649999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>4.5599999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>22.45</v>
       </c>
     </row>
-    <row r="53" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>21.69</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>27.09</v>
       </c>
     </row>
-    <row r="55" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -8618,7 +8618,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="56" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -8749,7 +8749,7 @@
         <v>33.46</v>
       </c>
     </row>
-    <row r="57" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>16.920000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>24.62</v>
       </c>
     </row>
-    <row r="59" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="60" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>-2.19</v>
       </c>
     </row>
-    <row r="61" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -9404,7 +9404,7 @@
         <v>6.86</v>
       </c>
     </row>
-    <row r="62" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>-8.99</v>
       </c>
     </row>
-    <row r="63" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -9666,7 +9666,7 @@
         <v>-18.84</v>
       </c>
     </row>
-    <row r="64" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>-13.19</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -9928,7 +9928,7 @@
         <v>-10.11</v>
       </c>
     </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>78</v>
       </c>
@@ -10059,7 +10059,7 @@
         <v>-17.760000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -10190,7 +10190,7 @@
         <v>-1.99</v>
       </c>
     </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>80</v>
       </c>
@@ -10321,7 +10321,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -10452,7 +10452,7 @@
         <v>4.66</v>
       </c>
     </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>82</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>14.66</v>
       </c>
     </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>83</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>84</v>
       </c>
@@ -10845,7 +10845,7 @@
         <v>8.44</v>
       </c>
     </row>
-    <row r="73" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>85</v>
       </c>
@@ -10976,7 +10976,7 @@
         <v>16.29</v>
       </c>
     </row>
-    <row r="74" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>86</v>
       </c>
@@ -11107,7 +11107,7 @@
         <v>17.89</v>
       </c>
     </row>
-    <row r="75" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>87</v>
       </c>
@@ -11238,7 +11238,7 @@
         <v>-3.24</v>
       </c>
     </row>
-    <row r="76" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>88</v>
       </c>
@@ -11369,7 +11369,7 @@
         <v>10.28</v>
       </c>
     </row>
-    <row r="77" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>89</v>
       </c>
@@ -11500,7 +11500,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="78" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -11631,7 +11631,7 @@
         <v>6.05</v>
       </c>
     </row>
-    <row r="79" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>91</v>
       </c>
@@ -11762,7 +11762,7 @@
         <v>-11.16</v>
       </c>
     </row>
-    <row r="80" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>92</v>
       </c>
@@ -11893,7 +11893,7 @@
         <v>4.63</v>
       </c>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>93</v>
       </c>
@@ -12024,7 +12024,7 @@
         <v>4.17</v>
       </c>
     </row>
-    <row r="82" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>94</v>
       </c>
@@ -12155,7 +12155,7 @@
         <v>16.59</v>
       </c>
     </row>
-    <row r="83" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>95</v>
       </c>
@@ -12286,7 +12286,7 @@
         <v>-0.46</v>
       </c>
     </row>
-    <row r="84" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>96</v>
       </c>
@@ -12417,7 +12417,7 @@
         <v>13.49</v>
       </c>
     </row>
-    <row r="85" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>97</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>9.39</v>
       </c>
     </row>
-    <row r="86" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>98</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>-0.93</v>
       </c>
     </row>
-    <row r="87" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>99</v>
       </c>
@@ -12810,7 +12810,7 @@
         <v>17.54</v>
       </c>
     </row>
-    <row r="88" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>100</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="89" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>101</v>
       </c>
@@ -13072,7 +13072,7 @@
         <v>-8.57</v>
       </c>
     </row>
-    <row r="90" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>102</v>
       </c>
@@ -13203,7 +13203,7 @@
         <v>2.83</v>
       </c>
     </row>
-    <row r="91" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>103</v>
       </c>
@@ -13334,7 +13334,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="92" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -13465,7 +13465,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="93" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>105</v>
       </c>
@@ -13596,7 +13596,7 @@
         <v>10.65</v>
       </c>
     </row>
-    <row r="94" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -13727,7 +13727,7 @@
         <v>8.14</v>
       </c>
     </row>
-    <row r="95" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -13858,7 +13858,7 @@
         <v>6.73</v>
       </c>
     </row>
-    <row r="96" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -13989,7 +13989,7 @@
         <v>26.99</v>
       </c>
     </row>
-    <row r="97" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>109</v>
       </c>
@@ -14120,7 +14120,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="98" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>110</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>32.46</v>
       </c>
     </row>
-    <row r="99" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>111</v>
       </c>
@@ -14382,7 +14382,7 @@
         <v>47.83</v>
       </c>
     </row>
-    <row r="100" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>112</v>
       </c>
@@ -14513,7 +14513,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="101" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>113</v>
       </c>
@@ -14644,7 +14644,7 @@
         <v>75.849999999999994</v>
       </c>
     </row>
-    <row r="102" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>114</v>
       </c>
@@ -14775,7 +14775,7 @@
         <v>69.33</v>
       </c>
     </row>
-    <row r="103" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>115</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="104" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>116</v>
       </c>
@@ -15037,7 +15037,7 @@
         <v>45.68</v>
       </c>
     </row>
-    <row r="105" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>117</v>
       </c>
@@ -15168,7 +15168,7 @@
         <v>27.53</v>
       </c>
     </row>
-    <row r="106" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>118</v>
       </c>
@@ -15299,7 +15299,7 @@
         <v>16.73</v>
       </c>
     </row>
-    <row r="107" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>119</v>
       </c>
@@ -15430,7 +15430,7 @@
         <v>9.4499999999999993</v>
       </c>
     </row>
-    <row r="108" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>120</v>
       </c>
@@ -15561,7 +15561,7 @@
         <v>-10.85</v>
       </c>
     </row>
-    <row r="109" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -15692,7 +15692,7 @@
         <v>-9.58</v>
       </c>
     </row>
-    <row r="110" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>122</v>
       </c>
@@ -15823,7 +15823,7 @@
         <v>-4.8899999999999997</v>
       </c>
     </row>
-    <row r="111" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -15891,7 +15891,7 @@
         <v>667</v>
       </c>
       <c r="Y111">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z111">
         <v>512</v>
@@ -15943,7 +15943,7 @@
       </c>
       <c r="AN111">
         <f t="shared" si="33"/>
-        <v>-15.05</v>
+        <v>-13.98</v>
       </c>
       <c r="AO111">
         <f t="shared" si="34"/>
@@ -15954,7 +15954,7 @@
         <v>-12.82</v>
       </c>
     </row>
-    <row r="112" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>124</v>
       </c>
@@ -16028,7 +16028,7 @@
         <v>473</v>
       </c>
       <c r="AA112">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AC112">
         <v>2022</v>
@@ -16082,10 +16082,10 @@
       </c>
       <c r="AP112">
         <f t="shared" si="35"/>
-        <v>-12.73</v>
+        <v>-12.36</v>
       </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>125</v>
       </c>
@@ -16150,7 +16150,7 @@
         <v>515</v>
       </c>
       <c r="X113">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="Y113">
         <v>103</v>
@@ -16201,7 +16201,7 @@
       </c>
       <c r="AM113">
         <f t="shared" si="32"/>
-        <v>-1.01</v>
+        <v>-0.86</v>
       </c>
       <c r="AN113">
         <f t="shared" si="33"/>
@@ -16216,7 +16216,7 @@
         <v>-7.19</v>
       </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -16347,7 +16347,7 @@
         <v>-5.71</v>
       </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>127</v>
       </c>
@@ -16409,10 +16409,10 @@
         <v>208</v>
       </c>
       <c r="W115">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="X115">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="Y115">
         <v>95</v>
@@ -16459,11 +16459,11 @@
       </c>
       <c r="AL115">
         <f t="shared" si="31"/>
-        <v>-2.73</v>
+        <v>-2.5299999999999998</v>
       </c>
       <c r="AM115">
         <f t="shared" si="32"/>
-        <v>-8.39</v>
+        <v>-8.25</v>
       </c>
       <c r="AN115">
         <f t="shared" si="33"/>
@@ -16478,7 +16478,7 @@
         <v>-6.86</v>
       </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>128</v>
       </c>
@@ -16543,7 +16543,7 @@
         <v>524</v>
       </c>
       <c r="X116">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="Y116">
         <v>84</v>
@@ -16594,7 +16594,7 @@
       </c>
       <c r="AM116">
         <f t="shared" si="32"/>
-        <v>0.3</v>
+        <v>0.44</v>
       </c>
       <c r="AN116">
         <f t="shared" si="33"/>
@@ -16609,7 +16609,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>129</v>
       </c>
@@ -16671,7 +16671,7 @@
         <v>236</v>
       </c>
       <c r="W117">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="X117">
         <v>673</v>
@@ -16721,7 +16721,7 @@
       </c>
       <c r="AL117">
         <f t="shared" si="31"/>
-        <v>4.04</v>
+        <v>4.24</v>
       </c>
       <c r="AM117">
         <f t="shared" si="32"/>
@@ -16740,7 +16740,7 @@
         <v>10.45</v>
       </c>
     </row>
-    <row r="118" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>130</v>
       </c>
@@ -16802,7 +16802,7 @@
         <v>246</v>
       </c>
       <c r="W118">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="X118">
         <v>722</v>
@@ -16852,7 +16852,7 @@
       </c>
       <c r="AL118">
         <f t="shared" si="31"/>
-        <v>9.52</v>
+        <v>9.73</v>
       </c>
       <c r="AM118">
         <f t="shared" si="32"/>
@@ -16871,7 +16871,7 @@
         <v>22.31</v>
       </c>
     </row>
-    <row r="119" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>131</v>
       </c>
@@ -17002,7 +17002,7 @@
         <v>-0.79</v>
       </c>
     </row>
-    <row r="120" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>132</v>
       </c>
@@ -17064,10 +17064,10 @@
         <v>239</v>
       </c>
       <c r="W120">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="X120">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="Y120">
         <v>97</v>
@@ -17114,11 +17114,11 @@
       </c>
       <c r="AL120">
         <f t="shared" si="31"/>
-        <v>17.75</v>
+        <v>17.97</v>
       </c>
       <c r="AM120">
         <f t="shared" si="32"/>
-        <v>18.510000000000002</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="AN120">
         <f t="shared" si="33"/>
@@ -17133,7 +17133,7 @@
         <v>11.48</v>
       </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>133</v>
       </c>
@@ -17192,10 +17192,10 @@
         <v>448</v>
       </c>
       <c r="V121">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="W121">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="X121">
         <v>657</v>
@@ -17204,10 +17204,10 @@
         <v>108</v>
       </c>
       <c r="Z121">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AA121">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AC121">
         <v>2022</v>
@@ -17241,11 +17241,11 @@
       </c>
       <c r="AK121">
         <f t="shared" si="30"/>
-        <v>17.5</v>
+        <v>18</v>
       </c>
       <c r="AL121">
         <f t="shared" si="31"/>
-        <v>22.96</v>
+        <v>23.18</v>
       </c>
       <c r="AM121">
         <f t="shared" si="32"/>
@@ -17257,14 +17257,14 @@
       </c>
       <c r="AO121">
         <f t="shared" si="34"/>
-        <v>10.09</v>
+        <v>10.31</v>
       </c>
       <c r="AP121">
         <f t="shared" si="35"/>
-        <v>27.85</v>
+        <v>28.27</v>
       </c>
     </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>134</v>
       </c>
@@ -17395,7 +17395,7 @@
         <v>15.02</v>
       </c>
     </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>135</v>
       </c>
@@ -17526,7 +17526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>136</v>
       </c>
@@ -17591,7 +17591,7 @@
         <v>484</v>
       </c>
       <c r="X124">
-        <v>635</v>
+        <v>637</v>
       </c>
       <c r="Y124">
         <v>69</v>
@@ -17642,7 +17642,7 @@
       </c>
       <c r="AM124">
         <f t="shared" si="56"/>
-        <v>9.11</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="AN124">
         <f t="shared" si="57"/>
@@ -17657,7 +17657,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>137</v>
       </c>
@@ -17716,10 +17716,10 @@
         <v>414</v>
       </c>
       <c r="V125">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="W125">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="X125">
         <v>584</v>
@@ -17731,7 +17731,7 @@
         <v>461</v>
       </c>
       <c r="AA125">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AC125">
         <v>2022</v>
@@ -17765,11 +17765,11 @@
       </c>
       <c r="AK125">
         <f t="shared" ref="AK125:AK126" si="66">ROUND((V125-H125)/H125*100,2)</f>
-        <v>7.81</v>
+        <v>8.33</v>
       </c>
       <c r="AL125">
         <f t="shared" ref="AL125:AL126" si="67">ROUND((W125-I125)/I125*100,2)</f>
-        <v>15.8</v>
+        <v>16.03</v>
       </c>
       <c r="AM125">
         <f t="shared" ref="AM125:AM126" si="68">ROUND((X125-J125)/J125*100,2)</f>
@@ -17785,10 +17785,10 @@
       </c>
       <c r="AP125">
         <f t="shared" ref="AP125:AP126" si="71">ROUND((AA125-M125)/M125*100,2)</f>
-        <v>2.25</v>
+        <v>2.7</v>
       </c>
     </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>138</v>
       </c>
@@ -17853,7 +17853,7 @@
         <v>454</v>
       </c>
       <c r="X126">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="Y126">
         <v>65</v>
@@ -17904,7 +17904,7 @@
       </c>
       <c r="AM126">
         <f t="shared" si="68"/>
-        <v>-0.18</v>
+        <v>0</v>
       </c>
       <c r="AN126">
         <f t="shared" si="69"/>
@@ -17919,7 +17919,7 @@
         <v>3.65</v>
       </c>
     </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>139</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>430</v>
       </c>
       <c r="X127">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="Y127">
         <v>80</v>
@@ -18035,7 +18035,7 @@
       </c>
       <c r="AM127">
         <f t="shared" ref="AM127:AM132" si="80">ROUND((X127-J127)/J127*100,2)</f>
-        <v>3.34</v>
+        <v>3.51</v>
       </c>
       <c r="AN127">
         <f t="shared" ref="AN127:AN132" si="81">ROUND((Y127-K127)/K127*100,2)</f>
@@ -18050,7 +18050,7 @@
         <v>4.6100000000000003</v>
       </c>
     </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>140</v>
       </c>
@@ -18091,7 +18091,7 @@
         <v>215</v>
       </c>
       <c r="P128">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="Q128">
         <v>112</v>
@@ -18103,19 +18103,19 @@
         <v>210</v>
       </c>
       <c r="T128">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U128">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="V128">
         <v>194</v>
       </c>
       <c r="W128">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="X128">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="Y128">
         <v>88</v>
@@ -18134,7 +18134,7 @@
       </c>
       <c r="AE128">
         <f t="shared" si="72"/>
-        <v>2.91</v>
+        <v>3.88</v>
       </c>
       <c r="AF128">
         <f t="shared" si="73"/>
@@ -18150,11 +18150,11 @@
       </c>
       <c r="AI128">
         <f t="shared" si="76"/>
-        <v>23.81</v>
+        <v>26.19</v>
       </c>
       <c r="AJ128">
         <f t="shared" si="77"/>
-        <v>1.1499999999999999</v>
+        <v>1.44</v>
       </c>
       <c r="AK128">
         <f t="shared" si="78"/>
@@ -18162,11 +18162,11 @@
       </c>
       <c r="AL128">
         <f t="shared" si="79"/>
-        <v>4.13</v>
+        <v>4.3600000000000003</v>
       </c>
       <c r="AM128">
         <f t="shared" si="80"/>
-        <v>10.85</v>
+        <v>11.03</v>
       </c>
       <c r="AN128">
         <f t="shared" si="81"/>
@@ -18181,7 +18181,7 @@
         <v>-4.6500000000000004</v>
       </c>
     </row>
-    <row r="129" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>141</v>
       </c>
@@ -18237,16 +18237,16 @@
         <v>59</v>
       </c>
       <c r="U129">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="V129">
         <v>213</v>
       </c>
       <c r="W129">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="X129">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="Y129">
         <v>73</v>
@@ -18285,7 +18285,7 @@
       </c>
       <c r="AJ129">
         <f t="shared" si="77"/>
-        <v>14.53</v>
+        <v>14.83</v>
       </c>
       <c r="AK129">
         <f t="shared" si="78"/>
@@ -18293,11 +18293,11 @@
       </c>
       <c r="AL129">
         <f t="shared" si="79"/>
-        <v>1.1599999999999999</v>
+        <v>1.62</v>
       </c>
       <c r="AM129">
         <f t="shared" si="80"/>
-        <v>5.19</v>
+        <v>5.37</v>
       </c>
       <c r="AN129">
         <f t="shared" si="81"/>
@@ -18312,7 +18312,7 @@
         <v>-4.1900000000000004</v>
       </c>
     </row>
-    <row r="130" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>142</v>
       </c>
@@ -18353,7 +18353,7 @@
         <v>215</v>
       </c>
       <c r="P130">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="Q130">
         <v>120</v>
@@ -18365,28 +18365,28 @@
         <v>202</v>
       </c>
       <c r="T130">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="U130">
         <v>367</v>
       </c>
       <c r="V130">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="W130">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="X130">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="Y130">
         <v>65</v>
       </c>
       <c r="Z130">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AA130">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="AC130">
         <v>2022</v>
@@ -18396,7 +18396,7 @@
       </c>
       <c r="AE130">
         <f t="shared" si="72"/>
-        <v>10.68</v>
+        <v>11.65</v>
       </c>
       <c r="AF130">
         <f t="shared" si="73"/>
@@ -18412,7 +18412,7 @@
       </c>
       <c r="AI130">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>2.33</v>
       </c>
       <c r="AJ130">
         <f t="shared" si="77"/>
@@ -18420,15 +18420,15 @@
       </c>
       <c r="AK130">
         <f t="shared" si="78"/>
-        <v>19.57</v>
+        <v>20.11</v>
       </c>
       <c r="AL130">
         <f t="shared" si="79"/>
-        <v>3.26</v>
+        <v>3.72</v>
       </c>
       <c r="AM130">
         <f t="shared" si="80"/>
-        <v>7.5</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="AN130">
         <f t="shared" si="81"/>
@@ -18436,14 +18436,14 @@
       </c>
       <c r="AO130">
         <f t="shared" si="82"/>
-        <v>12.05</v>
+        <v>12.29</v>
       </c>
       <c r="AP130">
         <f t="shared" si="83"/>
-        <v>4.6500000000000004</v>
+        <v>5.58</v>
       </c>
     </row>
-    <row r="131" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>143</v>
       </c>
@@ -18484,7 +18484,7 @@
         <v>216</v>
       </c>
       <c r="P131">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q131">
         <v>134</v>
@@ -18499,25 +18499,25 @@
         <v>54</v>
       </c>
       <c r="U131">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="V131">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="W131">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="X131">
-        <v>691</v>
+        <v>697</v>
       </c>
       <c r="Y131">
         <v>92</v>
       </c>
       <c r="Z131">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="AA131">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="AC131">
         <v>2022</v>
@@ -18527,7 +18527,7 @@
       </c>
       <c r="AE131">
         <f t="shared" si="72"/>
-        <v>9.52</v>
+        <v>10.48</v>
       </c>
       <c r="AF131">
         <f t="shared" si="73"/>
@@ -18547,19 +18547,19 @@
       </c>
       <c r="AJ131">
         <f t="shared" si="77"/>
-        <v>11.76</v>
+        <v>12.65</v>
       </c>
       <c r="AK131">
         <f t="shared" si="78"/>
-        <v>13.66</v>
+        <v>14.75</v>
       </c>
       <c r="AL131">
         <f t="shared" si="79"/>
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>24.06</v>
+        <v>25.13</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
@@ -18567,14 +18567,14 @@
       </c>
       <c r="AO131">
         <f t="shared" si="82"/>
-        <v>8.2100000000000009</v>
+        <v>8.94</v>
       </c>
       <c r="AP131">
         <f t="shared" si="83"/>
-        <v>-2.78</v>
+        <v>-2.31</v>
       </c>
     </row>
-    <row r="132" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>144</v>
       </c>
@@ -18615,40 +18615,40 @@
         <v>216</v>
       </c>
       <c r="P132">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="Q132">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="R132">
         <v>123</v>
       </c>
       <c r="S132">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="T132">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="U132">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="V132">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="W132">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="X132">
-        <v>582</v>
+        <v>566</v>
       </c>
       <c r="Y132">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Z132">
-        <v>472</v>
+        <v>496</v>
       </c>
       <c r="AA132">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="AC132">
         <v>2022</v>
@@ -18658,11 +18658,11 @@
       </c>
       <c r="AE132">
         <f t="shared" si="72"/>
-        <v>3.81</v>
+        <v>10.48</v>
       </c>
       <c r="AF132">
         <f t="shared" si="73"/>
-        <v>17.09</v>
+        <v>27.35</v>
       </c>
       <c r="AG132">
         <f t="shared" si="74"/>
@@ -18670,42 +18670,42 @@
       </c>
       <c r="AH132">
         <f t="shared" si="75"/>
-        <v>13.68</v>
+        <v>8.42</v>
       </c>
       <c r="AI132">
         <f t="shared" si="76"/>
-        <v>4.55</v>
+        <v>15.91</v>
       </c>
       <c r="AJ132">
         <f t="shared" si="77"/>
-        <v>9.1999999999999993</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="AK132">
         <f t="shared" si="78"/>
-        <v>0.55000000000000004</v>
+        <v>6.04</v>
       </c>
       <c r="AL132">
         <f t="shared" si="79"/>
-        <v>11.71</v>
+        <v>11.48</v>
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
-        <v>4.1100000000000003</v>
+        <v>1.25</v>
       </c>
       <c r="AN132">
         <f t="shared" si="81"/>
-        <v>-1.37</v>
+        <v>-6.85</v>
       </c>
       <c r="AO132">
         <f t="shared" si="82"/>
-        <v>15.12</v>
+        <v>20.98</v>
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
-        <v>20.83</v>
+        <v>18.98</v>
       </c>
     </row>
-    <row r="133" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>145</v>
       </c>
@@ -18745,8 +18745,98 @@
       <c r="M133">
         <v>217</v>
       </c>
+      <c r="P133">
+        <v>95</v>
+      </c>
+      <c r="Q133">
+        <v>131</v>
+      </c>
+      <c r="R133">
+        <v>116</v>
+      </c>
+      <c r="S133">
+        <v>183</v>
+      </c>
+      <c r="T133">
+        <v>52</v>
+      </c>
+      <c r="U133">
+        <v>379</v>
+      </c>
+      <c r="V133">
+        <v>194</v>
+      </c>
+      <c r="W133">
+        <v>467</v>
+      </c>
+      <c r="X133">
+        <v>597</v>
+      </c>
+      <c r="Y133">
+        <v>77</v>
+      </c>
+      <c r="Z133">
+        <v>443</v>
+      </c>
+      <c r="AA133">
+        <v>205</v>
+      </c>
+      <c r="AC133">
+        <v>2022</v>
+      </c>
+      <c r="AD133">
+        <v>27</v>
+      </c>
+      <c r="AE133">
+        <f t="shared" ref="AE133:AE134" si="84">ROUND((P133-B133)/B133*100,2)</f>
+        <v>-9.52</v>
+      </c>
+      <c r="AF133">
+        <f t="shared" ref="AF133:AF134" si="85">ROUND((Q133-C133)/C133*100,2)</f>
+        <v>12.93</v>
+      </c>
+      <c r="AG133">
+        <f t="shared" ref="AG133:AG134" si="86">ROUND((R133-D133)/D133*100,2)</f>
+        <v>20.83</v>
+      </c>
+      <c r="AH133">
+        <f t="shared" ref="AH133:AH134" si="87">ROUND((S133-E133)/E133*100,2)</f>
+        <v>-3.17</v>
+      </c>
+      <c r="AI133">
+        <f t="shared" ref="AI133:AI134" si="88">ROUND((T133-F133)/F133*100,2)</f>
+        <v>15.56</v>
+      </c>
+      <c r="AJ133">
+        <f t="shared" ref="AJ133:AJ134" si="89">ROUND((U133-G133)/G133*100,2)</f>
+        <v>11.47</v>
+      </c>
+      <c r="AK133">
+        <f t="shared" ref="AK133:AK134" si="90">ROUND((V133-H133)/H133*100,2)</f>
+        <v>6.01</v>
+      </c>
+      <c r="AL133">
+        <f t="shared" ref="AL133:AL134" si="91">ROUND((W133-I133)/I133*100,2)</f>
+        <v>9.11</v>
+      </c>
+      <c r="AM133">
+        <f t="shared" ref="AM133:AM134" si="92">ROUND((X133-J133)/J133*100,2)</f>
+        <v>6.61</v>
+      </c>
+      <c r="AN133">
+        <f t="shared" ref="AN133:AN134" si="93">ROUND((Y133-K133)/K133*100,2)</f>
+        <v>5.48</v>
+      </c>
+      <c r="AO133">
+        <f t="shared" ref="AO133:AO134" si="94">ROUND((Z133-L133)/L133*100,2)</f>
+        <v>7.79</v>
+      </c>
+      <c r="AP133">
+        <f t="shared" ref="AP133:AP134" si="95">ROUND((AA133-M133)/M133*100,2)</f>
+        <v>-5.53</v>
+      </c>
     </row>
-    <row r="134" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>146</v>
       </c>
@@ -18786,8 +18876,98 @@
       <c r="M134">
         <v>217</v>
       </c>
+      <c r="P134">
+        <v>124</v>
+      </c>
+      <c r="Q134">
+        <v>118</v>
+      </c>
+      <c r="R134">
+        <v>111</v>
+      </c>
+      <c r="S134">
+        <v>196</v>
+      </c>
+      <c r="T134">
+        <v>58</v>
+      </c>
+      <c r="U134">
+        <v>349</v>
+      </c>
+      <c r="V134">
+        <v>219</v>
+      </c>
+      <c r="W134">
+        <v>529</v>
+      </c>
+      <c r="X134">
+        <v>650</v>
+      </c>
+      <c r="Y134">
+        <v>79</v>
+      </c>
+      <c r="Z134">
+        <v>440</v>
+      </c>
+      <c r="AA134">
+        <v>264</v>
+      </c>
+      <c r="AC134">
+        <v>2022</v>
+      </c>
+      <c r="AD134">
+        <v>28</v>
+      </c>
+      <c r="AE134">
+        <f t="shared" si="84"/>
+        <v>16.98</v>
+      </c>
+      <c r="AF134">
+        <f t="shared" si="85"/>
+        <v>1.72</v>
+      </c>
+      <c r="AG134">
+        <f t="shared" si="86"/>
+        <v>14.43</v>
+      </c>
+      <c r="AH134">
+        <f t="shared" si="87"/>
+        <v>3.7</v>
+      </c>
+      <c r="AI134">
+        <f t="shared" si="88"/>
+        <v>28.89</v>
+      </c>
+      <c r="AJ134">
+        <f t="shared" si="89"/>
+        <v>3.56</v>
+      </c>
+      <c r="AK134">
+        <f t="shared" si="90"/>
+        <v>19.02</v>
+      </c>
+      <c r="AL134">
+        <f t="shared" si="91"/>
+        <v>23.31</v>
+      </c>
+      <c r="AM134">
+        <f t="shared" si="92"/>
+        <v>16.489999999999998</v>
+      </c>
+      <c r="AN134">
+        <f t="shared" si="93"/>
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="AO134">
+        <f t="shared" si="94"/>
+        <v>7.58</v>
+      </c>
+      <c r="AP134">
+        <f t="shared" si="95"/>
+        <v>21.66</v>
+      </c>
     </row>
-    <row r="135" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>147</v>
       </c>
@@ -18828,7 +19008,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="136" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>148</v>
       </c>
@@ -18869,7 +19049,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="137" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>149</v>
       </c>
@@ -18910,7 +19090,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="138" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>150</v>
       </c>
@@ -18951,7 +19131,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="139" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -18992,7 +19172,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="140" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>152</v>
       </c>
@@ -19033,7 +19213,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="141" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>153</v>
       </c>
@@ -19074,7 +19254,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="142" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>154</v>
       </c>
@@ -19115,7 +19295,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="143" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>155</v>
       </c>
@@ -19156,7 +19336,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="144" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>156</v>
       </c>
@@ -19197,7 +19377,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>157</v>
       </c>
@@ -19238,7 +19418,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>158</v>
       </c>
@@ -19279,7 +19459,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>159</v>
       </c>
@@ -19320,7 +19500,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>160</v>
       </c>
@@ -19361,7 +19541,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>161</v>
       </c>
@@ -19402,7 +19582,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>162</v>
       </c>
@@ -19443,7 +19623,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>163</v>
       </c>
@@ -19484,7 +19664,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>164</v>
       </c>
@@ -19525,7 +19705,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>165</v>
       </c>
@@ -19566,7 +19746,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>166</v>
       </c>
@@ -19607,7 +19787,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>167</v>
       </c>
@@ -19648,7 +19828,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>168</v>
       </c>
@@ -19689,7 +19869,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>169</v>
       </c>
@@ -19730,7 +19910,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
[2022-07-29] Update death comparison tracker for Twitter thread (Friday update - part 2)
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5A7C59-DE59-4C3D-8693-319D26519E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556DADAF-391D-437B-A31E-D76877D3E532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3450" yWindow="795" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H109" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI133" sqref="AI133"/>
+    <sheetView tabSelected="1" topLeftCell="E100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AF135" sqref="AF135:AP135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15626,7 +15626,7 @@
         <v>514</v>
       </c>
       <c r="X109">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="Y109">
         <v>87</v>
@@ -15677,7 +15677,7 @@
       </c>
       <c r="AM109">
         <f t="shared" si="32"/>
-        <v>-2.86</v>
+        <v>-2.72</v>
       </c>
       <c r="AN109">
         <f t="shared" si="33"/>
@@ -15882,7 +15882,7 @@
         <v>399</v>
       </c>
       <c r="V111">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W111">
         <v>504</v>
@@ -15931,7 +15931,7 @@
       </c>
       <c r="AK111">
         <f t="shared" si="30"/>
-        <v>-14.41</v>
+        <v>-13.97</v>
       </c>
       <c r="AL111">
         <f t="shared" si="31"/>
@@ -16019,7 +16019,7 @@
         <v>530</v>
       </c>
       <c r="X112">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="Y112">
         <v>100</v>
@@ -16070,7 +16070,7 @@
       </c>
       <c r="AM112">
         <f t="shared" si="32"/>
-        <v>-3.58</v>
+        <v>-3.72</v>
       </c>
       <c r="AN112">
         <f t="shared" si="33"/>
@@ -16147,7 +16147,7 @@
         <v>213</v>
       </c>
       <c r="W113">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="X113">
         <v>689</v>
@@ -16197,7 +16197,7 @@
       </c>
       <c r="AL113">
         <f t="shared" si="31"/>
-        <v>-2.09</v>
+        <v>-1.9</v>
       </c>
       <c r="AM113">
         <f t="shared" si="32"/>
@@ -16287,7 +16287,7 @@
         <v>95</v>
       </c>
       <c r="Z114">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AA114">
         <v>264</v>
@@ -16340,7 +16340,7 @@
       </c>
       <c r="AO114">
         <f t="shared" si="34"/>
-        <v>1.89</v>
+        <v>2.08</v>
       </c>
       <c r="AP114">
         <f t="shared" si="35"/>
@@ -17439,7 +17439,7 @@
         <v>109</v>
       </c>
       <c r="Q123">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="R123">
         <v>115</v>
@@ -17483,7 +17483,7 @@
       </c>
       <c r="AF123">
         <f t="shared" ref="AF123:AF124" si="49">ROUND((Q123-C123)/C123*100,2)</f>
-        <v>19.670000000000002</v>
+        <v>20.49</v>
       </c>
       <c r="AG123">
         <f t="shared" ref="AG123:AG124" si="50">ROUND((R123-D123)/D123*100,2)</f>
@@ -18109,7 +18109,7 @@
         <v>353</v>
       </c>
       <c r="V128">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W128">
         <v>455</v>
@@ -18158,7 +18158,7 @@
       </c>
       <c r="AK128">
         <f t="shared" si="78"/>
-        <v>3.74</v>
+        <v>4.28</v>
       </c>
       <c r="AL128">
         <f t="shared" si="79"/>
@@ -18246,7 +18246,7 @@
         <v>438</v>
       </c>
       <c r="X129">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="Y129">
         <v>73</v>
@@ -18297,7 +18297,7 @@
       </c>
       <c r="AM129">
         <f t="shared" si="80"/>
-        <v>5.37</v>
+        <v>5.72</v>
       </c>
       <c r="AN129">
         <f t="shared" si="81"/>
@@ -18374,10 +18374,10 @@
         <v>221</v>
       </c>
       <c r="W130">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="X130">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="Y130">
         <v>65</v>
@@ -18386,7 +18386,7 @@
         <v>466</v>
       </c>
       <c r="AA130">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AC130">
         <v>2022</v>
@@ -18424,11 +18424,11 @@
       </c>
       <c r="AL130">
         <f t="shared" si="79"/>
-        <v>3.72</v>
+        <v>3.95</v>
       </c>
       <c r="AM130">
         <f t="shared" si="80"/>
-        <v>8.0399999999999991</v>
+        <v>8.39</v>
       </c>
       <c r="AN130">
         <f t="shared" si="81"/>
@@ -18440,7 +18440,7 @@
       </c>
       <c r="AP130">
         <f t="shared" si="83"/>
-        <v>5.58</v>
+        <v>6.05</v>
       </c>
     </row>
     <row r="131" spans="1:42" x14ac:dyDescent="0.25">
@@ -18490,10 +18490,10 @@
         <v>134</v>
       </c>
       <c r="R131">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S131">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="T131">
         <v>54</v>
@@ -18502,16 +18502,16 @@
         <v>383</v>
       </c>
       <c r="V131">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="W131">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="X131">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="Y131">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Z131">
         <v>451</v>
@@ -18535,11 +18535,11 @@
       </c>
       <c r="AG131">
         <f t="shared" si="74"/>
-        <v>7.22</v>
+        <v>8.25</v>
       </c>
       <c r="AH131">
         <f t="shared" si="75"/>
-        <v>15.79</v>
+        <v>16.32</v>
       </c>
       <c r="AI131">
         <f t="shared" si="76"/>
@@ -18551,19 +18551,19 @@
       </c>
       <c r="AK131">
         <f t="shared" si="78"/>
-        <v>14.75</v>
+        <v>15.85</v>
       </c>
       <c r="AL131">
         <f t="shared" si="79"/>
-        <v>2.8</v>
+        <v>3.5</v>
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>25.13</v>
+        <v>25.49</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
-        <v>24.32</v>
+        <v>25.68</v>
       </c>
       <c r="AO131">
         <f t="shared" si="82"/>
@@ -18630,7 +18630,7 @@
         <v>51</v>
       </c>
       <c r="U132">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="V132">
         <v>193</v>
@@ -18639,7 +18639,7 @@
         <v>476</v>
       </c>
       <c r="X132">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="Y132">
         <v>68</v>
@@ -18678,7 +18678,7 @@
       </c>
       <c r="AJ132">
         <f t="shared" si="77"/>
-        <v>9.7899999999999991</v>
+        <v>10.09</v>
       </c>
       <c r="AK132">
         <f t="shared" si="78"/>
@@ -18690,7 +18690,7 @@
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
-        <v>1.25</v>
+        <v>1.61</v>
       </c>
       <c r="AN132">
         <f t="shared" si="81"/>
@@ -18758,28 +18758,28 @@
         <v>183</v>
       </c>
       <c r="T133">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U133">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="V133">
         <v>194</v>
       </c>
       <c r="W133">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="X133">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="Y133">
         <v>77</v>
       </c>
       <c r="Z133">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AA133">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AC133">
         <v>2022</v>
@@ -18788,7 +18788,7 @@
         <v>27</v>
       </c>
       <c r="AE133">
-        <f t="shared" ref="AE133:AE134" si="84">ROUND((P133-B133)/B133*100,2)</f>
+        <f t="shared" ref="AE133:AF135" si="84">ROUND((P133-B133)/B133*100,2)</f>
         <v>-9.52</v>
       </c>
       <c r="AF133">
@@ -18796,44 +18796,44 @@
         <v>12.93</v>
       </c>
       <c r="AG133">
-        <f t="shared" ref="AG133:AG134" si="86">ROUND((R133-D133)/D133*100,2)</f>
+        <f t="shared" ref="AG133:AG135" si="86">ROUND((R133-D133)/D133*100,2)</f>
         <v>20.83</v>
       </c>
       <c r="AH133">
-        <f t="shared" ref="AH133:AH134" si="87">ROUND((S133-E133)/E133*100,2)</f>
+        <f t="shared" ref="AH133:AH135" si="87">ROUND((S133-E133)/E133*100,2)</f>
         <v>-3.17</v>
       </c>
       <c r="AI133">
-        <f t="shared" ref="AI133:AI134" si="88">ROUND((T133-F133)/F133*100,2)</f>
-        <v>15.56</v>
+        <f t="shared" ref="AI133:AI135" si="88">ROUND((T133-F133)/F133*100,2)</f>
+        <v>17.78</v>
       </c>
       <c r="AJ133">
-        <f t="shared" ref="AJ133:AJ134" si="89">ROUND((U133-G133)/G133*100,2)</f>
-        <v>11.47</v>
+        <f t="shared" ref="AJ133:AJ135" si="89">ROUND((U133-G133)/G133*100,2)</f>
+        <v>11.76</v>
       </c>
       <c r="AK133">
-        <f t="shared" ref="AK133:AK134" si="90">ROUND((V133-H133)/H133*100,2)</f>
+        <f t="shared" ref="AK133:AK135" si="90">ROUND((V133-H133)/H133*100,2)</f>
         <v>6.01</v>
       </c>
       <c r="AL133">
-        <f t="shared" ref="AL133:AL134" si="91">ROUND((W133-I133)/I133*100,2)</f>
-        <v>9.11</v>
+        <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
+        <v>9.35</v>
       </c>
       <c r="AM133">
-        <f t="shared" ref="AM133:AM134" si="92">ROUND((X133-J133)/J133*100,2)</f>
-        <v>6.61</v>
+        <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
+        <v>7.14</v>
       </c>
       <c r="AN133">
-        <f t="shared" ref="AN133:AN134" si="93">ROUND((Y133-K133)/K133*100,2)</f>
+        <f t="shared" ref="AN133:AN135" si="93">ROUND((Y133-K133)/K133*100,2)</f>
         <v>5.48</v>
       </c>
       <c r="AO133">
-        <f t="shared" ref="AO133:AO134" si="94">ROUND((Z133-L133)/L133*100,2)</f>
-        <v>7.79</v>
+        <f t="shared" ref="AO133:AO135" si="94">ROUND((Z133-L133)/L133*100,2)</f>
+        <v>8.0299999999999994</v>
       </c>
       <c r="AP133">
-        <f t="shared" ref="AP133:AP134" si="95">ROUND((AA133-M133)/M133*100,2)</f>
-        <v>-5.53</v>
+        <f t="shared" ref="AP133:AP135" si="95">ROUND((AA133-M133)/M133*100,2)</f>
+        <v>-4.6100000000000003</v>
       </c>
     </row>
     <row r="134" spans="1:42" x14ac:dyDescent="0.25">
@@ -18877,40 +18877,40 @@
         <v>217</v>
       </c>
       <c r="P134">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="Q134">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="R134">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="S134">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="T134">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="U134">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="V134">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="W134">
-        <v>529</v>
+        <v>499</v>
       </c>
       <c r="X134">
-        <v>650</v>
+        <v>614</v>
       </c>
       <c r="Y134">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Z134">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AA134">
-        <v>264</v>
+        <v>240</v>
       </c>
       <c r="AC134">
         <v>2022</v>
@@ -18920,51 +18920,51 @@
       </c>
       <c r="AE134">
         <f t="shared" si="84"/>
-        <v>16.98</v>
+        <v>14.15</v>
       </c>
       <c r="AF134">
-        <f t="shared" si="85"/>
-        <v>1.72</v>
+        <f t="shared" si="84"/>
+        <v>-1.72</v>
       </c>
       <c r="AG134">
         <f t="shared" si="86"/>
-        <v>14.43</v>
+        <v>15.46</v>
       </c>
       <c r="AH134">
         <f t="shared" si="87"/>
-        <v>3.7</v>
+        <v>2.65</v>
       </c>
       <c r="AI134">
         <f t="shared" si="88"/>
-        <v>28.89</v>
+        <v>15.56</v>
       </c>
       <c r="AJ134">
         <f t="shared" si="89"/>
-        <v>3.56</v>
+        <v>8.01</v>
       </c>
       <c r="AK134">
         <f t="shared" si="90"/>
-        <v>19.02</v>
+        <v>16.850000000000001</v>
       </c>
       <c r="AL134">
         <f t="shared" si="91"/>
-        <v>23.31</v>
+        <v>16.32</v>
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
-        <v>16.489999999999998</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AN134">
         <f t="shared" si="93"/>
-        <v>9.7200000000000006</v>
+        <v>6.94</v>
       </c>
       <c r="AO134">
         <f t="shared" si="94"/>
-        <v>7.58</v>
+        <v>7.33</v>
       </c>
       <c r="AP134">
         <f t="shared" si="95"/>
-        <v>21.66</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="135" spans="1:42" x14ac:dyDescent="0.25">
@@ -19006,6 +19006,96 @@
       </c>
       <c r="M135">
         <v>218</v>
+      </c>
+      <c r="P135">
+        <v>123</v>
+      </c>
+      <c r="Q135">
+        <v>133</v>
+      </c>
+      <c r="R135">
+        <v>134</v>
+      </c>
+      <c r="S135">
+        <v>204</v>
+      </c>
+      <c r="T135">
+        <v>59</v>
+      </c>
+      <c r="U135">
+        <v>407</v>
+      </c>
+      <c r="V135">
+        <v>201</v>
+      </c>
+      <c r="W135">
+        <v>511</v>
+      </c>
+      <c r="X135">
+        <v>687</v>
+      </c>
+      <c r="Y135">
+        <v>90</v>
+      </c>
+      <c r="Z135">
+        <v>453</v>
+      </c>
+      <c r="AA135">
+        <v>239</v>
+      </c>
+      <c r="AC135">
+        <v>2022</v>
+      </c>
+      <c r="AD135">
+        <v>29</v>
+      </c>
+      <c r="AE135">
+        <f t="shared" si="84"/>
+        <v>17.14</v>
+      </c>
+      <c r="AF135">
+        <f t="shared" si="84"/>
+        <v>15.65</v>
+      </c>
+      <c r="AG135">
+        <f t="shared" si="86"/>
+        <v>38.14</v>
+      </c>
+      <c r="AH135">
+        <f t="shared" si="87"/>
+        <v>10.27</v>
+      </c>
+      <c r="AI135">
+        <f t="shared" si="88"/>
+        <v>31.11</v>
+      </c>
+      <c r="AJ135">
+        <f t="shared" si="89"/>
+        <v>20.41</v>
+      </c>
+      <c r="AK135">
+        <f t="shared" si="90"/>
+        <v>8.06</v>
+      </c>
+      <c r="AL135">
+        <f t="shared" si="91"/>
+        <v>19.39</v>
+      </c>
+      <c r="AM135">
+        <f t="shared" si="92"/>
+        <v>22.46</v>
+      </c>
+      <c r="AN135">
+        <f t="shared" si="93"/>
+        <v>25</v>
+      </c>
+      <c r="AO135">
+        <f t="shared" si="94"/>
+        <v>11.3</v>
+      </c>
+      <c r="AP135">
+        <f t="shared" si="95"/>
+        <v>9.6300000000000008</v>
       </c>
     </row>
     <row r="136" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update excess mortality, prepare data for nowcast monkeypox
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556DADAF-391D-437B-A31E-D76877D3E532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D6511E-918C-414D-8CF2-BB760E1515E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4485" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AF135" sqref="AF135:AP135"/>
+    <sheetView tabSelected="1" topLeftCell="E103" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AI105" sqref="AI105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15492,7 +15492,7 @@
         <v>221</v>
       </c>
       <c r="W108">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="X108">
         <v>634</v>
@@ -15542,7 +15542,7 @@
       </c>
       <c r="AL108">
         <f t="shared" ref="AL108:AL121" si="31">ROUND((W108-I108)/I108*100,2)</f>
-        <v>-9.86</v>
+        <v>-9.67</v>
       </c>
       <c r="AM108">
         <f t="shared" ref="AM108:AM121" si="32">ROUND((X108-J108)/J108*100,2)</f>
@@ -15623,7 +15623,7 @@
         <v>215</v>
       </c>
       <c r="W109">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="X109">
         <v>680</v>
@@ -15673,7 +15673,7 @@
       </c>
       <c r="AL109">
         <f t="shared" si="31"/>
-        <v>-2.1</v>
+        <v>-1.9</v>
       </c>
       <c r="AM109">
         <f t="shared" si="32"/>
@@ -16525,7 +16525,7 @@
         <v>161</v>
       </c>
       <c r="R116">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S116">
         <v>245</v>
@@ -16570,7 +16570,7 @@
       </c>
       <c r="AG116">
         <f t="shared" si="26"/>
-        <v>-10.62</v>
+        <v>-9.73</v>
       </c>
       <c r="AH116">
         <f t="shared" si="27"/>
@@ -17457,7 +17457,7 @@
         <v>214</v>
       </c>
       <c r="W123">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="X123">
         <v>686</v>
@@ -17507,7 +17507,7 @@
       </c>
       <c r="AL123">
         <f t="shared" ref="AL123:AL124" si="55">ROUND((W123-I123)/I123*100,2)</f>
-        <v>-0.22</v>
+        <v>0</v>
       </c>
       <c r="AM123">
         <f t="shared" ref="AM123:AM124" si="56">ROUND((X123-J123)/J123*100,2)</f>
@@ -17588,7 +17588,7 @@
         <v>207</v>
       </c>
       <c r="W124">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="X124">
         <v>637</v>
@@ -17638,7 +17638,7 @@
       </c>
       <c r="AL124">
         <f t="shared" si="55"/>
-        <v>9.26</v>
+        <v>9.48</v>
       </c>
       <c r="AM124">
         <f t="shared" si="56"/>
@@ -17847,7 +17847,7 @@
         <v>397</v>
       </c>
       <c r="V126">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W126">
         <v>454</v>
@@ -17896,7 +17896,7 @@
       </c>
       <c r="AK126">
         <f t="shared" si="66"/>
-        <v>3.16</v>
+        <v>3.68</v>
       </c>
       <c r="AL126">
         <f t="shared" si="67"/>
@@ -17981,7 +17981,7 @@
         <v>171</v>
       </c>
       <c r="W127">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="X127">
         <v>589</v>
@@ -17990,7 +17990,7 @@
         <v>80</v>
       </c>
       <c r="Z127">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AA127">
         <v>227</v>
@@ -18031,7 +18031,7 @@
       </c>
       <c r="AL127">
         <f t="shared" ref="AL127:AL132" si="79">ROUND((W127-I127)/I127*100,2)</f>
-        <v>-1.6</v>
+        <v>-1.37</v>
       </c>
       <c r="AM127">
         <f t="shared" ref="AM127:AM132" si="80">ROUND((X127-J127)/J127*100,2)</f>
@@ -18043,7 +18043,7 @@
       </c>
       <c r="AO127">
         <f t="shared" ref="AO127:AO132" si="82">ROUND((Z127-L127)/L127*100,2)</f>
-        <v>5.69</v>
+        <v>5.92</v>
       </c>
       <c r="AP127">
         <f t="shared" ref="AP127:AP132" si="83">ROUND((AA127-M127)/M127*100,2)</f>
@@ -18112,7 +18112,7 @@
         <v>195</v>
       </c>
       <c r="W128">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="X128">
         <v>624</v>
@@ -18162,7 +18162,7 @@
       </c>
       <c r="AL128">
         <f t="shared" si="79"/>
-        <v>4.3600000000000003</v>
+        <v>4.59</v>
       </c>
       <c r="AM128">
         <f t="shared" si="80"/>
@@ -18362,7 +18362,7 @@
         <v>118</v>
       </c>
       <c r="S130">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="T130">
         <v>44</v>
@@ -18408,7 +18408,7 @@
       </c>
       <c r="AH130">
         <f t="shared" si="75"/>
-        <v>5.76</v>
+        <v>6.28</v>
       </c>
       <c r="AI130">
         <f t="shared" si="76"/>
@@ -18493,7 +18493,7 @@
         <v>105</v>
       </c>
       <c r="S131">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T131">
         <v>54</v>
@@ -18505,10 +18505,10 @@
         <v>212</v>
       </c>
       <c r="W131">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="X131">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="Y131">
         <v>93</v>
@@ -18539,7 +18539,7 @@
       </c>
       <c r="AH131">
         <f t="shared" si="75"/>
-        <v>16.32</v>
+        <v>16.84</v>
       </c>
       <c r="AI131">
         <f t="shared" si="76"/>
@@ -18555,11 +18555,11 @@
       </c>
       <c r="AL131">
         <f t="shared" si="79"/>
-        <v>3.5</v>
+        <v>3.74</v>
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>25.49</v>
+        <v>25.67</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
@@ -18648,7 +18648,7 @@
         <v>496</v>
       </c>
       <c r="AA132">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AC132">
         <v>2022</v>
@@ -18702,7 +18702,7 @@
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
-        <v>18.98</v>
+        <v>19.440000000000001</v>
       </c>
     </row>
     <row r="133" spans="1:42" x14ac:dyDescent="0.25">
@@ -18746,7 +18746,7 @@
         <v>217</v>
       </c>
       <c r="P133">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q133">
         <v>131</v>
@@ -18755,22 +18755,22 @@
         <v>116</v>
       </c>
       <c r="S133">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T133">
         <v>53</v>
       </c>
       <c r="U133">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="V133">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="W133">
         <v>468</v>
       </c>
       <c r="X133">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Y133">
         <v>77</v>
@@ -18779,7 +18779,7 @@
         <v>444</v>
       </c>
       <c r="AA133">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AC133">
         <v>2022</v>
@@ -18789,10 +18789,10 @@
       </c>
       <c r="AE133">
         <f t="shared" ref="AE133:AF135" si="84">ROUND((P133-B133)/B133*100,2)</f>
-        <v>-9.52</v>
+        <v>-8.57</v>
       </c>
       <c r="AF133">
-        <f t="shared" ref="AF133:AF134" si="85">ROUND((Q133-C133)/C133*100,2)</f>
+        <f t="shared" ref="AF133" si="85">ROUND((Q133-C133)/C133*100,2)</f>
         <v>12.93</v>
       </c>
       <c r="AG133">
@@ -18801,7 +18801,7 @@
       </c>
       <c r="AH133">
         <f t="shared" ref="AH133:AH135" si="87">ROUND((S133-E133)/E133*100,2)</f>
-        <v>-3.17</v>
+        <v>-2.65</v>
       </c>
       <c r="AI133">
         <f t="shared" ref="AI133:AI135" si="88">ROUND((T133-F133)/F133*100,2)</f>
@@ -18809,11 +18809,11 @@
       </c>
       <c r="AJ133">
         <f t="shared" ref="AJ133:AJ135" si="89">ROUND((U133-G133)/G133*100,2)</f>
-        <v>11.76</v>
+        <v>12.35</v>
       </c>
       <c r="AK133">
         <f t="shared" ref="AK133:AK135" si="90">ROUND((V133-H133)/H133*100,2)</f>
-        <v>6.01</v>
+        <v>6.56</v>
       </c>
       <c r="AL133">
         <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
@@ -18821,7 +18821,7 @@
       </c>
       <c r="AM133">
         <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
-        <v>7.14</v>
+        <v>7.32</v>
       </c>
       <c r="AN133">
         <f t="shared" ref="AN133:AN135" si="93">ROUND((Y133-K133)/K133*100,2)</f>
@@ -18833,7 +18833,7 @@
       </c>
       <c r="AP133">
         <f t="shared" ref="AP133:AP135" si="95">ROUND((AA133-M133)/M133*100,2)</f>
-        <v>-4.6100000000000003</v>
+        <v>-4.1500000000000004</v>
       </c>
     </row>
     <row r="134" spans="1:42" x14ac:dyDescent="0.25">
@@ -18892,25 +18892,25 @@
         <v>52</v>
       </c>
       <c r="U134">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="V134">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="W134">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="X134">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="Y134">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Z134">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="AA134">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="AC134">
         <v>2022</v>
@@ -18940,31 +18940,31 @@
       </c>
       <c r="AJ134">
         <f t="shared" si="89"/>
-        <v>8.01</v>
+        <v>9.5</v>
       </c>
       <c r="AK134">
         <f t="shared" si="90"/>
-        <v>16.850000000000001</v>
+        <v>17.39</v>
       </c>
       <c r="AL134">
         <f t="shared" si="91"/>
-        <v>16.32</v>
+        <v>17.72</v>
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
-        <v>10.039999999999999</v>
+        <v>10.93</v>
       </c>
       <c r="AN134">
         <f t="shared" si="93"/>
-        <v>6.94</v>
+        <v>8.33</v>
       </c>
       <c r="AO134">
         <f t="shared" si="94"/>
-        <v>7.33</v>
+        <v>8.56</v>
       </c>
       <c r="AP134">
         <f t="shared" si="95"/>
-        <v>10.6</v>
+        <v>11.98</v>
       </c>
     </row>
     <row r="135" spans="1:42" x14ac:dyDescent="0.25">
@@ -19008,40 +19008,40 @@
         <v>218</v>
       </c>
       <c r="P135">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q135">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="R135">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="S135">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="T135">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U135">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="V135">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="W135">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="X135">
-        <v>687</v>
+        <v>625</v>
       </c>
       <c r="Y135">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="Z135">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AA135">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="AC135">
         <v>2022</v>
@@ -19051,51 +19051,51 @@
       </c>
       <c r="AE135">
         <f t="shared" si="84"/>
-        <v>17.14</v>
+        <v>16.190000000000001</v>
       </c>
       <c r="AF135">
         <f t="shared" si="84"/>
-        <v>15.65</v>
+        <v>11.3</v>
       </c>
       <c r="AG135">
         <f t="shared" si="86"/>
-        <v>38.14</v>
+        <v>31.96</v>
       </c>
       <c r="AH135">
         <f t="shared" si="87"/>
-        <v>10.27</v>
+        <v>9.19</v>
       </c>
       <c r="AI135">
         <f t="shared" si="88"/>
-        <v>31.11</v>
+        <v>28.89</v>
       </c>
       <c r="AJ135">
         <f t="shared" si="89"/>
-        <v>20.41</v>
+        <v>18.34</v>
       </c>
       <c r="AK135">
         <f t="shared" si="90"/>
-        <v>8.06</v>
+        <v>3.76</v>
       </c>
       <c r="AL135">
         <f t="shared" si="91"/>
-        <v>19.39</v>
+        <v>16.36</v>
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>22.46</v>
+        <v>11.41</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
-        <v>25</v>
+        <v>33.33</v>
       </c>
       <c r="AO135">
         <f t="shared" si="94"/>
-        <v>11.3</v>
+        <v>10.81</v>
       </c>
       <c r="AP135">
         <f t="shared" si="95"/>
-        <v>9.6300000000000008</v>
+        <v>11.47</v>
       </c>
     </row>
     <row r="136" spans="1:42" x14ac:dyDescent="0.25">
@@ -19137,6 +19137,96 @@
       </c>
       <c r="M136">
         <v>216</v>
+      </c>
+      <c r="P136">
+        <v>116</v>
+      </c>
+      <c r="Q136">
+        <v>135</v>
+      </c>
+      <c r="R136">
+        <v>98</v>
+      </c>
+      <c r="S136">
+        <v>228</v>
+      </c>
+      <c r="T136">
+        <v>58</v>
+      </c>
+      <c r="U136">
+        <v>421</v>
+      </c>
+      <c r="V136">
+        <v>201</v>
+      </c>
+      <c r="W136">
+        <v>539</v>
+      </c>
+      <c r="X136">
+        <v>637</v>
+      </c>
+      <c r="Y136">
+        <v>57</v>
+      </c>
+      <c r="Z136">
+        <v>475</v>
+      </c>
+      <c r="AA136">
+        <v>248</v>
+      </c>
+      <c r="AC136">
+        <v>2022</v>
+      </c>
+      <c r="AD136">
+        <v>30</v>
+      </c>
+      <c r="AE136">
+        <f t="shared" ref="AE136" si="96">ROUND((P136-B136)/B136*100,2)</f>
+        <v>13.73</v>
+      </c>
+      <c r="AF136">
+        <f t="shared" ref="AF136" si="97">ROUND((Q136-C136)/C136*100,2)</f>
+        <v>18.420000000000002</v>
+      </c>
+      <c r="AG136">
+        <f t="shared" ref="AG136" si="98">ROUND((R136-D136)/D136*100,2)</f>
+        <v>2.08</v>
+      </c>
+      <c r="AH136">
+        <f t="shared" ref="AH136" si="99">ROUND((S136-E136)/E136*100,2)</f>
+        <v>23.24</v>
+      </c>
+      <c r="AI136">
+        <f t="shared" ref="AI136" si="100">ROUND((T136-F136)/F136*100,2)</f>
+        <v>28.89</v>
+      </c>
+      <c r="AJ136">
+        <f t="shared" ref="AJ136" si="101">ROUND((U136-G136)/G136*100,2)</f>
+        <v>24.56</v>
+      </c>
+      <c r="AK136">
+        <f t="shared" ref="AK136" si="102">ROUND((V136-H136)/H136*100,2)</f>
+        <v>8.65</v>
+      </c>
+      <c r="AL136">
+        <f t="shared" ref="AL136" si="103">ROUND((W136-I136)/I136*100,2)</f>
+        <v>26.53</v>
+      </c>
+      <c r="AM136">
+        <f t="shared" ref="AM136" si="104">ROUND((X136-J136)/J136*100,2)</f>
+        <v>13.35</v>
+      </c>
+      <c r="AN136">
+        <f t="shared" ref="AN136" si="105">ROUND((Y136-K136)/K136*100,2)</f>
+        <v>-18.57</v>
+      </c>
+      <c r="AO136">
+        <f t="shared" ref="AO136" si="106">ROUND((Z136-L136)/L136*100,2)</f>
+        <v>17.28</v>
+      </c>
+      <c r="AP136">
+        <f t="shared" ref="AP136" si="107">ROUND((AA136-M136)/M136*100,2)</f>
+        <v>14.81</v>
       </c>
     </row>
     <row r="137" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[2022-09-02] Update death comparison tracker for Twitter thread (Friday update - part 2)
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B75D467F-6753-4139-BB8D-FACB102FA350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A872C5-8D5A-4056-925E-AA99894CF651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="420" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="75" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="171">
   <si>
     <t>Groningen</t>
   </si>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH137" sqref="AH137"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,6 +1465,12 @@
       <c r="M1" t="s">
         <v>11</v>
       </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
       <c r="P1" t="s">
         <v>0</v>
       </c>
@@ -1584,6 +1590,12 @@
       <c r="M2">
         <v>251</v>
       </c>
+      <c r="N2">
+        <v>2020</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
       <c r="P2">
         <v>104</v>
       </c>
@@ -1715,6 +1727,12 @@
       <c r="M3">
         <v>254</v>
       </c>
+      <c r="N3">
+        <v>2020</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
       <c r="P3">
         <v>121</v>
       </c>
@@ -1846,6 +1864,12 @@
       <c r="M4">
         <v>258</v>
       </c>
+      <c r="N4">
+        <v>2020</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
       <c r="P4">
         <v>120</v>
       </c>
@@ -1977,6 +2001,12 @@
       <c r="M5">
         <v>262</v>
       </c>
+      <c r="N5">
+        <v>2020</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
       <c r="P5">
         <v>129</v>
       </c>
@@ -2108,6 +2138,12 @@
       <c r="M6">
         <v>269</v>
       </c>
+      <c r="N6">
+        <v>2020</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
       <c r="P6">
         <v>115</v>
       </c>
@@ -2239,6 +2275,12 @@
       <c r="M7">
         <v>272</v>
       </c>
+      <c r="N7">
+        <v>2020</v>
+      </c>
+      <c r="O7">
+        <v>6</v>
+      </c>
       <c r="P7">
         <v>123</v>
       </c>
@@ -2370,6 +2412,12 @@
       <c r="M8">
         <v>274</v>
       </c>
+      <c r="N8">
+        <v>2020</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
       <c r="P8">
         <v>91</v>
       </c>
@@ -2501,6 +2549,12 @@
       <c r="M9">
         <v>276</v>
       </c>
+      <c r="N9">
+        <v>2020</v>
+      </c>
+      <c r="O9">
+        <v>8</v>
+      </c>
       <c r="P9">
         <v>122</v>
       </c>
@@ -2632,6 +2686,12 @@
       <c r="M10">
         <v>273</v>
       </c>
+      <c r="N10">
+        <v>2020</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
       <c r="P10">
         <v>102</v>
       </c>
@@ -2763,6 +2823,12 @@
       <c r="M11">
         <v>270</v>
       </c>
+      <c r="N11">
+        <v>2020</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
       <c r="P11">
         <v>126</v>
       </c>
@@ -2894,6 +2960,12 @@
       <c r="M12">
         <v>265</v>
       </c>
+      <c r="N12">
+        <v>2020</v>
+      </c>
+      <c r="O12">
+        <v>11</v>
+      </c>
       <c r="P12">
         <v>116</v>
       </c>
@@ -3025,6 +3097,12 @@
       <c r="M13">
         <v>257</v>
       </c>
+      <c r="N13">
+        <v>2020</v>
+      </c>
+      <c r="O13">
+        <v>12</v>
+      </c>
       <c r="P13">
         <v>124</v>
       </c>
@@ -3156,6 +3234,12 @@
       <c r="M14">
         <v>249</v>
       </c>
+      <c r="N14">
+        <v>2020</v>
+      </c>
+      <c r="O14">
+        <v>13</v>
+      </c>
       <c r="P14">
         <v>122</v>
       </c>
@@ -3287,6 +3371,12 @@
       <c r="M15">
         <v>241</v>
       </c>
+      <c r="N15">
+        <v>2020</v>
+      </c>
+      <c r="O15">
+        <v>14</v>
+      </c>
       <c r="P15">
         <v>124</v>
       </c>
@@ -3418,6 +3508,12 @@
       <c r="M16">
         <v>234</v>
       </c>
+      <c r="N16">
+        <v>2020</v>
+      </c>
+      <c r="O16">
+        <v>15</v>
+      </c>
       <c r="P16">
         <v>104</v>
       </c>
@@ -3549,6 +3645,12 @@
       <c r="M17">
         <v>230</v>
       </c>
+      <c r="N17">
+        <v>2020</v>
+      </c>
+      <c r="O17">
+        <v>16</v>
+      </c>
       <c r="P17">
         <v>117</v>
       </c>
@@ -3680,6 +3782,12 @@
       <c r="M18">
         <v>226</v>
       </c>
+      <c r="N18">
+        <v>2020</v>
+      </c>
+      <c r="O18">
+        <v>17</v>
+      </c>
       <c r="P18">
         <v>107</v>
       </c>
@@ -3811,6 +3919,12 @@
       <c r="M19">
         <v>222</v>
       </c>
+      <c r="N19">
+        <v>2020</v>
+      </c>
+      <c r="O19">
+        <v>18</v>
+      </c>
       <c r="P19">
         <v>103</v>
       </c>
@@ -3942,6 +4056,12 @@
       <c r="M20">
         <v>219</v>
       </c>
+      <c r="N20">
+        <v>2020</v>
+      </c>
+      <c r="O20">
+        <v>19</v>
+      </c>
       <c r="P20">
         <v>102</v>
       </c>
@@ -4073,6 +4193,12 @@
       <c r="M21">
         <v>216</v>
       </c>
+      <c r="N21">
+        <v>2020</v>
+      </c>
+      <c r="O21">
+        <v>20</v>
+      </c>
       <c r="P21">
         <v>82</v>
       </c>
@@ -4204,6 +4330,12 @@
       <c r="M22">
         <v>214</v>
       </c>
+      <c r="N22">
+        <v>2020</v>
+      </c>
+      <c r="O22">
+        <v>21</v>
+      </c>
       <c r="P22">
         <v>95</v>
       </c>
@@ -4335,6 +4467,12 @@
       <c r="M23">
         <v>212</v>
       </c>
+      <c r="N23">
+        <v>2020</v>
+      </c>
+      <c r="O23">
+        <v>22</v>
+      </c>
       <c r="P23">
         <v>100</v>
       </c>
@@ -4466,6 +4604,12 @@
       <c r="M24">
         <v>212</v>
       </c>
+      <c r="N24">
+        <v>2020</v>
+      </c>
+      <c r="O24">
+        <v>23</v>
+      </c>
       <c r="P24">
         <v>108</v>
       </c>
@@ -4597,6 +4741,12 @@
       <c r="M25">
         <v>213</v>
       </c>
+      <c r="N25">
+        <v>2020</v>
+      </c>
+      <c r="O25">
+        <v>24</v>
+      </c>
       <c r="P25">
         <v>111</v>
       </c>
@@ -4728,6 +4878,12 @@
       <c r="M26">
         <v>213</v>
       </c>
+      <c r="N26">
+        <v>2020</v>
+      </c>
+      <c r="O26">
+        <v>25</v>
+      </c>
       <c r="P26">
         <v>97</v>
       </c>
@@ -4859,6 +5015,12 @@
       <c r="M27">
         <v>213</v>
       </c>
+      <c r="N27">
+        <v>2020</v>
+      </c>
+      <c r="O27">
+        <v>26</v>
+      </c>
       <c r="P27">
         <v>105</v>
       </c>
@@ -4990,6 +5152,12 @@
       <c r="M28">
         <v>214</v>
       </c>
+      <c r="N28">
+        <v>2020</v>
+      </c>
+      <c r="O28">
+        <v>27</v>
+      </c>
       <c r="P28">
         <v>93</v>
       </c>
@@ -5121,6 +5289,12 @@
       <c r="M29">
         <v>215</v>
       </c>
+      <c r="N29">
+        <v>2020</v>
+      </c>
+      <c r="O29">
+        <v>28</v>
+      </c>
       <c r="P29">
         <v>103</v>
       </c>
@@ -5252,6 +5426,12 @@
       <c r="M30">
         <v>216</v>
       </c>
+      <c r="N30">
+        <v>2020</v>
+      </c>
+      <c r="O30">
+        <v>29</v>
+      </c>
       <c r="P30">
         <v>88</v>
       </c>
@@ -5383,6 +5563,12 @@
       <c r="M31">
         <v>213</v>
       </c>
+      <c r="N31">
+        <v>2020</v>
+      </c>
+      <c r="O31">
+        <v>30</v>
+      </c>
       <c r="P31">
         <v>102</v>
       </c>
@@ -5514,6 +5700,12 @@
       <c r="M32">
         <v>211</v>
       </c>
+      <c r="N32">
+        <v>2020</v>
+      </c>
+      <c r="O32">
+        <v>31</v>
+      </c>
       <c r="P32">
         <v>85</v>
       </c>
@@ -5645,6 +5837,12 @@
       <c r="M33">
         <v>212</v>
       </c>
+      <c r="N33">
+        <v>2020</v>
+      </c>
+      <c r="O33">
+        <v>32</v>
+      </c>
       <c r="P33">
         <v>95</v>
       </c>
@@ -5776,6 +5974,12 @@
       <c r="M34">
         <v>209</v>
       </c>
+      <c r="N34">
+        <v>2020</v>
+      </c>
+      <c r="O34">
+        <v>33</v>
+      </c>
       <c r="P34">
         <v>128</v>
       </c>
@@ -5907,6 +6111,12 @@
       <c r="M35">
         <v>209</v>
       </c>
+      <c r="N35">
+        <v>2020</v>
+      </c>
+      <c r="O35">
+        <v>34</v>
+      </c>
       <c r="P35">
         <v>104</v>
       </c>
@@ -6038,6 +6248,12 @@
       <c r="M36">
         <v>208</v>
       </c>
+      <c r="N36">
+        <v>2020</v>
+      </c>
+      <c r="O36">
+        <v>35</v>
+      </c>
       <c r="P36">
         <v>103</v>
       </c>
@@ -6169,6 +6385,12 @@
       <c r="M37">
         <v>210</v>
       </c>
+      <c r="N37">
+        <v>2020</v>
+      </c>
+      <c r="O37">
+        <v>36</v>
+      </c>
       <c r="P37">
         <v>95</v>
       </c>
@@ -6300,6 +6522,12 @@
       <c r="M38">
         <v>213</v>
       </c>
+      <c r="N38">
+        <v>2020</v>
+      </c>
+      <c r="O38">
+        <v>37</v>
+      </c>
       <c r="P38">
         <v>109</v>
       </c>
@@ -6431,6 +6659,12 @@
       <c r="M39">
         <v>215</v>
       </c>
+      <c r="N39">
+        <v>2020</v>
+      </c>
+      <c r="O39">
+        <v>38</v>
+      </c>
       <c r="P39">
         <v>110</v>
       </c>
@@ -6562,6 +6796,12 @@
       <c r="M40">
         <v>214</v>
       </c>
+      <c r="N40">
+        <v>2020</v>
+      </c>
+      <c r="O40">
+        <v>39</v>
+      </c>
       <c r="P40">
         <v>97</v>
       </c>
@@ -6693,6 +6933,12 @@
       <c r="M41">
         <v>219</v>
       </c>
+      <c r="N41">
+        <v>2020</v>
+      </c>
+      <c r="O41">
+        <v>40</v>
+      </c>
       <c r="P41">
         <v>87</v>
       </c>
@@ -6824,6 +7070,12 @@
       <c r="M42">
         <v>221</v>
       </c>
+      <c r="N42">
+        <v>2020</v>
+      </c>
+      <c r="O42">
+        <v>41</v>
+      </c>
       <c r="P42">
         <v>89</v>
       </c>
@@ -6955,6 +7207,12 @@
       <c r="M43">
         <v>224</v>
       </c>
+      <c r="N43">
+        <v>2020</v>
+      </c>
+      <c r="O43">
+        <v>42</v>
+      </c>
       <c r="P43">
         <v>109</v>
       </c>
@@ -7086,6 +7344,12 @@
       <c r="M44">
         <v>224</v>
       </c>
+      <c r="N44">
+        <v>2020</v>
+      </c>
+      <c r="O44">
+        <v>43</v>
+      </c>
       <c r="P44">
         <v>116</v>
       </c>
@@ -7217,6 +7481,12 @@
       <c r="M45">
         <v>226</v>
       </c>
+      <c r="N45">
+        <v>2020</v>
+      </c>
+      <c r="O45">
+        <v>44</v>
+      </c>
       <c r="P45">
         <v>119</v>
       </c>
@@ -7348,6 +7618,12 @@
       <c r="M46">
         <v>228</v>
       </c>
+      <c r="N46">
+        <v>2020</v>
+      </c>
+      <c r="O46">
+        <v>45</v>
+      </c>
       <c r="P46">
         <v>118</v>
       </c>
@@ -7479,6 +7755,12 @@
       <c r="M47">
         <v>233</v>
       </c>
+      <c r="N47">
+        <v>2020</v>
+      </c>
+      <c r="O47">
+        <v>46</v>
+      </c>
       <c r="P47">
         <v>102</v>
       </c>
@@ -7610,6 +7892,12 @@
       <c r="M48">
         <v>234</v>
       </c>
+      <c r="N48">
+        <v>2020</v>
+      </c>
+      <c r="O48">
+        <v>47</v>
+      </c>
       <c r="P48">
         <v>99</v>
       </c>
@@ -7741,6 +8029,12 @@
       <c r="M49">
         <v>236</v>
       </c>
+      <c r="N49">
+        <v>2020</v>
+      </c>
+      <c r="O49">
+        <v>48</v>
+      </c>
       <c r="P49">
         <v>95</v>
       </c>
@@ -7872,6 +8166,12 @@
       <c r="M50">
         <v>238</v>
       </c>
+      <c r="N50">
+        <v>2020</v>
+      </c>
+      <c r="O50">
+        <v>49</v>
+      </c>
       <c r="P50">
         <v>131</v>
       </c>
@@ -8003,6 +8303,12 @@
       <c r="M51">
         <v>241</v>
       </c>
+      <c r="N51">
+        <v>2020</v>
+      </c>
+      <c r="O51">
+        <v>50</v>
+      </c>
       <c r="P51">
         <v>121</v>
       </c>
@@ -8134,6 +8440,12 @@
       <c r="M52">
         <v>245</v>
       </c>
+      <c r="N52">
+        <v>2020</v>
+      </c>
+      <c r="O52">
+        <v>51</v>
+      </c>
       <c r="P52">
         <v>145</v>
       </c>
@@ -8265,6 +8577,12 @@
       <c r="M53">
         <v>249</v>
       </c>
+      <c r="N53">
+        <v>2020</v>
+      </c>
+      <c r="O53">
+        <v>52</v>
+      </c>
       <c r="P53">
         <v>138</v>
       </c>
@@ -8396,6 +8714,12 @@
       <c r="M54">
         <v>251</v>
       </c>
+      <c r="N54">
+        <v>2020</v>
+      </c>
+      <c r="O54">
+        <v>53</v>
+      </c>
       <c r="P54">
         <v>150</v>
       </c>
@@ -8527,6 +8851,12 @@
       <c r="M55">
         <v>253</v>
       </c>
+      <c r="N55">
+        <v>2021</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
       <c r="P55">
         <v>147</v>
       </c>
@@ -8658,6 +8988,12 @@
       <c r="M56">
         <v>257</v>
       </c>
+      <c r="N56">
+        <v>2021</v>
+      </c>
+      <c r="O56">
+        <v>2</v>
+      </c>
       <c r="P56">
         <v>166</v>
       </c>
@@ -8789,6 +9125,12 @@
       <c r="M57">
         <v>260</v>
       </c>
+      <c r="N57">
+        <v>2021</v>
+      </c>
+      <c r="O57">
+        <v>3</v>
+      </c>
       <c r="P57">
         <v>142</v>
       </c>
@@ -8920,6 +9262,12 @@
       <c r="M58">
         <v>264</v>
       </c>
+      <c r="N58">
+        <v>2021</v>
+      </c>
+      <c r="O58">
+        <v>4</v>
+      </c>
       <c r="P58">
         <v>162</v>
       </c>
@@ -9051,6 +9399,12 @@
       <c r="M59">
         <v>272</v>
       </c>
+      <c r="N59">
+        <v>2021</v>
+      </c>
+      <c r="O59">
+        <v>5</v>
+      </c>
       <c r="P59">
         <v>133</v>
       </c>
@@ -9182,6 +9536,12 @@
       <c r="M60">
         <v>274</v>
       </c>
+      <c r="N60">
+        <v>2021</v>
+      </c>
+      <c r="O60">
+        <v>6</v>
+      </c>
       <c r="P60">
         <v>131</v>
       </c>
@@ -9313,6 +9673,12 @@
       <c r="M61">
         <v>277</v>
       </c>
+      <c r="N61">
+        <v>2021</v>
+      </c>
+      <c r="O61">
+        <v>7</v>
+      </c>
       <c r="P61">
         <v>142</v>
       </c>
@@ -9444,6 +9810,12 @@
       <c r="M62">
         <v>278</v>
       </c>
+      <c r="N62">
+        <v>2021</v>
+      </c>
+      <c r="O62">
+        <v>8</v>
+      </c>
       <c r="P62">
         <v>145</v>
       </c>
@@ -9575,6 +9947,12 @@
       <c r="M63">
         <v>276</v>
       </c>
+      <c r="N63">
+        <v>2021</v>
+      </c>
+      <c r="O63">
+        <v>9</v>
+      </c>
       <c r="P63">
         <v>135</v>
       </c>
@@ -9706,6 +10084,12 @@
       <c r="M64">
         <v>273</v>
       </c>
+      <c r="N64">
+        <v>2021</v>
+      </c>
+      <c r="O64">
+        <v>10</v>
+      </c>
       <c r="P64">
         <v>113</v>
       </c>
@@ -9837,6 +10221,12 @@
       <c r="M65">
         <v>267</v>
       </c>
+      <c r="N65">
+        <v>2021</v>
+      </c>
+      <c r="O65">
+        <v>11</v>
+      </c>
       <c r="P65">
         <v>112</v>
       </c>
@@ -9968,6 +10358,12 @@
       <c r="M66">
         <v>259</v>
       </c>
+      <c r="N66">
+        <v>2021</v>
+      </c>
+      <c r="O66">
+        <v>12</v>
+      </c>
       <c r="P66">
         <v>101</v>
       </c>
@@ -10099,6 +10495,12 @@
       <c r="M67">
         <v>251</v>
       </c>
+      <c r="N67">
+        <v>2021</v>
+      </c>
+      <c r="O67">
+        <v>13</v>
+      </c>
       <c r="P67">
         <v>113</v>
       </c>
@@ -10230,6 +10632,12 @@
       <c r="M68">
         <v>243</v>
       </c>
+      <c r="N68">
+        <v>2021</v>
+      </c>
+      <c r="O68">
+        <v>14</v>
+      </c>
       <c r="P68">
         <v>119</v>
       </c>
@@ -10361,6 +10769,12 @@
       <c r="M69">
         <v>236</v>
       </c>
+      <c r="N69">
+        <v>2021</v>
+      </c>
+      <c r="O69">
+        <v>15</v>
+      </c>
       <c r="P69">
         <v>100</v>
       </c>
@@ -10492,6 +10906,12 @@
       <c r="M70">
         <v>232</v>
       </c>
+      <c r="N70">
+        <v>2021</v>
+      </c>
+      <c r="O70">
+        <v>16</v>
+      </c>
       <c r="P70">
         <v>118</v>
       </c>
@@ -10623,6 +11043,12 @@
       <c r="M71">
         <v>228</v>
       </c>
+      <c r="N71">
+        <v>2021</v>
+      </c>
+      <c r="O71">
+        <v>17</v>
+      </c>
       <c r="P71">
         <v>101</v>
       </c>
@@ -10754,6 +11180,12 @@
       <c r="M72">
         <v>225</v>
       </c>
+      <c r="N72">
+        <v>2021</v>
+      </c>
+      <c r="O72">
+        <v>18</v>
+      </c>
       <c r="P72">
         <v>102</v>
       </c>
@@ -10885,6 +11317,12 @@
       <c r="M73">
         <v>221</v>
       </c>
+      <c r="N73">
+        <v>2021</v>
+      </c>
+      <c r="O73">
+        <v>19</v>
+      </c>
       <c r="P73">
         <v>116</v>
       </c>
@@ -11016,6 +11454,12 @@
       <c r="M74">
         <v>218</v>
       </c>
+      <c r="N74">
+        <v>2021</v>
+      </c>
+      <c r="O74">
+        <v>20</v>
+      </c>
       <c r="P74">
         <v>108</v>
       </c>
@@ -11147,6 +11591,12 @@
       <c r="M75">
         <v>216</v>
       </c>
+      <c r="N75">
+        <v>2021</v>
+      </c>
+      <c r="O75">
+        <v>21</v>
+      </c>
       <c r="P75">
         <v>109</v>
       </c>
@@ -11278,6 +11728,12 @@
       <c r="M76">
         <v>214</v>
       </c>
+      <c r="N76">
+        <v>2021</v>
+      </c>
+      <c r="O76">
+        <v>22</v>
+      </c>
       <c r="P76">
         <v>113</v>
       </c>
@@ -11409,6 +11865,12 @@
       <c r="M77">
         <v>214</v>
       </c>
+      <c r="N77">
+        <v>2021</v>
+      </c>
+      <c r="O77">
+        <v>23</v>
+      </c>
       <c r="P77">
         <v>101</v>
       </c>
@@ -11540,6 +12002,12 @@
       <c r="M78">
         <v>215</v>
       </c>
+      <c r="N78">
+        <v>2021</v>
+      </c>
+      <c r="O78">
+        <v>24</v>
+      </c>
       <c r="P78">
         <v>119</v>
       </c>
@@ -11671,6 +12139,12 @@
       <c r="M79">
         <v>215</v>
       </c>
+      <c r="N79">
+        <v>2021</v>
+      </c>
+      <c r="O79">
+        <v>25</v>
+      </c>
       <c r="P79">
         <v>96</v>
       </c>
@@ -11802,6 +12276,12 @@
       <c r="M80">
         <v>216</v>
       </c>
+      <c r="N80">
+        <v>2021</v>
+      </c>
+      <c r="O80">
+        <v>26</v>
+      </c>
       <c r="P80">
         <v>105</v>
       </c>
@@ -11933,6 +12413,12 @@
       <c r="M81">
         <v>216</v>
       </c>
+      <c r="N81">
+        <v>2021</v>
+      </c>
+      <c r="O81">
+        <v>27</v>
+      </c>
       <c r="P81">
         <v>98</v>
       </c>
@@ -12064,6 +12550,12 @@
       <c r="M82">
         <v>217</v>
       </c>
+      <c r="N82">
+        <v>2021</v>
+      </c>
+      <c r="O82">
+        <v>28</v>
+      </c>
       <c r="P82">
         <v>82</v>
       </c>
@@ -12195,6 +12687,12 @@
       <c r="M83">
         <v>218</v>
       </c>
+      <c r="N83">
+        <v>2021</v>
+      </c>
+      <c r="O83">
+        <v>29</v>
+      </c>
       <c r="P83">
         <v>97</v>
       </c>
@@ -12326,6 +12824,12 @@
       <c r="M84">
         <v>215</v>
       </c>
+      <c r="N84">
+        <v>2021</v>
+      </c>
+      <c r="O84">
+        <v>30</v>
+      </c>
       <c r="P84">
         <v>109</v>
       </c>
@@ -12457,6 +12961,12 @@
       <c r="M85">
         <v>213</v>
       </c>
+      <c r="N85">
+        <v>2021</v>
+      </c>
+      <c r="O85">
+        <v>31</v>
+      </c>
       <c r="P85">
         <v>103</v>
       </c>
@@ -12588,6 +13098,12 @@
       <c r="M86">
         <v>214</v>
       </c>
+      <c r="N86">
+        <v>2021</v>
+      </c>
+      <c r="O86">
+        <v>32</v>
+      </c>
       <c r="P86">
         <v>115</v>
       </c>
@@ -12719,6 +13235,12 @@
       <c r="M87">
         <v>211</v>
       </c>
+      <c r="N87">
+        <v>2021</v>
+      </c>
+      <c r="O87">
+        <v>33</v>
+      </c>
       <c r="P87">
         <v>106</v>
       </c>
@@ -12850,6 +13372,12 @@
       <c r="M88">
         <v>211</v>
       </c>
+      <c r="N88">
+        <v>2021</v>
+      </c>
+      <c r="O88">
+        <v>34</v>
+      </c>
       <c r="P88">
         <v>86</v>
       </c>
@@ -12981,6 +13509,12 @@
       <c r="M89">
         <v>210</v>
       </c>
+      <c r="N89">
+        <v>2021</v>
+      </c>
+      <c r="O89">
+        <v>35</v>
+      </c>
       <c r="P89">
         <v>112</v>
       </c>
@@ -13112,6 +13646,12 @@
       <c r="M90">
         <v>212</v>
       </c>
+      <c r="N90">
+        <v>2021</v>
+      </c>
+      <c r="O90">
+        <v>36</v>
+      </c>
       <c r="P90">
         <v>108</v>
       </c>
@@ -13243,6 +13783,12 @@
       <c r="M91">
         <v>215</v>
       </c>
+      <c r="N91">
+        <v>2021</v>
+      </c>
+      <c r="O91">
+        <v>37</v>
+      </c>
       <c r="P91">
         <v>93</v>
       </c>
@@ -13374,6 +13920,12 @@
       <c r="M92">
         <v>217</v>
       </c>
+      <c r="N92">
+        <v>2021</v>
+      </c>
+      <c r="O92">
+        <v>38</v>
+      </c>
       <c r="P92">
         <v>108</v>
       </c>
@@ -13505,6 +14057,12 @@
       <c r="M93">
         <v>216</v>
       </c>
+      <c r="N93">
+        <v>2021</v>
+      </c>
+      <c r="O93">
+        <v>39</v>
+      </c>
       <c r="P93">
         <v>97</v>
       </c>
@@ -13636,6 +14194,12 @@
       <c r="M94">
         <v>221</v>
       </c>
+      <c r="N94">
+        <v>2021</v>
+      </c>
+      <c r="O94">
+        <v>40</v>
+      </c>
       <c r="P94">
         <v>127</v>
       </c>
@@ -13767,6 +14331,12 @@
       <c r="M95">
         <v>223</v>
       </c>
+      <c r="N95">
+        <v>2021</v>
+      </c>
+      <c r="O95">
+        <v>41</v>
+      </c>
       <c r="P95">
         <v>109</v>
       </c>
@@ -13898,6 +14468,12 @@
       <c r="M96">
         <v>226</v>
       </c>
+      <c r="N96">
+        <v>2021</v>
+      </c>
+      <c r="O96">
+        <v>42</v>
+      </c>
       <c r="P96">
         <v>111</v>
       </c>
@@ -14029,6 +14605,12 @@
       <c r="M97">
         <v>226</v>
       </c>
+      <c r="N97">
+        <v>2021</v>
+      </c>
+      <c r="O97">
+        <v>43</v>
+      </c>
       <c r="P97">
         <v>136</v>
       </c>
@@ -14160,6 +14742,12 @@
       <c r="M98">
         <v>228</v>
       </c>
+      <c r="N98">
+        <v>2021</v>
+      </c>
+      <c r="O98">
+        <v>44</v>
+      </c>
       <c r="P98">
         <v>114</v>
       </c>
@@ -14291,6 +14879,12 @@
       <c r="M99">
         <v>230</v>
       </c>
+      <c r="N99">
+        <v>2021</v>
+      </c>
+      <c r="O99">
+        <v>45</v>
+      </c>
       <c r="P99">
         <v>156</v>
       </c>
@@ -14422,6 +15016,12 @@
       <c r="M100">
         <v>235</v>
       </c>
+      <c r="N100">
+        <v>2021</v>
+      </c>
+      <c r="O100">
+        <v>46</v>
+      </c>
       <c r="P100">
         <v>132</v>
       </c>
@@ -14553,6 +15153,12 @@
       <c r="M101">
         <v>236</v>
       </c>
+      <c r="N101">
+        <v>2021</v>
+      </c>
+      <c r="O101">
+        <v>47</v>
+      </c>
       <c r="P101">
         <v>140</v>
       </c>
@@ -14684,6 +15290,12 @@
       <c r="M102">
         <v>238</v>
       </c>
+      <c r="N102">
+        <v>2021</v>
+      </c>
+      <c r="O102">
+        <v>48</v>
+      </c>
       <c r="P102">
         <v>156</v>
       </c>
@@ -14815,6 +15427,12 @@
       <c r="M103">
         <v>240</v>
       </c>
+      <c r="N103">
+        <v>2021</v>
+      </c>
+      <c r="O103">
+        <v>49</v>
+      </c>
       <c r="P103">
         <v>137</v>
       </c>
@@ -14946,6 +15564,12 @@
       <c r="M104">
         <v>243</v>
       </c>
+      <c r="N104">
+        <v>2021</v>
+      </c>
+      <c r="O104">
+        <v>50</v>
+      </c>
       <c r="P104">
         <v>140</v>
       </c>
@@ -15077,6 +15701,12 @@
       <c r="M105">
         <v>247</v>
       </c>
+      <c r="N105">
+        <v>2021</v>
+      </c>
+      <c r="O105">
+        <v>51</v>
+      </c>
       <c r="P105">
         <v>136</v>
       </c>
@@ -15208,6 +15838,12 @@
       <c r="M106">
         <v>251</v>
       </c>
+      <c r="N106">
+        <v>2021</v>
+      </c>
+      <c r="O106">
+        <v>52</v>
+      </c>
       <c r="P106">
         <v>127</v>
       </c>
@@ -15339,6 +15975,12 @@
       <c r="M107">
         <v>254</v>
       </c>
+      <c r="N107">
+        <v>2022</v>
+      </c>
+      <c r="O107">
+        <v>1</v>
+      </c>
       <c r="P107">
         <v>119</v>
       </c>
@@ -15470,6 +16112,12 @@
       <c r="M108">
         <v>258</v>
       </c>
+      <c r="N108">
+        <v>2022</v>
+      </c>
+      <c r="O108">
+        <v>2</v>
+      </c>
       <c r="P108">
         <v>118</v>
       </c>
@@ -15601,6 +16249,12 @@
       <c r="M109">
         <v>261</v>
       </c>
+      <c r="N109">
+        <v>2022</v>
+      </c>
+      <c r="O109">
+        <v>3</v>
+      </c>
       <c r="P109">
         <v>111</v>
       </c>
@@ -15732,6 +16386,12 @@
       <c r="M110">
         <v>266</v>
       </c>
+      <c r="N110">
+        <v>2022</v>
+      </c>
+      <c r="O110">
+        <v>4</v>
+      </c>
       <c r="P110">
         <v>107</v>
       </c>
@@ -15863,6 +16523,12 @@
       <c r="M111">
         <v>273</v>
       </c>
+      <c r="N111">
+        <v>2022</v>
+      </c>
+      <c r="O111">
+        <v>5</v>
+      </c>
       <c r="P111">
         <v>110</v>
       </c>
@@ -15994,6 +16660,12 @@
       <c r="M112">
         <v>275</v>
       </c>
+      <c r="N112">
+        <v>2022</v>
+      </c>
+      <c r="O112">
+        <v>6</v>
+      </c>
       <c r="P112">
         <v>104</v>
       </c>
@@ -16019,7 +16691,7 @@
         <v>531</v>
       </c>
       <c r="X112">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="Y112">
         <v>100</v>
@@ -16070,7 +16742,7 @@
       </c>
       <c r="AM112">
         <f t="shared" si="32"/>
-        <v>-3.72</v>
+        <v>-3.58</v>
       </c>
       <c r="AN112">
         <f t="shared" si="33"/>
@@ -16125,6 +16797,12 @@
       <c r="M113">
         <v>278</v>
       </c>
+      <c r="N113">
+        <v>2022</v>
+      </c>
+      <c r="O113">
+        <v>7</v>
+      </c>
       <c r="P113">
         <v>132</v>
       </c>
@@ -16256,6 +16934,12 @@
       <c r="M114">
         <v>280</v>
       </c>
+      <c r="N114">
+        <v>2022</v>
+      </c>
+      <c r="O114">
+        <v>8</v>
+      </c>
       <c r="P114">
         <v>137</v>
       </c>
@@ -16387,6 +17071,12 @@
       <c r="M115">
         <v>277</v>
       </c>
+      <c r="N115">
+        <v>2022</v>
+      </c>
+      <c r="O115">
+        <v>9</v>
+      </c>
       <c r="P115">
         <v>106</v>
       </c>
@@ -16518,6 +17208,12 @@
       <c r="M116">
         <v>274</v>
       </c>
+      <c r="N116">
+        <v>2022</v>
+      </c>
+      <c r="O116">
+        <v>10</v>
+      </c>
       <c r="P116">
         <v>138</v>
       </c>
@@ -16649,6 +17345,12 @@
       <c r="M117">
         <v>268</v>
       </c>
+      <c r="N117">
+        <v>2022</v>
+      </c>
+      <c r="O117">
+        <v>11</v>
+      </c>
       <c r="P117">
         <v>126</v>
       </c>
@@ -16780,6 +17482,12 @@
       <c r="M118">
         <v>260</v>
       </c>
+      <c r="N118">
+        <v>2022</v>
+      </c>
+      <c r="O118">
+        <v>12</v>
+      </c>
       <c r="P118">
         <v>137</v>
       </c>
@@ -16911,6 +17619,12 @@
       <c r="M119">
         <v>252</v>
       </c>
+      <c r="N119">
+        <v>2022</v>
+      </c>
+      <c r="O119">
+        <v>13</v>
+      </c>
       <c r="P119">
         <v>127</v>
       </c>
@@ -16921,7 +17635,7 @@
         <v>128</v>
       </c>
       <c r="S119">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T119">
         <v>79</v>
@@ -16967,7 +17681,7 @@
       </c>
       <c r="AH119">
         <f t="shared" si="27"/>
-        <v>16.2</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="AI119">
         <f t="shared" si="28"/>
@@ -17042,6 +17756,12 @@
       <c r="M120">
         <v>244</v>
       </c>
+      <c r="N120">
+        <v>2022</v>
+      </c>
+      <c r="O120">
+        <v>14</v>
+      </c>
       <c r="P120">
         <v>123</v>
       </c>
@@ -17067,7 +17787,7 @@
         <v>545</v>
       </c>
       <c r="X120">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="Y120">
         <v>97</v>
@@ -17118,7 +17838,7 @@
       </c>
       <c r="AM120">
         <f t="shared" si="32"/>
-        <v>18.670000000000002</v>
+        <v>18.829999999999998</v>
       </c>
       <c r="AN120">
         <f t="shared" si="33"/>
@@ -17173,6 +17893,12 @@
       <c r="M121">
         <v>237</v>
       </c>
+      <c r="N121">
+        <v>2022</v>
+      </c>
+      <c r="O121">
+        <v>15</v>
+      </c>
       <c r="P121">
         <v>124</v>
       </c>
@@ -17304,6 +18030,12 @@
       <c r="M122">
         <v>233</v>
       </c>
+      <c r="N122">
+        <v>2022</v>
+      </c>
+      <c r="O122">
+        <v>16</v>
+      </c>
       <c r="P122">
         <v>139</v>
       </c>
@@ -17435,6 +18167,12 @@
       <c r="M123">
         <v>229</v>
       </c>
+      <c r="N123">
+        <v>2022</v>
+      </c>
+      <c r="O123">
+        <v>17</v>
+      </c>
       <c r="P123">
         <v>109</v>
       </c>
@@ -17566,6 +18304,12 @@
       <c r="M124">
         <v>225</v>
       </c>
+      <c r="N124">
+        <v>2022</v>
+      </c>
+      <c r="O124">
+        <v>18</v>
+      </c>
       <c r="P124">
         <v>135</v>
       </c>
@@ -17591,13 +18335,13 @@
         <v>485</v>
       </c>
       <c r="X124">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="Y124">
         <v>69</v>
       </c>
       <c r="Z124">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AA124">
         <v>251</v>
@@ -17642,7 +18386,7 @@
       </c>
       <c r="AM124">
         <f t="shared" si="56"/>
-        <v>9.4499999999999993</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="AN124">
         <f t="shared" si="57"/>
@@ -17650,7 +18394,7 @@
       </c>
       <c r="AO124">
         <f t="shared" si="58"/>
-        <v>12.33</v>
+        <v>12.56</v>
       </c>
       <c r="AP124">
         <f t="shared" si="59"/>
@@ -17697,6 +18441,12 @@
       <c r="M125">
         <v>222</v>
       </c>
+      <c r="N125">
+        <v>2022</v>
+      </c>
+      <c r="O125">
+        <v>19</v>
+      </c>
       <c r="P125">
         <v>126</v>
       </c>
@@ -17828,6 +18578,12 @@
       <c r="M126">
         <v>219</v>
       </c>
+      <c r="N126">
+        <v>2022</v>
+      </c>
+      <c r="O126">
+        <v>20</v>
+      </c>
       <c r="P126">
         <v>100</v>
       </c>
@@ -17844,7 +18600,7 @@
         <v>53</v>
       </c>
       <c r="U126">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="V126">
         <v>197</v>
@@ -17892,7 +18648,7 @@
       </c>
       <c r="AJ126">
         <f t="shared" si="65"/>
-        <v>12.78</v>
+        <v>13.07</v>
       </c>
       <c r="AK126">
         <f t="shared" si="66"/>
@@ -17959,6 +18715,12 @@
       <c r="M127">
         <v>217</v>
       </c>
+      <c r="N127">
+        <v>2022</v>
+      </c>
+      <c r="O127">
+        <v>21</v>
+      </c>
       <c r="P127">
         <v>108</v>
       </c>
@@ -17981,7 +18743,7 @@
         <v>171</v>
       </c>
       <c r="W127">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="X127">
         <v>590</v>
@@ -17990,7 +18752,7 @@
         <v>80</v>
       </c>
       <c r="Z127">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AA127">
         <v>227</v>
@@ -18031,7 +18793,7 @@
       </c>
       <c r="AL127">
         <f t="shared" ref="AL127:AL132" si="79">ROUND((W127-I127)/I127*100,2)</f>
-        <v>-1.1399999999999999</v>
+        <v>-0.92</v>
       </c>
       <c r="AM127">
         <f t="shared" ref="AM127:AM132" si="80">ROUND((X127-J127)/J127*100,2)</f>
@@ -18043,7 +18805,7 @@
       </c>
       <c r="AO127">
         <f t="shared" ref="AO127:AO132" si="82">ROUND((Z127-L127)/L127*100,2)</f>
-        <v>5.92</v>
+        <v>6.16</v>
       </c>
       <c r="AP127">
         <f t="shared" ref="AP127:AP132" si="83">ROUND((AA127-M127)/M127*100,2)</f>
@@ -18090,6 +18852,12 @@
       <c r="M128">
         <v>215</v>
       </c>
+      <c r="N128">
+        <v>2022</v>
+      </c>
+      <c r="O128">
+        <v>22</v>
+      </c>
       <c r="P128">
         <v>107</v>
       </c>
@@ -18115,7 +18883,7 @@
         <v>456</v>
       </c>
       <c r="X128">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="Y128">
         <v>88</v>
@@ -18166,7 +18934,7 @@
       </c>
       <c r="AM128">
         <f t="shared" si="80"/>
-        <v>11.03</v>
+        <v>11.21</v>
       </c>
       <c r="AN128">
         <f t="shared" si="81"/>
@@ -18221,6 +18989,12 @@
       <c r="M129">
         <v>215</v>
       </c>
+      <c r="N129">
+        <v>2022</v>
+      </c>
+      <c r="O129">
+        <v>23</v>
+      </c>
       <c r="P129">
         <v>109</v>
       </c>
@@ -18246,7 +19020,7 @@
         <v>438</v>
       </c>
       <c r="X129">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="Y129">
         <v>73</v>
@@ -18297,7 +19071,7 @@
       </c>
       <c r="AM129">
         <f t="shared" si="80"/>
-        <v>5.72</v>
+        <v>5.9</v>
       </c>
       <c r="AN129">
         <f t="shared" si="81"/>
@@ -18352,6 +19126,12 @@
       <c r="M130">
         <v>215</v>
       </c>
+      <c r="N130">
+        <v>2022</v>
+      </c>
+      <c r="O130">
+        <v>24</v>
+      </c>
       <c r="P130">
         <v>115</v>
       </c>
@@ -18368,16 +19148,16 @@
         <v>44</v>
       </c>
       <c r="U130">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="V130">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="W130">
         <v>447</v>
       </c>
       <c r="X130">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="Y130">
         <v>65</v>
@@ -18416,11 +19196,11 @@
       </c>
       <c r="AJ130">
         <f t="shared" si="77"/>
-        <v>5.76</v>
+        <v>6.05</v>
       </c>
       <c r="AK130">
         <f t="shared" si="78"/>
-        <v>20.11</v>
+        <v>20.65</v>
       </c>
       <c r="AL130">
         <f t="shared" si="79"/>
@@ -18428,7 +19208,7 @@
       </c>
       <c r="AM130">
         <f t="shared" si="80"/>
-        <v>8.57</v>
+        <v>8.93</v>
       </c>
       <c r="AN130">
         <f t="shared" si="81"/>
@@ -18483,6 +19263,12 @@
       <c r="M131">
         <v>216</v>
       </c>
+      <c r="N131">
+        <v>2022</v>
+      </c>
+      <c r="O131">
+        <v>25</v>
+      </c>
       <c r="P131">
         <v>116</v>
       </c>
@@ -18508,13 +19294,13 @@
         <v>444</v>
       </c>
       <c r="X131">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="Y131">
         <v>93</v>
       </c>
       <c r="Z131">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AA131">
         <v>211</v>
@@ -18559,7 +19345,7 @@
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>26.03</v>
+        <v>26.39</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
@@ -18567,7 +19353,7 @@
       </c>
       <c r="AO131">
         <f t="shared" si="82"/>
-        <v>8.94</v>
+        <v>9.18</v>
       </c>
       <c r="AP131">
         <f t="shared" si="83"/>
@@ -18614,6 +19400,12 @@
       <c r="M132">
         <v>216</v>
       </c>
+      <c r="N132">
+        <v>2022</v>
+      </c>
+      <c r="O132">
+        <v>26</v>
+      </c>
       <c r="P132">
         <v>116</v>
       </c>
@@ -18636,7 +19428,7 @@
         <v>194</v>
       </c>
       <c r="W132">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="X132">
         <v>571</v>
@@ -18645,7 +19437,7 @@
         <v>68</v>
       </c>
       <c r="Z132">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AA132">
         <v>258</v>
@@ -18686,7 +19478,7 @@
       </c>
       <c r="AL132">
         <f t="shared" si="79"/>
-        <v>11.48</v>
+        <v>11.94</v>
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
@@ -18698,7 +19490,7 @@
       </c>
       <c r="AO132">
         <f t="shared" si="82"/>
-        <v>21.22</v>
+        <v>21.46</v>
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
@@ -18745,6 +19537,12 @@
       <c r="M133">
         <v>217</v>
       </c>
+      <c r="N133">
+        <v>2022</v>
+      </c>
+      <c r="O133">
+        <v>27</v>
+      </c>
       <c r="P133">
         <v>96</v>
       </c>
@@ -18767,7 +19565,7 @@
         <v>195</v>
       </c>
       <c r="W133">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="X133">
         <v>603</v>
@@ -18817,7 +19615,7 @@
       </c>
       <c r="AL133">
         <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
-        <v>9.81</v>
+        <v>10.28</v>
       </c>
       <c r="AM133">
         <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
@@ -18876,6 +19674,12 @@
       <c r="M134">
         <v>217</v>
       </c>
+      <c r="N134">
+        <v>2022</v>
+      </c>
+      <c r="O134">
+        <v>28</v>
+      </c>
       <c r="P134">
         <v>121</v>
       </c>
@@ -18892,16 +19696,16 @@
         <v>52</v>
       </c>
       <c r="U134">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="V134">
         <v>217</v>
       </c>
       <c r="W134">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="X134">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="Y134">
         <v>78</v>
@@ -18940,7 +19744,7 @@
       </c>
       <c r="AJ134">
         <f t="shared" si="89"/>
-        <v>9.5</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="AK134">
         <f t="shared" si="90"/>
@@ -18948,11 +19752,11 @@
       </c>
       <c r="AL134">
         <f t="shared" si="91"/>
-        <v>18.18</v>
+        <v>18.649999999999999</v>
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
-        <v>11.29</v>
+        <v>11.65</v>
       </c>
       <c r="AN134">
         <f t="shared" si="93"/>
@@ -19007,6 +19811,12 @@
       <c r="M135">
         <v>218</v>
       </c>
+      <c r="N135">
+        <v>2022</v>
+      </c>
+      <c r="O135">
+        <v>29</v>
+      </c>
       <c r="P135">
         <v>122</v>
       </c>
@@ -19017,22 +19827,22 @@
         <v>128</v>
       </c>
       <c r="S135">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="T135">
         <v>59</v>
       </c>
       <c r="U135">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="V135">
         <v>193</v>
       </c>
       <c r="W135">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="X135">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="Y135">
         <v>97</v>
@@ -19063,7 +19873,7 @@
       </c>
       <c r="AH135">
         <f t="shared" si="87"/>
-        <v>9.73</v>
+        <v>11.35</v>
       </c>
       <c r="AI135">
         <f t="shared" si="88"/>
@@ -19071,7 +19881,7 @@
       </c>
       <c r="AJ135">
         <f t="shared" si="89"/>
-        <v>18.64</v>
+        <v>18.93</v>
       </c>
       <c r="AK135">
         <f t="shared" si="90"/>
@@ -19079,11 +19889,11 @@
       </c>
       <c r="AL135">
         <f t="shared" si="91"/>
-        <v>17.29</v>
+        <v>18.46</v>
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>12.3</v>
+        <v>13.01</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
@@ -19138,41 +19948,47 @@
       <c r="M136">
         <v>216</v>
       </c>
+      <c r="N136">
+        <v>2022</v>
+      </c>
+      <c r="O136">
+        <v>30</v>
+      </c>
       <c r="P136">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q136">
         <v>126</v>
       </c>
       <c r="R136">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="S136">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="T136">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="U136">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="V136">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="W136">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="X136">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="Y136">
         <v>58</v>
       </c>
       <c r="Z136">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AA136">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AC136">
         <v>2022</v>
@@ -19182,7 +19998,7 @@
       </c>
       <c r="AE136">
         <f t="shared" ref="AE136:AE137" si="96">ROUND((P136-B136)/B136*100,2)</f>
-        <v>6.86</v>
+        <v>7.84</v>
       </c>
       <c r="AF136">
         <f t="shared" ref="AF136:AF137" si="97">ROUND((Q136-C136)/C136*100,2)</f>
@@ -19190,31 +20006,31 @@
       </c>
       <c r="AG136">
         <f t="shared" ref="AG136:AG137" si="98">ROUND((R136-D136)/D136*100,2)</f>
-        <v>4.17</v>
+        <v>5.21</v>
       </c>
       <c r="AH136">
         <f t="shared" ref="AH136:AH137" si="99">ROUND((S136-E136)/E136*100,2)</f>
-        <v>19.46</v>
+        <v>20</v>
       </c>
       <c r="AI136">
         <f t="shared" ref="AI136:AI137" si="100">ROUND((T136-F136)/F136*100,2)</f>
-        <v>35.56</v>
+        <v>40</v>
       </c>
       <c r="AJ136">
         <f t="shared" ref="AJ136:AJ137" si="101">ROUND((U136-G136)/G136*100,2)</f>
-        <v>21.6</v>
+        <v>22.19</v>
       </c>
       <c r="AK136">
         <f t="shared" ref="AK136:AK137" si="102">ROUND((V136-H136)/H136*100,2)</f>
-        <v>3.78</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="AL136">
         <f t="shared" ref="AL136:AL137" si="103">ROUND((W136-I136)/I136*100,2)</f>
-        <v>19.010000000000002</v>
+        <v>19.48</v>
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>4.8</v>
+        <v>5.34</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -19222,11 +20038,11 @@
       </c>
       <c r="AO136">
         <f t="shared" ref="AO136:AO137" si="106">ROUND((Z136-L136)/L136*100,2)</f>
-        <v>17.04</v>
+        <v>17.28</v>
       </c>
       <c r="AP136">
         <f t="shared" ref="AP136:AP137" si="107">ROUND((AA136-M136)/M136*100,2)</f>
-        <v>15.28</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="137" spans="1:42" x14ac:dyDescent="0.25">
@@ -19269,8 +20085,14 @@
       <c r="M137">
         <v>214</v>
       </c>
+      <c r="N137">
+        <v>2022</v>
+      </c>
+      <c r="O137">
+        <v>31</v>
+      </c>
       <c r="P137">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="Q137">
         <v>107</v>
@@ -19279,31 +20101,31 @@
         <v>114</v>
       </c>
       <c r="S137">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="T137">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U137">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="V137">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="W137">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="X137">
-        <v>595</v>
+        <v>604</v>
       </c>
       <c r="Y137">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z137">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="AA137">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="AC137">
         <v>2022</v>
@@ -19313,7 +20135,7 @@
       </c>
       <c r="AE137">
         <f t="shared" si="96"/>
-        <v>0</v>
+        <v>1.96</v>
       </c>
       <c r="AF137">
         <f t="shared" si="97"/>
@@ -19325,39 +20147,39 @@
       </c>
       <c r="AH137">
         <f t="shared" si="99"/>
-        <v>15.3</v>
+        <v>15.85</v>
       </c>
       <c r="AI137">
         <f t="shared" si="100"/>
-        <v>-15.56</v>
+        <v>-13.33</v>
       </c>
       <c r="AJ137">
         <f t="shared" si="101"/>
-        <v>12.61</v>
+        <v>14.11</v>
       </c>
       <c r="AK137">
         <f t="shared" si="102"/>
-        <v>4.92</v>
+        <v>6.56</v>
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>3.54</v>
+        <v>5.66</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>6.44</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
-        <v>-8.57</v>
+        <v>-7.14</v>
       </c>
       <c r="AO137">
         <f t="shared" si="106"/>
-        <v>8.89</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="AP137">
         <f t="shared" si="107"/>
-        <v>-0.93</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="138" spans="1:42" x14ac:dyDescent="0.25">
@@ -19400,38 +20222,44 @@
       <c r="M138">
         <v>215</v>
       </c>
+      <c r="N138">
+        <v>2022</v>
+      </c>
+      <c r="O138">
+        <v>32</v>
+      </c>
       <c r="P138">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="Q138">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="R138">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="S138">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="T138">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="U138">
-        <v>385</v>
+        <v>393</v>
       </c>
       <c r="V138">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="W138">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="X138">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="Y138">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Z138">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="AA138">
         <v>228</v>
@@ -19443,51 +20271,51 @@
         <v>32</v>
       </c>
       <c r="AE138">
-        <f t="shared" ref="AE138" si="108">ROUND((P138-B138)/B138*100,2)</f>
-        <v>5.94</v>
+        <f t="shared" ref="AE138:AE139" si="108">ROUND((P138-B138)/B138*100,2)</f>
+        <v>9.9</v>
       </c>
       <c r="AF138">
-        <f t="shared" ref="AF138" si="109">ROUND((Q138-C138)/C138*100,2)</f>
-        <v>3.54</v>
+        <f t="shared" ref="AF138:AF139" si="109">ROUND((Q138-C138)/C138*100,2)</f>
+        <v>4.42</v>
       </c>
       <c r="AG138">
-        <f t="shared" ref="AG138" si="110">ROUND((R138-D138)/D138*100,2)</f>
-        <v>20</v>
+        <f t="shared" ref="AG138:AG139" si="110">ROUND((R138-D138)/D138*100,2)</f>
+        <v>25.26</v>
       </c>
       <c r="AH138">
-        <f t="shared" ref="AH138" si="111">ROUND((S138-E138)/E138*100,2)</f>
-        <v>14.75</v>
+        <f t="shared" ref="AH138:AH139" si="111">ROUND((S138-E138)/E138*100,2)</f>
+        <v>14.21</v>
       </c>
       <c r="AI138">
-        <f t="shared" ref="AI138" si="112">ROUND((T138-F138)/F138*100,2)</f>
-        <v>6.67</v>
+        <f t="shared" ref="AI138:AI139" si="112">ROUND((T138-F138)/F138*100,2)</f>
+        <v>8.89</v>
       </c>
       <c r="AJ138">
-        <f t="shared" ref="AJ138" si="113">ROUND((U138-G138)/G138*100,2)</f>
-        <v>15.27</v>
+        <f t="shared" ref="AJ138:AJ139" si="113">ROUND((U138-G138)/G138*100,2)</f>
+        <v>17.66</v>
       </c>
       <c r="AK138">
-        <f t="shared" ref="AK138" si="114">ROUND((V138-H138)/H138*100,2)</f>
-        <v>-1.63</v>
+        <f t="shared" ref="AK138:AK139" si="114">ROUND((V138-H138)/H138*100,2)</f>
+        <v>-5.98</v>
       </c>
       <c r="AL138">
-        <f t="shared" ref="AL138" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>4.24</v>
+        <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
+        <v>4</v>
       </c>
       <c r="AM138">
-        <f t="shared" ref="AM138" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>10.45</v>
+        <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
+        <v>5.95</v>
       </c>
       <c r="AN138">
-        <f t="shared" ref="AN138" si="117">ROUND((Y138-K138)/K138*100,2)</f>
-        <v>11.59</v>
+        <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
+        <v>13.04</v>
       </c>
       <c r="AO138">
-        <f t="shared" ref="AO138" si="118">ROUND((Z138-L138)/L138*100,2)</f>
-        <v>13.68</v>
+        <f t="shared" ref="AO138:AO139" si="118">ROUND((Z138-L138)/L138*100,2)</f>
+        <v>10.95</v>
       </c>
       <c r="AP138">
-        <f t="shared" ref="AP138" si="119">ROUND((AA138-M138)/M138*100,2)</f>
+        <f t="shared" ref="AP138:AP139" si="119">ROUND((AA138-M138)/M138*100,2)</f>
         <v>6.05</v>
       </c>
     </row>
@@ -19531,6 +20359,102 @@
       <c r="M139">
         <v>212</v>
       </c>
+      <c r="N139">
+        <v>2022</v>
+      </c>
+      <c r="O139">
+        <v>33</v>
+      </c>
+      <c r="P139">
+        <v>115</v>
+      </c>
+      <c r="Q139">
+        <v>124</v>
+      </c>
+      <c r="R139">
+        <v>122</v>
+      </c>
+      <c r="S139">
+        <v>203</v>
+      </c>
+      <c r="T139">
+        <v>55</v>
+      </c>
+      <c r="U139">
+        <v>374</v>
+      </c>
+      <c r="V139">
+        <v>208</v>
+      </c>
+      <c r="W139">
+        <v>492</v>
+      </c>
+      <c r="X139">
+        <v>593</v>
+      </c>
+      <c r="Y139">
+        <v>68</v>
+      </c>
+      <c r="Z139">
+        <v>470</v>
+      </c>
+      <c r="AA139">
+        <v>200</v>
+      </c>
+      <c r="AC139">
+        <v>2022</v>
+      </c>
+      <c r="AD139">
+        <v>33</v>
+      </c>
+      <c r="AE139">
+        <f t="shared" si="108"/>
+        <v>17.350000000000001</v>
+      </c>
+      <c r="AF139">
+        <f t="shared" si="109"/>
+        <v>10.71</v>
+      </c>
+      <c r="AG139">
+        <f t="shared" si="110"/>
+        <v>27.08</v>
+      </c>
+      <c r="AH139">
+        <f t="shared" si="111"/>
+        <v>9.73</v>
+      </c>
+      <c r="AI139">
+        <f t="shared" si="112"/>
+        <v>22.22</v>
+      </c>
+      <c r="AJ139">
+        <f t="shared" si="113"/>
+        <v>11.98</v>
+      </c>
+      <c r="AK139">
+        <f t="shared" si="114"/>
+        <v>14.29</v>
+      </c>
+      <c r="AL139">
+        <f t="shared" si="115"/>
+        <v>16.309999999999999</v>
+      </c>
+      <c r="AM139">
+        <f t="shared" si="116"/>
+        <v>7.62</v>
+      </c>
+      <c r="AN139">
+        <f t="shared" si="117"/>
+        <v>-2.86</v>
+      </c>
+      <c r="AO139">
+        <f t="shared" si="118"/>
+        <v>17.5</v>
+      </c>
+      <c r="AP139">
+        <f t="shared" si="119"/>
+        <v>-5.66</v>
+      </c>
     </row>
     <row r="140" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
@@ -19571,6 +20495,102 @@
       </c>
       <c r="M140">
         <v>212</v>
+      </c>
+      <c r="N140">
+        <v>2022</v>
+      </c>
+      <c r="O140">
+        <v>34</v>
+      </c>
+      <c r="P140">
+        <v>121</v>
+      </c>
+      <c r="Q140">
+        <v>139</v>
+      </c>
+      <c r="R140">
+        <v>113</v>
+      </c>
+      <c r="S140">
+        <v>214</v>
+      </c>
+      <c r="T140">
+        <v>38</v>
+      </c>
+      <c r="U140">
+        <v>362</v>
+      </c>
+      <c r="V140">
+        <v>220</v>
+      </c>
+      <c r="W140">
+        <v>454</v>
+      </c>
+      <c r="X140">
+        <v>617</v>
+      </c>
+      <c r="Y140">
+        <v>78</v>
+      </c>
+      <c r="Z140">
+        <v>488</v>
+      </c>
+      <c r="AA140">
+        <v>222</v>
+      </c>
+      <c r="AC140">
+        <v>2022</v>
+      </c>
+      <c r="AD140">
+        <v>34</v>
+      </c>
+      <c r="AE140">
+        <f t="shared" ref="AE140" si="120">ROUND((P140-B140)/B140*100,2)</f>
+        <v>24.74</v>
+      </c>
+      <c r="AF140">
+        <f t="shared" ref="AF140" si="121">ROUND((Q140-C140)/C140*100,2)</f>
+        <v>23.01</v>
+      </c>
+      <c r="AG140">
+        <f t="shared" ref="AG140" si="122">ROUND((R140-D140)/D140*100,2)</f>
+        <v>18.95</v>
+      </c>
+      <c r="AH140">
+        <f t="shared" ref="AH140" si="123">ROUND((S140-E140)/E140*100,2)</f>
+        <v>15.68</v>
+      </c>
+      <c r="AI140">
+        <f t="shared" ref="AI140" si="124">ROUND((T140-F140)/F140*100,2)</f>
+        <v>-13.64</v>
+      </c>
+      <c r="AJ140">
+        <f t="shared" ref="AJ140" si="125">ROUND((U140-G140)/G140*100,2)</f>
+        <v>10.029999999999999</v>
+      </c>
+      <c r="AK140">
+        <f t="shared" ref="AK140" si="126">ROUND((V140-H140)/H140*100,2)</f>
+        <v>21.55</v>
+      </c>
+      <c r="AL140">
+        <f t="shared" ref="AL140" si="127">ROUND((W140-I140)/I140*100,2)</f>
+        <v>7.58</v>
+      </c>
+      <c r="AM140">
+        <f t="shared" ref="AM140" si="128">ROUND((X140-J140)/J140*100,2)</f>
+        <v>11.78</v>
+      </c>
+      <c r="AN140">
+        <f t="shared" ref="AN140" si="129">ROUND((Y140-K140)/K140*100,2)</f>
+        <v>11.43</v>
+      </c>
+      <c r="AO140">
+        <f t="shared" ref="AO140" si="130">ROUND((Z140-L140)/L140*100,2)</f>
+        <v>22.31</v>
+      </c>
+      <c r="AP140">
+        <f t="shared" ref="AP140" si="131">ROUND((AA140-M140)/M140*100,2)</f>
+        <v>4.72</v>
       </c>
     </row>
     <row r="141" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[2022-09-15] - Monkeypox update
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A872C5-8D5A-4056-925E-AA99894CF651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B72955E-7E5B-4565-B4D1-E5B441BCDF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="75" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC139" sqref="AC139:AP141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18335,7 +18335,7 @@
         <v>485</v>
       </c>
       <c r="X124">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="Y124">
         <v>69</v>
@@ -18386,7 +18386,7 @@
       </c>
       <c r="AM124">
         <f t="shared" si="56"/>
-        <v>9.6199999999999992</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="AN124">
         <f t="shared" si="57"/>
@@ -18609,7 +18609,7 @@
         <v>454</v>
       </c>
       <c r="X126">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="Y126">
         <v>65</v>
@@ -18618,7 +18618,7 @@
         <v>494</v>
       </c>
       <c r="AA126">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AC126">
         <v>2022</v>
@@ -18660,7 +18660,7 @@
       </c>
       <c r="AM126">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="AN126">
         <f t="shared" si="69"/>
@@ -18672,7 +18672,7 @@
       </c>
       <c r="AP126">
         <f t="shared" si="71"/>
-        <v>3.65</v>
+        <v>4.1100000000000003</v>
       </c>
     </row>
     <row r="127" spans="1:42" x14ac:dyDescent="0.25">
@@ -19270,7 +19270,7 @@
         <v>25</v>
       </c>
       <c r="P131">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q131">
         <v>134</v>
@@ -19313,7 +19313,7 @@
       </c>
       <c r="AE131">
         <f t="shared" si="72"/>
-        <v>10.48</v>
+        <v>9.52</v>
       </c>
       <c r="AF131">
         <f t="shared" si="73"/>
@@ -19407,7 +19407,7 @@
         <v>26</v>
       </c>
       <c r="P132">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Q132">
         <v>149</v>
@@ -19428,7 +19428,7 @@
         <v>194</v>
       </c>
       <c r="W132">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="X132">
         <v>571</v>
@@ -19437,7 +19437,7 @@
         <v>68</v>
       </c>
       <c r="Z132">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AA132">
         <v>258</v>
@@ -19450,7 +19450,7 @@
       </c>
       <c r="AE132">
         <f t="shared" si="72"/>
-        <v>10.48</v>
+        <v>11.43</v>
       </c>
       <c r="AF132">
         <f t="shared" si="73"/>
@@ -19478,7 +19478,7 @@
       </c>
       <c r="AL132">
         <f t="shared" si="79"/>
-        <v>11.94</v>
+        <v>12.41</v>
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
@@ -19490,7 +19490,7 @@
       </c>
       <c r="AO132">
         <f t="shared" si="82"/>
-        <v>21.46</v>
+        <v>21.71</v>
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
@@ -19562,13 +19562,13 @@
         <v>382</v>
       </c>
       <c r="V133">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="W133">
         <v>472</v>
       </c>
       <c r="X133">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Y133">
         <v>77</v>
@@ -19611,7 +19611,7 @@
       </c>
       <c r="AK133">
         <f t="shared" ref="AK133:AK135" si="90">ROUND((V133-H133)/H133*100,2)</f>
-        <v>6.56</v>
+        <v>7.1</v>
       </c>
       <c r="AL133">
         <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
@@ -19619,7 +19619,7 @@
       </c>
       <c r="AM133">
         <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
-        <v>7.68</v>
+        <v>7.86</v>
       </c>
       <c r="AN133">
         <f t="shared" ref="AN133:AN135" si="93">ROUND((Y133-K133)/K133*100,2)</f>
@@ -19696,7 +19696,7 @@
         <v>52</v>
       </c>
       <c r="U134">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="V134">
         <v>217</v>
@@ -19711,7 +19711,7 @@
         <v>78</v>
       </c>
       <c r="Z134">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AA134">
         <v>244</v>
@@ -19744,7 +19744,7 @@
       </c>
       <c r="AJ134">
         <f t="shared" si="89"/>
-        <v>9.7899999999999991</v>
+        <v>10.09</v>
       </c>
       <c r="AK134">
         <f t="shared" si="90"/>
@@ -19764,7 +19764,7 @@
       </c>
       <c r="AO134">
         <f t="shared" si="94"/>
-        <v>9.0500000000000007</v>
+        <v>9.2899999999999991</v>
       </c>
       <c r="AP134">
         <f t="shared" si="95"/>
@@ -19842,7 +19842,7 @@
         <v>507</v>
       </c>
       <c r="X135">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="Y135">
         <v>97</v>
@@ -19893,7 +19893,7 @@
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>13.01</v>
+        <v>13.37</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
@@ -19961,7 +19961,7 @@
         <v>126</v>
       </c>
       <c r="R136">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S136">
         <v>222</v>
@@ -19970,7 +19970,7 @@
         <v>63</v>
       </c>
       <c r="U136">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="V136">
         <v>194</v>
@@ -19979,7 +19979,7 @@
         <v>509</v>
       </c>
       <c r="X136">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="Y136">
         <v>58</v>
@@ -20006,7 +20006,7 @@
       </c>
       <c r="AG136">
         <f t="shared" ref="AG136:AG137" si="98">ROUND((R136-D136)/D136*100,2)</f>
-        <v>5.21</v>
+        <v>6.25</v>
       </c>
       <c r="AH136">
         <f t="shared" ref="AH136:AH137" si="99">ROUND((S136-E136)/E136*100,2)</f>
@@ -20018,7 +20018,7 @@
       </c>
       <c r="AJ136">
         <f t="shared" ref="AJ136:AJ137" si="101">ROUND((U136-G136)/G136*100,2)</f>
-        <v>22.19</v>
+        <v>22.49</v>
       </c>
       <c r="AK136">
         <f t="shared" ref="AK136:AK137" si="102">ROUND((V136-H136)/H136*100,2)</f>
@@ -20030,7 +20030,7 @@
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>5.34</v>
+        <v>5.87</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20110,13 +20110,13 @@
         <v>380</v>
       </c>
       <c r="V137">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="W137">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="X137">
-        <v>604</v>
+        <v>610</v>
       </c>
       <c r="Y137">
         <v>65</v>
@@ -20159,15 +20159,15 @@
       </c>
       <c r="AK137">
         <f t="shared" si="102"/>
-        <v>6.56</v>
+        <v>7.1</v>
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>5.66</v>
+        <v>6.13</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>8.0500000000000007</v>
+        <v>9.1199999999999992</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
@@ -20229,7 +20229,7 @@
         <v>32</v>
       </c>
       <c r="P138">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Q138">
         <v>118</v>
@@ -20241,19 +20241,19 @@
         <v>209</v>
       </c>
       <c r="T138">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U138">
         <v>393</v>
       </c>
       <c r="V138">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="W138">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="X138">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="Y138">
         <v>78</v>
@@ -20262,7 +20262,7 @@
         <v>446</v>
       </c>
       <c r="AA138">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AC138">
         <v>2022</v>
@@ -20272,7 +20272,7 @@
       </c>
       <c r="AE138">
         <f t="shared" ref="AE138:AE139" si="108">ROUND((P138-B138)/B138*100,2)</f>
-        <v>9.9</v>
+        <v>10.89</v>
       </c>
       <c r="AF138">
         <f t="shared" ref="AF138:AF139" si="109">ROUND((Q138-C138)/C138*100,2)</f>
@@ -20288,7 +20288,7 @@
       </c>
       <c r="AI138">
         <f t="shared" ref="AI138:AI139" si="112">ROUND((T138-F138)/F138*100,2)</f>
-        <v>8.89</v>
+        <v>11.11</v>
       </c>
       <c r="AJ138">
         <f t="shared" ref="AJ138:AJ139" si="113">ROUND((U138-G138)/G138*100,2)</f>
@@ -20296,15 +20296,15 @@
       </c>
       <c r="AK138">
         <f t="shared" ref="AK138:AK139" si="114">ROUND((V138-H138)/H138*100,2)</f>
-        <v>-5.98</v>
+        <v>-5.43</v>
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>4</v>
+        <v>4.47</v>
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>5.95</v>
+        <v>6.13</v>
       </c>
       <c r="AN138">
         <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
@@ -20316,7 +20316,7 @@
       </c>
       <c r="AP138">
         <f t="shared" ref="AP138:AP139" si="119">ROUND((AA138-M138)/M138*100,2)</f>
-        <v>6.05</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="139" spans="1:42" x14ac:dyDescent="0.25">
@@ -20375,31 +20375,31 @@
         <v>122</v>
       </c>
       <c r="S139">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="T139">
         <v>55</v>
       </c>
       <c r="U139">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="V139">
         <v>208</v>
       </c>
       <c r="W139">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="X139">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="Y139">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Z139">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AA139">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AC139">
         <v>2022</v>
@@ -20421,7 +20421,7 @@
       </c>
       <c r="AH139">
         <f t="shared" si="111"/>
-        <v>9.73</v>
+        <v>10.81</v>
       </c>
       <c r="AI139">
         <f t="shared" si="112"/>
@@ -20429,7 +20429,7 @@
       </c>
       <c r="AJ139">
         <f t="shared" si="113"/>
-        <v>11.98</v>
+        <v>12.28</v>
       </c>
       <c r="AK139">
         <f t="shared" si="114"/>
@@ -20437,23 +20437,23 @@
       </c>
       <c r="AL139">
         <f t="shared" si="115"/>
-        <v>16.309999999999999</v>
+        <v>17.260000000000002</v>
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>7.62</v>
+        <v>8.17</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
-        <v>-2.86</v>
+        <v>0</v>
       </c>
       <c r="AO139">
         <f t="shared" si="118"/>
-        <v>17.5</v>
+        <v>17.75</v>
       </c>
       <c r="AP139">
         <f t="shared" si="119"/>
-        <v>-5.66</v>
+        <v>-4.72</v>
       </c>
     </row>
     <row r="140" spans="1:42" x14ac:dyDescent="0.25">
@@ -20503,40 +20503,40 @@
         <v>34</v>
       </c>
       <c r="P140">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="Q140">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="R140">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="S140">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="T140">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U140">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="V140">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="W140">
-        <v>454</v>
+        <v>430</v>
       </c>
       <c r="X140">
-        <v>617</v>
+        <v>589</v>
       </c>
       <c r="Y140">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="Z140">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="AA140">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="AC140">
         <v>2022</v>
@@ -20545,52 +20545,52 @@
         <v>34</v>
       </c>
       <c r="AE140">
-        <f t="shared" ref="AE140" si="120">ROUND((P140-B140)/B140*100,2)</f>
-        <v>24.74</v>
+        <f t="shared" ref="AE140:AE141" si="120">ROUND((P140-B140)/B140*100,2)</f>
+        <v>21.65</v>
       </c>
       <c r="AF140">
-        <f t="shared" ref="AF140" si="121">ROUND((Q140-C140)/C140*100,2)</f>
-        <v>23.01</v>
+        <f t="shared" ref="AF140:AF141" si="121">ROUND((Q140-C140)/C140*100,2)</f>
+        <v>21.24</v>
       </c>
       <c r="AG140">
-        <f t="shared" ref="AG140" si="122">ROUND((R140-D140)/D140*100,2)</f>
-        <v>18.95</v>
+        <f t="shared" ref="AG140:AG141" si="122">ROUND((R140-D140)/D140*100,2)</f>
+        <v>13.68</v>
       </c>
       <c r="AH140">
-        <f t="shared" ref="AH140" si="123">ROUND((S140-E140)/E140*100,2)</f>
-        <v>15.68</v>
+        <f t="shared" ref="AH140:AH141" si="123">ROUND((S140-E140)/E140*100,2)</f>
+        <v>18.38</v>
       </c>
       <c r="AI140">
-        <f t="shared" ref="AI140" si="124">ROUND((T140-F140)/F140*100,2)</f>
-        <v>-13.64</v>
+        <f t="shared" ref="AI140:AI141" si="124">ROUND((T140-F140)/F140*100,2)</f>
+        <v>-11.36</v>
       </c>
       <c r="AJ140">
-        <f t="shared" ref="AJ140" si="125">ROUND((U140-G140)/G140*100,2)</f>
-        <v>10.029999999999999</v>
+        <f t="shared" ref="AJ140:AJ141" si="125">ROUND((U140-G140)/G140*100,2)</f>
+        <v>6.69</v>
       </c>
       <c r="AK140">
-        <f t="shared" ref="AK140" si="126">ROUND((V140-H140)/H140*100,2)</f>
-        <v>21.55</v>
+        <f t="shared" ref="AK140:AK141" si="126">ROUND((V140-H140)/H140*100,2)</f>
+        <v>13.81</v>
       </c>
       <c r="AL140">
-        <f t="shared" ref="AL140" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>7.58</v>
+        <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
+        <v>1.9</v>
       </c>
       <c r="AM140">
-        <f t="shared" ref="AM140" si="128">ROUND((X140-J140)/J140*100,2)</f>
-        <v>11.78</v>
+        <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
+        <v>6.7</v>
       </c>
       <c r="AN140">
-        <f t="shared" ref="AN140" si="129">ROUND((Y140-K140)/K140*100,2)</f>
-        <v>11.43</v>
+        <f t="shared" ref="AN140:AN141" si="129">ROUND((Y140-K140)/K140*100,2)</f>
+        <v>20</v>
       </c>
       <c r="AO140">
-        <f t="shared" ref="AO140" si="130">ROUND((Z140-L140)/L140*100,2)</f>
-        <v>22.31</v>
+        <f t="shared" ref="AO140:AO141" si="130">ROUND((Z140-L140)/L140*100,2)</f>
+        <v>21.05</v>
       </c>
       <c r="AP140">
-        <f t="shared" ref="AP140" si="131">ROUND((AA140-M140)/M140*100,2)</f>
-        <v>4.72</v>
+        <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
+        <v>8.02</v>
       </c>
     </row>
     <row r="141" spans="1:42" x14ac:dyDescent="0.25">
@@ -20632,6 +20632,102 @@
       </c>
       <c r="M141">
         <v>211</v>
+      </c>
+      <c r="N141">
+        <v>2022</v>
+      </c>
+      <c r="O141">
+        <v>35</v>
+      </c>
+      <c r="P141">
+        <v>85</v>
+      </c>
+      <c r="Q141">
+        <v>114</v>
+      </c>
+      <c r="R141">
+        <v>118</v>
+      </c>
+      <c r="S141">
+        <v>206</v>
+      </c>
+      <c r="T141">
+        <v>55</v>
+      </c>
+      <c r="U141">
+        <v>393</v>
+      </c>
+      <c r="V141">
+        <v>196</v>
+      </c>
+      <c r="W141">
+        <v>396</v>
+      </c>
+      <c r="X141">
+        <v>600</v>
+      </c>
+      <c r="Y141">
+        <v>66</v>
+      </c>
+      <c r="Z141">
+        <v>459</v>
+      </c>
+      <c r="AA141">
+        <v>237</v>
+      </c>
+      <c r="AC141">
+        <v>2022</v>
+      </c>
+      <c r="AD141">
+        <v>35</v>
+      </c>
+      <c r="AE141">
+        <f t="shared" si="120"/>
+        <v>-13.27</v>
+      </c>
+      <c r="AF141">
+        <f t="shared" si="121"/>
+        <v>0.88</v>
+      </c>
+      <c r="AG141">
+        <f t="shared" si="122"/>
+        <v>22.92</v>
+      </c>
+      <c r="AH141">
+        <f t="shared" si="123"/>
+        <v>11.35</v>
+      </c>
+      <c r="AI141">
+        <f t="shared" si="124"/>
+        <v>27.91</v>
+      </c>
+      <c r="AJ141">
+        <f t="shared" si="125"/>
+        <v>18.37</v>
+      </c>
+      <c r="AK141">
+        <f t="shared" si="126"/>
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="AL141">
+        <f t="shared" si="127"/>
+        <v>-6.6</v>
+      </c>
+      <c r="AM141">
+        <f t="shared" si="128"/>
+        <v>8.89</v>
+      </c>
+      <c r="AN141">
+        <f t="shared" si="129"/>
+        <v>-5.71</v>
+      </c>
+      <c r="AO141">
+        <f t="shared" si="130"/>
+        <v>14.18</v>
+      </c>
+      <c r="AP141">
+        <f t="shared" si="131"/>
+        <v>12.32</v>
       </c>
     </row>
     <row r="142" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Automate parsing data for causes of death
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B72955E-7E5B-4565-B4D1-E5B441BCDF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB99B8F3-B5AF-4A12-BD20-537224857BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC139" sqref="AC139:AP141"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH141" sqref="AH141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17796,7 +17796,7 @@
         <v>529</v>
       </c>
       <c r="AA120">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AC120">
         <v>2022</v>
@@ -17850,7 +17850,7 @@
       </c>
       <c r="AP120">
         <f t="shared" si="35"/>
-        <v>11.48</v>
+        <v>11.89</v>
       </c>
     </row>
     <row r="121" spans="1:42" x14ac:dyDescent="0.25">
@@ -18195,7 +18195,7 @@
         <v>215</v>
       </c>
       <c r="W123">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="X123">
         <v>686</v>
@@ -18245,7 +18245,7 @@
       </c>
       <c r="AL123">
         <f t="shared" ref="AL123:AL124" si="55">ROUND((W123-I123)/I123*100,2)</f>
-        <v>0</v>
+        <v>0.22</v>
       </c>
       <c r="AM123">
         <f t="shared" ref="AM123:AM124" si="56">ROUND((X123-J123)/J123*100,2)</f>
@@ -18472,7 +18472,7 @@
         <v>514</v>
       </c>
       <c r="X125">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="Y125">
         <v>91</v>
@@ -18523,7 +18523,7 @@
       </c>
       <c r="AM125">
         <f t="shared" ref="AM125:AM126" si="68">ROUND((X125-J125)/J125*100,2)</f>
-        <v>1.04</v>
+        <v>1.21</v>
       </c>
       <c r="AN125">
         <f t="shared" ref="AN125:AN126" si="69">ROUND((Y125-K125)/K125*100,2)</f>
@@ -18606,7 +18606,7 @@
         <v>197</v>
       </c>
       <c r="W126">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="X126">
         <v>572</v>
@@ -18615,7 +18615,7 @@
         <v>65</v>
       </c>
       <c r="Z126">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AA126">
         <v>228</v>
@@ -18656,7 +18656,7 @@
       </c>
       <c r="AL126">
         <f t="shared" si="67"/>
-        <v>2.95</v>
+        <v>3.17</v>
       </c>
       <c r="AM126">
         <f t="shared" si="68"/>
@@ -18668,7 +18668,7 @@
       </c>
       <c r="AO126">
         <f t="shared" si="70"/>
-        <v>15.69</v>
+        <v>15.93</v>
       </c>
       <c r="AP126">
         <f t="shared" si="71"/>
@@ -19166,7 +19166,7 @@
         <v>466</v>
       </c>
       <c r="AA130">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AC130">
         <v>2022</v>
@@ -19220,7 +19220,7 @@
       </c>
       <c r="AP130">
         <f t="shared" si="83"/>
-        <v>6.05</v>
+        <v>6.51</v>
       </c>
     </row>
     <row r="131" spans="1:42" x14ac:dyDescent="0.25">
@@ -19419,7 +19419,7 @@
         <v>206</v>
       </c>
       <c r="T132">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="U132">
         <v>373</v>
@@ -19440,7 +19440,7 @@
         <v>499</v>
       </c>
       <c r="AA132">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="AC132">
         <v>2022</v>
@@ -19466,7 +19466,7 @@
       </c>
       <c r="AI132">
         <f t="shared" si="76"/>
-        <v>15.91</v>
+        <v>18.18</v>
       </c>
       <c r="AJ132">
         <f t="shared" si="77"/>
@@ -19494,7 +19494,7 @@
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
-        <v>19.440000000000001</v>
+        <v>19.91</v>
       </c>
     </row>
     <row r="133" spans="1:42" x14ac:dyDescent="0.25">
@@ -19562,7 +19562,7 @@
         <v>382</v>
       </c>
       <c r="V133">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W133">
         <v>472</v>
@@ -19611,7 +19611,7 @@
       </c>
       <c r="AK133">
         <f t="shared" ref="AK133:AK135" si="90">ROUND((V133-H133)/H133*100,2)</f>
-        <v>7.1</v>
+        <v>7.65</v>
       </c>
       <c r="AL133">
         <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
@@ -19705,7 +19705,7 @@
         <v>509</v>
       </c>
       <c r="X134">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="Y134">
         <v>78</v>
@@ -19756,7 +19756,7 @@
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
-        <v>11.65</v>
+        <v>11.83</v>
       </c>
       <c r="AN134">
         <f t="shared" si="93"/>
@@ -19839,7 +19839,7 @@
         <v>193</v>
       </c>
       <c r="W135">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="X135">
         <v>636</v>
@@ -19851,7 +19851,7 @@
         <v>452</v>
       </c>
       <c r="AA135">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AC135">
         <v>2022</v>
@@ -19889,7 +19889,7 @@
       </c>
       <c r="AL135">
         <f t="shared" si="91"/>
-        <v>18.46</v>
+        <v>18.690000000000001</v>
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
@@ -19905,7 +19905,7 @@
       </c>
       <c r="AP135">
         <f t="shared" si="95"/>
-        <v>11.93</v>
+        <v>12.39</v>
       </c>
     </row>
     <row r="136" spans="1:42" x14ac:dyDescent="0.25">
@@ -19979,7 +19979,7 @@
         <v>509</v>
       </c>
       <c r="X136">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="Y136">
         <v>58</v>
@@ -20030,7 +20030,7 @@
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>5.87</v>
+        <v>6.05</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20101,7 +20101,7 @@
         <v>114</v>
       </c>
       <c r="S137">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="T137">
         <v>39</v>
@@ -20110,13 +20110,13 @@
         <v>380</v>
       </c>
       <c r="V137">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="W137">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="X137">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="Y137">
         <v>65</v>
@@ -20125,7 +20125,7 @@
         <v>443</v>
       </c>
       <c r="AA137">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="AC137">
         <v>2022</v>
@@ -20147,7 +20147,7 @@
       </c>
       <c r="AH137">
         <f t="shared" si="99"/>
-        <v>15.85</v>
+        <v>16.39</v>
       </c>
       <c r="AI137">
         <f t="shared" si="100"/>
@@ -20159,15 +20159,15 @@
       </c>
       <c r="AK137">
         <f t="shared" si="102"/>
-        <v>7.1</v>
+        <v>7.65</v>
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>6.13</v>
+        <v>6.6</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>9.1199999999999992</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
@@ -20179,7 +20179,7 @@
       </c>
       <c r="AP137">
         <f t="shared" si="107"/>
-        <v>0.93</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="138" spans="1:42" x14ac:dyDescent="0.25">
@@ -20232,28 +20232,28 @@
         <v>112</v>
       </c>
       <c r="Q138">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="R138">
         <v>119</v>
       </c>
       <c r="S138">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="T138">
         <v>50</v>
       </c>
       <c r="U138">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="V138">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="W138">
         <v>444</v>
       </c>
       <c r="X138">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="Y138">
         <v>78</v>
@@ -20276,7 +20276,7 @@
       </c>
       <c r="AF138">
         <f t="shared" ref="AF138:AF139" si="109">ROUND((Q138-C138)/C138*100,2)</f>
-        <v>4.42</v>
+        <v>5.31</v>
       </c>
       <c r="AG138">
         <f t="shared" ref="AG138:AG139" si="110">ROUND((R138-D138)/D138*100,2)</f>
@@ -20284,7 +20284,7 @@
       </c>
       <c r="AH138">
         <f t="shared" ref="AH138:AH139" si="111">ROUND((S138-E138)/E138*100,2)</f>
-        <v>14.21</v>
+        <v>15.3</v>
       </c>
       <c r="AI138">
         <f t="shared" ref="AI138:AI139" si="112">ROUND((T138-F138)/F138*100,2)</f>
@@ -20292,11 +20292,11 @@
       </c>
       <c r="AJ138">
         <f t="shared" ref="AJ138:AJ139" si="113">ROUND((U138-G138)/G138*100,2)</f>
-        <v>17.66</v>
+        <v>17.96</v>
       </c>
       <c r="AK138">
         <f t="shared" ref="AK138:AK139" si="114">ROUND((V138-H138)/H138*100,2)</f>
-        <v>-5.43</v>
+        <v>-4.8899999999999997</v>
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
@@ -20304,7 +20304,7 @@
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>6.13</v>
+        <v>6.31</v>
       </c>
       <c r="AN138">
         <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
@@ -20381,25 +20381,25 @@
         <v>55</v>
       </c>
       <c r="U139">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="V139">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="W139">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="X139">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="Y139">
         <v>70</v>
       </c>
       <c r="Z139">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AA139">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="AC139">
         <v>2022</v>
@@ -20429,19 +20429,19 @@
       </c>
       <c r="AJ139">
         <f t="shared" si="113"/>
-        <v>12.28</v>
+        <v>13.47</v>
       </c>
       <c r="AK139">
         <f t="shared" si="114"/>
-        <v>14.29</v>
+        <v>14.84</v>
       </c>
       <c r="AL139">
         <f t="shared" si="115"/>
-        <v>17.260000000000002</v>
+        <v>17.489999999999998</v>
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>8.17</v>
+        <v>8.89</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20449,11 +20449,11 @@
       </c>
       <c r="AO139">
         <f t="shared" si="118"/>
-        <v>17.75</v>
+        <v>18</v>
       </c>
       <c r="AP139">
         <f t="shared" si="119"/>
-        <v>-4.72</v>
+        <v>-4.25</v>
       </c>
     </row>
     <row r="140" spans="1:42" x14ac:dyDescent="0.25">
@@ -20515,28 +20515,28 @@
         <v>219</v>
       </c>
       <c r="T140">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U140">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="V140">
         <v>206</v>
       </c>
       <c r="W140">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="X140">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="Y140">
         <v>84</v>
       </c>
       <c r="Z140">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AA140">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AC140">
         <v>2022</v>
@@ -20562,11 +20562,11 @@
       </c>
       <c r="AI140">
         <f t="shared" ref="AI140:AI141" si="124">ROUND((T140-F140)/F140*100,2)</f>
-        <v>-11.36</v>
+        <v>-9.09</v>
       </c>
       <c r="AJ140">
         <f t="shared" ref="AJ140:AJ141" si="125">ROUND((U140-G140)/G140*100,2)</f>
-        <v>6.69</v>
+        <v>7.9</v>
       </c>
       <c r="AK140">
         <f t="shared" ref="AK140:AK141" si="126">ROUND((V140-H140)/H140*100,2)</f>
@@ -20574,11 +20574,11 @@
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>1.9</v>
+        <v>3.32</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
-        <v>6.7</v>
+        <v>7.07</v>
       </c>
       <c r="AN140">
         <f t="shared" ref="AN140:AN141" si="129">ROUND((Y140-K140)/K140*100,2)</f>
@@ -20586,11 +20586,11 @@
       </c>
       <c r="AO140">
         <f t="shared" ref="AO140:AO141" si="130">ROUND((Z140-L140)/L140*100,2)</f>
-        <v>21.05</v>
+        <v>21.8</v>
       </c>
       <c r="AP140">
         <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
-        <v>8.02</v>
+        <v>8.49</v>
       </c>
     </row>
     <row r="141" spans="1:42" x14ac:dyDescent="0.25">
@@ -20640,40 +20640,40 @@
         <v>35</v>
       </c>
       <c r="P141">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="Q141">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="R141">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S141">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T141">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="U141">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="V141">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="W141">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="X141">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="Y141">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="Z141">
-        <v>459</v>
+        <v>471</v>
       </c>
       <c r="AA141">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AC141">
         <v>2022</v>
@@ -20683,51 +20683,51 @@
       </c>
       <c r="AE141">
         <f t="shared" si="120"/>
-        <v>-13.27</v>
+        <v>-10.199999999999999</v>
       </c>
       <c r="AF141">
         <f t="shared" si="121"/>
-        <v>0.88</v>
+        <v>7.08</v>
       </c>
       <c r="AG141">
         <f t="shared" si="122"/>
-        <v>22.92</v>
+        <v>20.83</v>
       </c>
       <c r="AH141">
         <f t="shared" si="123"/>
-        <v>11.35</v>
+        <v>9.19</v>
       </c>
       <c r="AI141">
         <f t="shared" si="124"/>
-        <v>27.91</v>
+        <v>16.28</v>
       </c>
       <c r="AJ141">
         <f t="shared" si="125"/>
-        <v>18.37</v>
+        <v>16.57</v>
       </c>
       <c r="AK141">
         <f t="shared" si="126"/>
-        <v>8.2899999999999991</v>
+        <v>3.31</v>
       </c>
       <c r="AL141">
         <f t="shared" si="127"/>
-        <v>-6.6</v>
+        <v>-7.78</v>
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>8.89</v>
+        <v>6.72</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
-        <v>-5.71</v>
+        <v>1.43</v>
       </c>
       <c r="AO141">
         <f t="shared" si="130"/>
-        <v>14.18</v>
+        <v>17.16</v>
       </c>
       <c r="AP141">
         <f t="shared" si="131"/>
-        <v>12.32</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="142" spans="1:42" x14ac:dyDescent="0.25">
@@ -20769,6 +20769,102 @@
       </c>
       <c r="M142">
         <v>213</v>
+      </c>
+      <c r="N142">
+        <v>2022</v>
+      </c>
+      <c r="O142">
+        <v>36</v>
+      </c>
+      <c r="P142">
+        <v>124</v>
+      </c>
+      <c r="Q142">
+        <v>115</v>
+      </c>
+      <c r="R142">
+        <v>89</v>
+      </c>
+      <c r="S142">
+        <v>197</v>
+      </c>
+      <c r="T142">
+        <v>47</v>
+      </c>
+      <c r="U142">
+        <v>368</v>
+      </c>
+      <c r="V142">
+        <v>183</v>
+      </c>
+      <c r="W142">
+        <v>484</v>
+      </c>
+      <c r="X142">
+        <v>594</v>
+      </c>
+      <c r="Y142">
+        <v>73</v>
+      </c>
+      <c r="Z142">
+        <v>442</v>
+      </c>
+      <c r="AA142">
+        <v>220</v>
+      </c>
+      <c r="AC142">
+        <v>2022</v>
+      </c>
+      <c r="AD142">
+        <v>36</v>
+      </c>
+      <c r="AE142">
+        <f t="shared" ref="AE142" si="132">ROUND((P142-B142)/B142*100,2)</f>
+        <v>26.53</v>
+      </c>
+      <c r="AF142">
+        <f t="shared" ref="AF142" si="133">ROUND((Q142-C142)/C142*100,2)</f>
+        <v>1.77</v>
+      </c>
+      <c r="AG142">
+        <f t="shared" ref="AG142" si="134">ROUND((R142-D142)/D142*100,2)</f>
+        <v>-6.32</v>
+      </c>
+      <c r="AH142">
+        <f t="shared" ref="AH142" si="135">ROUND((S142-E142)/E142*100,2)</f>
+        <v>4.79</v>
+      </c>
+      <c r="AI142">
+        <f t="shared" ref="AI142" si="136">ROUND((T142-F142)/F142*100,2)</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AJ142">
+        <f t="shared" ref="AJ142" si="137">ROUND((U142-G142)/G142*100,2)</f>
+        <v>10.18</v>
+      </c>
+      <c r="AK142">
+        <f t="shared" ref="AK142" si="138">ROUND((V142-H142)/H142*100,2)</f>
+        <v>1.67</v>
+      </c>
+      <c r="AL142">
+        <f t="shared" ref="AL142" si="139">ROUND((W142-I142)/I142*100,2)</f>
+        <v>14.15</v>
+      </c>
+      <c r="AM142">
+        <f t="shared" ref="AM142" si="140">ROUND((X142-J142)/J142*100,2)</f>
+        <v>7.03</v>
+      </c>
+      <c r="AN142">
+        <f t="shared" ref="AN142" si="141">ROUND((Y142-K142)/K142*100,2)</f>
+        <v>4.29</v>
+      </c>
+      <c r="AO142">
+        <f t="shared" ref="AO142" si="142">ROUND((Z142-L142)/L142*100,2)</f>
+        <v>9.68</v>
+      </c>
+      <c r="AP142">
+        <f t="shared" ref="AP142" si="143">ROUND((AA142-M142)/M142*100,2)</f>
+        <v>3.29</v>
       </c>
     </row>
     <row r="143" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[2022-09-30] - Monkeypox update (code)
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB99B8F3-B5AF-4A12-BD20-537224857BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE87BD37-D9BD-4403-8C3B-2B8199F11221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH141" sqref="AH141"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AL144" sqref="AL144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18189,7 +18189,7 @@
         <v>58</v>
       </c>
       <c r="U123">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="V123">
         <v>215</v>
@@ -18237,7 +18237,7 @@
       </c>
       <c r="AJ123">
         <f t="shared" ref="AJ123:AJ124" si="53">ROUND((U123-G123)/G123*100,2)</f>
-        <v>8.86</v>
+        <v>9.14</v>
       </c>
       <c r="AK123">
         <f t="shared" ref="AK123:AK124" si="54">ROUND((V123-H123)/H123*100,2)</f>
@@ -18469,7 +18469,7 @@
         <v>208</v>
       </c>
       <c r="W125">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="X125">
         <v>585</v>
@@ -18519,7 +18519,7 @@
       </c>
       <c r="AL125">
         <f t="shared" ref="AL125:AL126" si="67">ROUND((W125-I125)/I125*100,2)</f>
-        <v>16.03</v>
+        <v>16.25</v>
       </c>
       <c r="AM125">
         <f t="shared" ref="AM125:AM126" si="68">ROUND((X125-J125)/J125*100,2)</f>
@@ -18609,7 +18609,7 @@
         <v>455</v>
       </c>
       <c r="X126">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="Y126">
         <v>65</v>
@@ -18660,7 +18660,7 @@
       </c>
       <c r="AM126">
         <f t="shared" si="68"/>
-        <v>0.18</v>
+        <v>0.35</v>
       </c>
       <c r="AN126">
         <f t="shared" si="69"/>
@@ -19020,7 +19020,7 @@
         <v>438</v>
       </c>
       <c r="X129">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="Y129">
         <v>73</v>
@@ -19071,7 +19071,7 @@
       </c>
       <c r="AM129">
         <f t="shared" si="80"/>
-        <v>5.9</v>
+        <v>6.08</v>
       </c>
       <c r="AN129">
         <f t="shared" si="81"/>
@@ -19416,7 +19416,7 @@
         <v>123</v>
       </c>
       <c r="S132">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="T132">
         <v>52</v>
@@ -19431,16 +19431,16 @@
         <v>480</v>
       </c>
       <c r="X132">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="Y132">
         <v>68</v>
       </c>
       <c r="Z132">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AA132">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AC132">
         <v>2022</v>
@@ -19462,7 +19462,7 @@
       </c>
       <c r="AH132">
         <f t="shared" si="75"/>
-        <v>8.42</v>
+        <v>10</v>
       </c>
       <c r="AI132">
         <f t="shared" si="76"/>
@@ -19482,7 +19482,7 @@
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
-        <v>2.15</v>
+        <v>2.5</v>
       </c>
       <c r="AN132">
         <f t="shared" si="81"/>
@@ -19490,11 +19490,11 @@
       </c>
       <c r="AO132">
         <f t="shared" si="82"/>
-        <v>21.71</v>
+        <v>21.95</v>
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
-        <v>19.91</v>
+        <v>20.37</v>
       </c>
     </row>
     <row r="133" spans="1:42" x14ac:dyDescent="0.25">
@@ -19568,7 +19568,7 @@
         <v>472</v>
       </c>
       <c r="X133">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="Y133">
         <v>77</v>
@@ -19619,7 +19619,7 @@
       </c>
       <c r="AM133">
         <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
-        <v>7.86</v>
+        <v>8.0399999999999991</v>
       </c>
       <c r="AN133">
         <f t="shared" ref="AN133:AN135" si="93">ROUND((Y133-K133)/K133*100,2)</f>
@@ -19833,16 +19833,16 @@
         <v>59</v>
       </c>
       <c r="U135">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V135">
         <v>193</v>
       </c>
       <c r="W135">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="X135">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="Y135">
         <v>97</v>
@@ -19881,7 +19881,7 @@
       </c>
       <c r="AJ135">
         <f t="shared" si="89"/>
-        <v>18.93</v>
+        <v>19.23</v>
       </c>
       <c r="AK135">
         <f t="shared" si="90"/>
@@ -19889,11 +19889,11 @@
       </c>
       <c r="AL135">
         <f t="shared" si="91"/>
-        <v>18.690000000000001</v>
+        <v>18.93</v>
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>13.37</v>
+        <v>13.73</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
@@ -19967,7 +19967,7 @@
         <v>222</v>
       </c>
       <c r="T136">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U136">
         <v>414</v>
@@ -19976,16 +19976,16 @@
         <v>194</v>
       </c>
       <c r="W136">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="X136">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="Y136">
         <v>58</v>
       </c>
       <c r="Z136">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="AA136">
         <v>251</v>
@@ -20014,7 +20014,7 @@
       </c>
       <c r="AI136">
         <f t="shared" ref="AI136:AI137" si="100">ROUND((T136-F136)/F136*100,2)</f>
-        <v>40</v>
+        <v>42.22</v>
       </c>
       <c r="AJ136">
         <f t="shared" ref="AJ136:AJ137" si="101">ROUND((U136-G136)/G136*100,2)</f>
@@ -20026,11 +20026,11 @@
       </c>
       <c r="AL136">
         <f t="shared" ref="AL136:AL137" si="103">ROUND((W136-I136)/I136*100,2)</f>
-        <v>19.48</v>
+        <v>19.95</v>
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>6.05</v>
+        <v>6.58</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20038,7 +20038,7 @@
       </c>
       <c r="AO136">
         <f t="shared" ref="AO136:AO137" si="106">ROUND((Z136-L136)/L136*100,2)</f>
-        <v>17.28</v>
+        <v>17.53</v>
       </c>
       <c r="AP136">
         <f t="shared" ref="AP136:AP137" si="107">ROUND((AA136-M136)/M136*100,2)</f>
@@ -20104,28 +20104,28 @@
         <v>213</v>
       </c>
       <c r="T137">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="U137">
         <v>380</v>
       </c>
       <c r="V137">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="W137">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="X137">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="Y137">
         <v>65</v>
       </c>
       <c r="Z137">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AA137">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="AC137">
         <v>2022</v>
@@ -20151,7 +20151,7 @@
       </c>
       <c r="AI137">
         <f t="shared" si="100"/>
-        <v>-13.33</v>
+        <v>-11.11</v>
       </c>
       <c r="AJ137">
         <f t="shared" si="101"/>
@@ -20159,15 +20159,15 @@
       </c>
       <c r="AK137">
         <f t="shared" si="102"/>
-        <v>7.65</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>6.6</v>
+        <v>6.84</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>9.3000000000000007</v>
+        <v>9.48</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
@@ -20175,11 +20175,11 @@
       </c>
       <c r="AO137">
         <f t="shared" si="106"/>
-        <v>9.3800000000000008</v>
+        <v>9.6300000000000008</v>
       </c>
       <c r="AP137">
         <f t="shared" si="107"/>
-        <v>1.4</v>
+        <v>1.87</v>
       </c>
     </row>
     <row r="138" spans="1:42" x14ac:dyDescent="0.25">
@@ -20250,13 +20250,13 @@
         <v>175</v>
       </c>
       <c r="W138">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="X138">
-        <v>590</v>
+        <v>592</v>
       </c>
       <c r="Y138">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Z138">
         <v>446</v>
@@ -20300,15 +20300,15 @@
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>4.47</v>
+        <v>4.9400000000000004</v>
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>6.31</v>
+        <v>6.67</v>
       </c>
       <c r="AN138">
         <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
-        <v>13.04</v>
+        <v>14.49</v>
       </c>
       <c r="AO138">
         <f t="shared" ref="AO138:AO139" si="118">ROUND((Z138-L138)/L138*100,2)</f>
@@ -20381,25 +20381,25 @@
         <v>55</v>
       </c>
       <c r="U139">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="V139">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="W139">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="X139">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="Y139">
         <v>70</v>
       </c>
       <c r="Z139">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="AA139">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AC139">
         <v>2022</v>
@@ -20429,19 +20429,19 @@
       </c>
       <c r="AJ139">
         <f t="shared" si="113"/>
-        <v>13.47</v>
+        <v>14.07</v>
       </c>
       <c r="AK139">
         <f t="shared" si="114"/>
-        <v>14.84</v>
+        <v>15.38</v>
       </c>
       <c r="AL139">
         <f t="shared" si="115"/>
-        <v>17.489999999999998</v>
+        <v>18.2</v>
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>8.89</v>
+        <v>9.44</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20449,11 +20449,11 @@
       </c>
       <c r="AO139">
         <f t="shared" si="118"/>
-        <v>18</v>
+        <v>18.5</v>
       </c>
       <c r="AP139">
         <f t="shared" si="119"/>
-        <v>-4.25</v>
+        <v>-3.3</v>
       </c>
     </row>
     <row r="140" spans="1:42" x14ac:dyDescent="0.25">
@@ -20509,7 +20509,7 @@
         <v>137</v>
       </c>
       <c r="R140">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="S140">
         <v>219</v>
@@ -20518,22 +20518,22 @@
         <v>40</v>
       </c>
       <c r="U140">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="V140">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="W140">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="X140">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="Y140">
         <v>84</v>
       </c>
       <c r="Z140">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="AA140">
         <v>230</v>
@@ -20554,7 +20554,7 @@
       </c>
       <c r="AG140">
         <f t="shared" ref="AG140:AG141" si="122">ROUND((R140-D140)/D140*100,2)</f>
-        <v>13.68</v>
+        <v>14.74</v>
       </c>
       <c r="AH140">
         <f t="shared" ref="AH140:AH141" si="123">ROUND((S140-E140)/E140*100,2)</f>
@@ -20566,19 +20566,19 @@
       </c>
       <c r="AJ140">
         <f t="shared" ref="AJ140:AJ141" si="125">ROUND((U140-G140)/G140*100,2)</f>
-        <v>7.9</v>
+        <v>8.51</v>
       </c>
       <c r="AK140">
         <f t="shared" ref="AK140:AK141" si="126">ROUND((V140-H140)/H140*100,2)</f>
-        <v>13.81</v>
+        <v>14.36</v>
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>3.32</v>
+        <v>4.5</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
-        <v>7.07</v>
+        <v>7.61</v>
       </c>
       <c r="AN140">
         <f t="shared" ref="AN140:AN141" si="129">ROUND((Y140-K140)/K140*100,2)</f>
@@ -20586,7 +20586,7 @@
       </c>
       <c r="AO140">
         <f t="shared" ref="AO140:AO141" si="130">ROUND((Z140-L140)/L140*100,2)</f>
-        <v>21.8</v>
+        <v>22.31</v>
       </c>
       <c r="AP140">
         <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
@@ -20655,22 +20655,22 @@
         <v>50</v>
       </c>
       <c r="U141">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="V141">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="W141">
-        <v>391</v>
+        <v>407</v>
       </c>
       <c r="X141">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="Y141">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Z141">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="AA141">
         <v>238</v>
@@ -20703,27 +20703,27 @@
       </c>
       <c r="AJ141">
         <f t="shared" si="125"/>
-        <v>16.57</v>
+        <v>18.37</v>
       </c>
       <c r="AK141">
         <f t="shared" si="126"/>
-        <v>3.31</v>
+        <v>3.87</v>
       </c>
       <c r="AL141">
         <f t="shared" si="127"/>
-        <v>-7.78</v>
+        <v>-4.01</v>
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>6.72</v>
+        <v>7.99</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
-        <v>1.43</v>
+        <v>2.86</v>
       </c>
       <c r="AO141">
         <f t="shared" si="130"/>
-        <v>17.16</v>
+        <v>18.41</v>
       </c>
       <c r="AP141">
         <f t="shared" si="131"/>
@@ -20777,40 +20777,40 @@
         <v>36</v>
       </c>
       <c r="P142">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="Q142">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="R142">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="S142">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="T142">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="U142">
         <v>368</v>
       </c>
       <c r="V142">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="W142">
-        <v>484</v>
+        <v>451</v>
       </c>
       <c r="X142">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="Y142">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="Z142">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="AA142">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="AC142">
         <v>2022</v>
@@ -20819,52 +20819,52 @@
         <v>36</v>
       </c>
       <c r="AE142">
-        <f t="shared" ref="AE142" si="132">ROUND((P142-B142)/B142*100,2)</f>
-        <v>26.53</v>
+        <f t="shared" ref="AE142:AE143" si="132">ROUND((P142-B142)/B142*100,2)</f>
+        <v>24.49</v>
       </c>
       <c r="AF142">
-        <f t="shared" ref="AF142" si="133">ROUND((Q142-C142)/C142*100,2)</f>
-        <v>1.77</v>
+        <f t="shared" ref="AF142:AF143" si="133">ROUND((Q142-C142)/C142*100,2)</f>
+        <v>7.96</v>
       </c>
       <c r="AG142">
-        <f t="shared" ref="AG142" si="134">ROUND((R142-D142)/D142*100,2)</f>
-        <v>-6.32</v>
+        <f t="shared" ref="AG142:AG143" si="134">ROUND((R142-D142)/D142*100,2)</f>
+        <v>-4.21</v>
       </c>
       <c r="AH142">
-        <f t="shared" ref="AH142" si="135">ROUND((S142-E142)/E142*100,2)</f>
-        <v>4.79</v>
+        <f t="shared" ref="AH142:AH143" si="135">ROUND((S142-E142)/E142*100,2)</f>
+        <v>6.91</v>
       </c>
       <c r="AI142">
-        <f t="shared" ref="AI142" si="136">ROUND((T142-F142)/F142*100,2)</f>
-        <v>9.3000000000000007</v>
+        <f t="shared" ref="AI142:AI143" si="136">ROUND((T142-F142)/F142*100,2)</f>
+        <v>2.33</v>
       </c>
       <c r="AJ142">
-        <f t="shared" ref="AJ142" si="137">ROUND((U142-G142)/G142*100,2)</f>
+        <f t="shared" ref="AJ142:AJ143" si="137">ROUND((U142-G142)/G142*100,2)</f>
         <v>10.18</v>
       </c>
       <c r="AK142">
-        <f t="shared" ref="AK142" si="138">ROUND((V142-H142)/H142*100,2)</f>
-        <v>1.67</v>
+        <f t="shared" ref="AK142:AK143" si="138">ROUND((V142-H142)/H142*100,2)</f>
+        <v>3.33</v>
       </c>
       <c r="AL142">
-        <f t="shared" ref="AL142" si="139">ROUND((W142-I142)/I142*100,2)</f>
-        <v>14.15</v>
+        <f t="shared" ref="AL142:AL143" si="139">ROUND((W142-I142)/I142*100,2)</f>
+        <v>6.37</v>
       </c>
       <c r="AM142">
-        <f t="shared" ref="AM142" si="140">ROUND((X142-J142)/J142*100,2)</f>
-        <v>7.03</v>
+        <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
+        <v>6.67</v>
       </c>
       <c r="AN142">
-        <f t="shared" ref="AN142" si="141">ROUND((Y142-K142)/K142*100,2)</f>
-        <v>4.29</v>
+        <f t="shared" ref="AN142:AN143" si="141">ROUND((Y142-K142)/K142*100,2)</f>
+        <v>12.86</v>
       </c>
       <c r="AO142">
-        <f t="shared" ref="AO142" si="142">ROUND((Z142-L142)/L142*100,2)</f>
-        <v>9.68</v>
+        <f t="shared" ref="AO142:AO143" si="142">ROUND((Z142-L142)/L142*100,2)</f>
+        <v>11.41</v>
       </c>
       <c r="AP142">
-        <f t="shared" ref="AP142" si="143">ROUND((AA142-M142)/M142*100,2)</f>
-        <v>3.29</v>
+        <f t="shared" ref="AP142:AP143" si="143">ROUND((AA142-M142)/M142*100,2)</f>
+        <v>-1.88</v>
       </c>
     </row>
     <row r="143" spans="1:42" x14ac:dyDescent="0.25">
@@ -20907,6 +20907,102 @@
       <c r="M143">
         <v>216</v>
       </c>
+      <c r="N143">
+        <v>2022</v>
+      </c>
+      <c r="O143">
+        <v>37</v>
+      </c>
+      <c r="P143">
+        <v>110</v>
+      </c>
+      <c r="Q143">
+        <v>109</v>
+      </c>
+      <c r="R143">
+        <v>85</v>
+      </c>
+      <c r="S143">
+        <v>191</v>
+      </c>
+      <c r="T143">
+        <v>46</v>
+      </c>
+      <c r="U143">
+        <v>368</v>
+      </c>
+      <c r="V143">
+        <v>169</v>
+      </c>
+      <c r="W143">
+        <v>399</v>
+      </c>
+      <c r="X143">
+        <v>596</v>
+      </c>
+      <c r="Y143">
+        <v>60</v>
+      </c>
+      <c r="Z143">
+        <v>417</v>
+      </c>
+      <c r="AA143">
+        <v>221</v>
+      </c>
+      <c r="AC143">
+        <v>2022</v>
+      </c>
+      <c r="AD143">
+        <v>37</v>
+      </c>
+      <c r="AE143">
+        <f t="shared" si="132"/>
+        <v>10</v>
+      </c>
+      <c r="AF143">
+        <f t="shared" si="133"/>
+        <v>-3.54</v>
+      </c>
+      <c r="AG143">
+        <f t="shared" si="134"/>
+        <v>-11.46</v>
+      </c>
+      <c r="AH143">
+        <f t="shared" si="135"/>
+        <v>1.06</v>
+      </c>
+      <c r="AI143">
+        <f t="shared" si="136"/>
+        <v>6.98</v>
+      </c>
+      <c r="AJ143">
+        <f t="shared" si="137"/>
+        <v>9.52</v>
+      </c>
+      <c r="AK143">
+        <f t="shared" si="138"/>
+        <v>-7.65</v>
+      </c>
+      <c r="AL143">
+        <f t="shared" si="139"/>
+        <v>-6.34</v>
+      </c>
+      <c r="AM143">
+        <f t="shared" si="140"/>
+        <v>6.81</v>
+      </c>
+      <c r="AN143">
+        <f t="shared" si="141"/>
+        <v>-15.49</v>
+      </c>
+      <c r="AO143">
+        <f t="shared" si="142"/>
+        <v>2.71</v>
+      </c>
+      <c r="AP143">
+        <f t="shared" si="143"/>
+        <v>2.31</v>
+      </c>
     </row>
     <row r="144" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
@@ -20947,6 +21043,102 @@
       </c>
       <c r="M144">
         <v>218</v>
+      </c>
+      <c r="N144">
+        <v>2022</v>
+      </c>
+      <c r="O144">
+        <v>38</v>
+      </c>
+      <c r="P144">
+        <v>101</v>
+      </c>
+      <c r="Q144">
+        <v>140</v>
+      </c>
+      <c r="R144">
+        <v>109</v>
+      </c>
+      <c r="S144">
+        <v>196</v>
+      </c>
+      <c r="T144">
+        <v>46</v>
+      </c>
+      <c r="U144">
+        <v>362</v>
+      </c>
+      <c r="V144">
+        <v>213</v>
+      </c>
+      <c r="W144">
+        <v>487</v>
+      </c>
+      <c r="X144">
+        <v>575</v>
+      </c>
+      <c r="Y144">
+        <v>69</v>
+      </c>
+      <c r="Z144">
+        <v>423</v>
+      </c>
+      <c r="AA144">
+        <v>221</v>
+      </c>
+      <c r="AC144">
+        <v>2022</v>
+      </c>
+      <c r="AD144">
+        <v>38</v>
+      </c>
+      <c r="AE144">
+        <f t="shared" ref="AE144" si="144">ROUND((P144-B144)/B144*100,2)</f>
+        <v>-0.98</v>
+      </c>
+      <c r="AF144">
+        <f t="shared" ref="AF144" si="145">ROUND((Q144-C144)/C144*100,2)</f>
+        <v>20.69</v>
+      </c>
+      <c r="AG144">
+        <f t="shared" ref="AG144" si="146">ROUND((R144-D144)/D144*100,2)</f>
+        <v>13.54</v>
+      </c>
+      <c r="AH144">
+        <f t="shared" ref="AH144" si="147">ROUND((S144-E144)/E144*100,2)</f>
+        <v>2.62</v>
+      </c>
+      <c r="AI144">
+        <f t="shared" ref="AI144" si="148">ROUND((T144-F144)/F144*100,2)</f>
+        <v>4.55</v>
+      </c>
+      <c r="AJ144">
+        <f t="shared" ref="AJ144" si="149">ROUND((U144-G144)/G144*100,2)</f>
+        <v>6.78</v>
+      </c>
+      <c r="AK144">
+        <f t="shared" ref="AK144" si="150">ROUND((V144-H144)/H144*100,2)</f>
+        <v>14.52</v>
+      </c>
+      <c r="AL144">
+        <f t="shared" ref="AL144" si="151">ROUND((W144-I144)/I144*100,2)</f>
+        <v>12.73</v>
+      </c>
+      <c r="AM144">
+        <f t="shared" ref="AM144" si="152">ROUND((X144-J144)/J144*100,2)</f>
+        <v>2.31</v>
+      </c>
+      <c r="AN144">
+        <f t="shared" ref="AN144" si="153">ROUND((Y144-K144)/K144*100,2)</f>
+        <v>-2.82</v>
+      </c>
+      <c r="AO144">
+        <f t="shared" ref="AO144" si="154">ROUND((Z144-L144)/L144*100,2)</f>
+        <v>2.17</v>
+      </c>
+      <c r="AP144">
+        <f t="shared" ref="AP144" si="155">ROUND((AA144-M144)/M144*100,2)</f>
+        <v>1.38</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update excess mortality scripts in line with rtweet update
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF256FE6-5530-46A5-ADB2-F21C76DC23C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C51CD1-3FF4-487B-92C2-9643DAB94244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1420,7 +1420,7 @@
   <dimension ref="A1:AP158"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA154" sqref="AA154"/>
+      <selection activeCell="AE138" sqref="AE138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17230,7 +17230,7 @@
         <v>44</v>
       </c>
       <c r="U116">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="V116">
         <v>210</v>
@@ -17278,7 +17278,7 @@
       </c>
       <c r="AJ116">
         <f t="shared" si="29"/>
-        <v>-7.91</v>
+        <v>-7.67</v>
       </c>
       <c r="AK116">
         <f t="shared" si="30"/>
@@ -18466,7 +18466,7 @@
         <v>414</v>
       </c>
       <c r="V125">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="W125">
         <v>515</v>
@@ -18515,7 +18515,7 @@
       </c>
       <c r="AK125">
         <f t="shared" ref="AK125:AK126" si="66">ROUND((V125-H125)/H125*100,2)</f>
-        <v>8.33</v>
+        <v>8.85</v>
       </c>
       <c r="AL125">
         <f t="shared" ref="AL125:AL126" si="67">ROUND((W125-I125)/I125*100,2)</f>
@@ -19154,7 +19154,7 @@
         <v>222</v>
       </c>
       <c r="W130">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="X130">
         <v>610</v>
@@ -19204,7 +19204,7 @@
       </c>
       <c r="AL130">
         <f t="shared" si="79"/>
-        <v>4.1900000000000004</v>
+        <v>4.42</v>
       </c>
       <c r="AM130">
         <f t="shared" si="80"/>
@@ -19696,7 +19696,7 @@
         <v>52</v>
       </c>
       <c r="U134">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="V134">
         <v>217</v>
@@ -19744,7 +19744,7 @@
       </c>
       <c r="AJ134">
         <f t="shared" si="89"/>
-        <v>10.09</v>
+        <v>10.39</v>
       </c>
       <c r="AK134">
         <f t="shared" si="90"/>
@@ -19842,7 +19842,7 @@
         <v>509</v>
       </c>
       <c r="X135">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="Y135">
         <v>97</v>
@@ -19893,7 +19893,7 @@
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>13.73</v>
+        <v>13.9</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
@@ -20113,16 +20113,16 @@
         <v>198</v>
       </c>
       <c r="W137">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="X137">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="Y137">
         <v>65</v>
       </c>
       <c r="Z137">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AA137">
         <v>218</v>
@@ -20163,11 +20163,11 @@
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>7.08</v>
+        <v>7.31</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>9.48</v>
+        <v>9.84</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
@@ -20175,7 +20175,7 @@
       </c>
       <c r="AO137">
         <f t="shared" si="106"/>
-        <v>9.8800000000000008</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="AP137">
         <f t="shared" si="107"/>
@@ -20253,7 +20253,7 @@
         <v>446</v>
       </c>
       <c r="X138">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="Y138">
         <v>79</v>
@@ -20304,7 +20304,7 @@
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>6.85</v>
+        <v>7.39</v>
       </c>
       <c r="AN138">
         <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
@@ -20390,7 +20390,7 @@
         <v>501</v>
       </c>
       <c r="X139">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="Y139">
         <v>70</v>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>9.26</v>
+        <v>9.6199999999999992</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20524,7 +20524,7 @@
         <v>207</v>
       </c>
       <c r="W140">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="X140">
         <v>594</v>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>4.74</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
@@ -20661,16 +20661,16 @@
         <v>188</v>
       </c>
       <c r="W141">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="X141">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="Y141">
         <v>72</v>
       </c>
       <c r="Z141">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AA141">
         <v>238</v>
@@ -20711,11 +20711,11 @@
       </c>
       <c r="AL141">
         <f t="shared" si="127"/>
-        <v>-3.54</v>
+        <v>-2.83</v>
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>7.99</v>
+        <v>8.35</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
@@ -20723,7 +20723,7 @@
       </c>
       <c r="AO141">
         <f t="shared" si="130"/>
-        <v>18.41</v>
+        <v>18.66</v>
       </c>
       <c r="AP141">
         <f t="shared" si="131"/>
@@ -20792,13 +20792,13 @@
         <v>44</v>
       </c>
       <c r="U142">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="V142">
         <v>186</v>
       </c>
       <c r="W142">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="X142">
         <v>593</v>
@@ -20840,7 +20840,7 @@
       </c>
       <c r="AJ142">
         <f t="shared" ref="AJ142:AJ143" si="137">ROUND((U142-G142)/G142*100,2)</f>
-        <v>10.48</v>
+        <v>10.78</v>
       </c>
       <c r="AK142">
         <f t="shared" ref="AK142:AK143" si="138">ROUND((V142-H142)/H142*100,2)</f>
@@ -20848,7 +20848,7 @@
       </c>
       <c r="AL142">
         <f t="shared" ref="AL142:AL143" si="139">ROUND((W142-I142)/I142*100,2)</f>
-        <v>6.84</v>
+        <v>7.08</v>
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
@@ -20917,28 +20917,28 @@
         <v>110</v>
       </c>
       <c r="Q143">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="R143">
         <v>86</v>
       </c>
       <c r="S143">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="T143">
         <v>46</v>
       </c>
       <c r="U143">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="V143">
         <v>169</v>
       </c>
       <c r="W143">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="X143">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="Y143">
         <v>60</v>
@@ -20947,7 +20947,7 @@
         <v>417</v>
       </c>
       <c r="AA143">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="AC143">
         <v>2022</v>
@@ -20961,7 +20961,7 @@
       </c>
       <c r="AF143">
         <f t="shared" si="133"/>
-        <v>-3.54</v>
+        <v>-2.65</v>
       </c>
       <c r="AG143">
         <f t="shared" si="134"/>
@@ -20969,7 +20969,7 @@
       </c>
       <c r="AH143">
         <f t="shared" si="135"/>
-        <v>1.59</v>
+        <v>2.12</v>
       </c>
       <c r="AI143">
         <f t="shared" si="136"/>
@@ -20977,7 +20977,7 @@
       </c>
       <c r="AJ143">
         <f t="shared" si="137"/>
-        <v>10.71</v>
+        <v>11.31</v>
       </c>
       <c r="AK143">
         <f t="shared" si="138"/>
@@ -20985,11 +20985,11 @@
       </c>
       <c r="AL143">
         <f t="shared" si="139"/>
-        <v>-5.16</v>
+        <v>-4.93</v>
       </c>
       <c r="AM143">
         <f t="shared" si="140"/>
-        <v>7.35</v>
+        <v>7.71</v>
       </c>
       <c r="AN143">
         <f t="shared" si="141"/>
@@ -21001,7 +21001,7 @@
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
-        <v>2.31</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="144" spans="1:42" x14ac:dyDescent="0.25">
@@ -21060,31 +21060,31 @@
         <v>108</v>
       </c>
       <c r="S144">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="T144">
         <v>42</v>
       </c>
       <c r="U144">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="V144">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="W144">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="X144">
-        <v>596</v>
+        <v>602</v>
       </c>
       <c r="Y144">
         <v>75</v>
       </c>
       <c r="Z144">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AA144">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="AC144">
         <v>2022</v>
@@ -21106,7 +21106,7 @@
       </c>
       <c r="AH144">
         <f t="shared" ref="AH144:AH145" si="147">ROUND((S144-E144)/E144*100,2)</f>
-        <v>6.81</v>
+        <v>7.33</v>
       </c>
       <c r="AI144">
         <f t="shared" ref="AI144:AI145" si="148">ROUND((T144-F144)/F144*100,2)</f>
@@ -21114,19 +21114,19 @@
       </c>
       <c r="AJ144">
         <f t="shared" ref="AJ144:AJ145" si="149">ROUND((U144-G144)/G144*100,2)</f>
-        <v>10.32</v>
+        <v>10.91</v>
       </c>
       <c r="AK144">
         <f t="shared" ref="AK144:AK145" si="150">ROUND((V144-H144)/H144*100,2)</f>
-        <v>21.51</v>
+        <v>22.04</v>
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
-        <v>10.42</v>
+        <v>10.88</v>
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
-        <v>6.05</v>
+        <v>7.12</v>
       </c>
       <c r="AN144">
         <f t="shared" ref="AN144:AN145" si="153">ROUND((Y144-K144)/K144*100,2)</f>
@@ -21134,11 +21134,11 @@
       </c>
       <c r="AO144">
         <f t="shared" ref="AO144:AO145" si="154">ROUND((Z144-L144)/L144*100,2)</f>
-        <v>2.17</v>
+        <v>2.42</v>
       </c>
       <c r="AP144">
         <f t="shared" ref="AP144:AP145" si="155">ROUND((AA144-M144)/M144*100,2)</f>
-        <v>-0.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:42" x14ac:dyDescent="0.25">
@@ -21188,37 +21188,37 @@
         <v>39</v>
       </c>
       <c r="P145">
+        <v>120</v>
+      </c>
+      <c r="Q145">
         <v>122</v>
       </c>
-      <c r="Q145">
-        <v>129</v>
-      </c>
       <c r="R145">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="S145">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="T145">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="U145">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="V145">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="W145">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="X145">
-        <v>602</v>
+        <v>648</v>
       </c>
       <c r="Y145">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="Z145">
-        <v>421</v>
+        <v>429</v>
       </c>
       <c r="AA145">
         <v>248</v>
@@ -21231,47 +21231,47 @@
       </c>
       <c r="AE145">
         <f t="shared" si="144"/>
-        <v>19.61</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="AF145">
         <f t="shared" si="145"/>
-        <v>10.26</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="AG145">
         <f t="shared" si="146"/>
-        <v>25</v>
+        <v>23.96</v>
       </c>
       <c r="AH145">
         <f t="shared" si="147"/>
-        <v>16.670000000000002</v>
+        <v>16.149999999999999</v>
       </c>
       <c r="AI145">
         <f t="shared" si="148"/>
-        <v>-13.33</v>
+        <v>-24.44</v>
       </c>
       <c r="AJ145">
         <f t="shared" si="149"/>
-        <v>26.47</v>
+        <v>27.94</v>
       </c>
       <c r="AK145">
         <f t="shared" si="150"/>
-        <v>19.350000000000001</v>
+        <v>24.19</v>
       </c>
       <c r="AL145">
         <f t="shared" si="151"/>
-        <v>4.6100000000000003</v>
+        <v>8.76</v>
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>5.24</v>
+        <v>13.29</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
-        <v>9.59</v>
+        <v>2.74</v>
       </c>
       <c r="AO145">
         <f t="shared" si="154"/>
-        <v>0.72</v>
+        <v>2.63</v>
       </c>
       <c r="AP145">
         <f t="shared" si="155"/>
@@ -21317,6 +21317,102 @@
       </c>
       <c r="M146">
         <v>222</v>
+      </c>
+      <c r="N146">
+        <v>2022</v>
+      </c>
+      <c r="O146">
+        <v>40</v>
+      </c>
+      <c r="P146">
+        <v>134</v>
+      </c>
+      <c r="Q146">
+        <v>131</v>
+      </c>
+      <c r="R146">
+        <v>104</v>
+      </c>
+      <c r="S146">
+        <v>247</v>
+      </c>
+      <c r="T146">
+        <v>47</v>
+      </c>
+      <c r="U146">
+        <v>454</v>
+      </c>
+      <c r="V146">
+        <v>198</v>
+      </c>
+      <c r="W146">
+        <v>456</v>
+      </c>
+      <c r="X146">
+        <v>611</v>
+      </c>
+      <c r="Y146">
+        <v>81</v>
+      </c>
+      <c r="Z146">
+        <v>474</v>
+      </c>
+      <c r="AA146">
+        <v>226</v>
+      </c>
+      <c r="AC146">
+        <v>2022</v>
+      </c>
+      <c r="AD146">
+        <v>40</v>
+      </c>
+      <c r="AE146">
+        <f t="shared" ref="AE146" si="156">ROUND((P146-B146)/B146*100,2)</f>
+        <v>28.85</v>
+      </c>
+      <c r="AF146">
+        <f t="shared" ref="AF146" si="157">ROUND((Q146-C146)/C146*100,2)</f>
+        <v>11.97</v>
+      </c>
+      <c r="AG146">
+        <f t="shared" ref="AG146" si="158">ROUND((R146-D146)/D146*100,2)</f>
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="AH146">
+        <f t="shared" ref="AH146" si="159">ROUND((S146-E146)/E146*100,2)</f>
+        <v>29.32</v>
+      </c>
+      <c r="AI146">
+        <f t="shared" ref="AI146" si="160">ROUND((T146-F146)/F146*100,2)</f>
+        <v>4.4400000000000004</v>
+      </c>
+      <c r="AJ146">
+        <f t="shared" ref="AJ146" si="161">ROUND((U146-G146)/G146*100,2)</f>
+        <v>31.98</v>
+      </c>
+      <c r="AK146">
+        <f t="shared" ref="AK146" si="162">ROUND((V146-H146)/H146*100,2)</f>
+        <v>3.66</v>
+      </c>
+      <c r="AL146">
+        <f t="shared" ref="AL146" si="163">ROUND((W146-I146)/I146*100,2)</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="AM146">
+        <f t="shared" ref="AM146" si="164">ROUND((X146-J146)/J146*100,2)</f>
+        <v>5.53</v>
+      </c>
+      <c r="AN146">
+        <f t="shared" ref="AN146" si="165">ROUND((Y146-K146)/K146*100,2)</f>
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="AO146">
+        <f t="shared" ref="AO146" si="166">ROUND((Z146-L146)/L146*100,2)</f>
+        <v>11.53</v>
+      </c>
+      <c r="AP146">
+        <f t="shared" ref="AP146" si="167">ROUND((AA146-M146)/M146*100,2)</f>
+        <v>1.8</v>
       </c>
     </row>
     <row r="147" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update excess mortality plots - Week 41 (2022)
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C51CD1-3FF4-487B-92C2-9643DAB94244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53CB49A-023F-44BA-87EA-29FC7483204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2085" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AE138" sqref="AE138"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AK146" sqref="AK146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17230,7 +17230,7 @@
         <v>44</v>
       </c>
       <c r="U116">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="V116">
         <v>210</v>
@@ -17278,7 +17278,7 @@
       </c>
       <c r="AJ116">
         <f t="shared" si="29"/>
-        <v>-7.67</v>
+        <v>-7.91</v>
       </c>
       <c r="AK116">
         <f t="shared" si="30"/>
@@ -18871,7 +18871,7 @@
         <v>210</v>
       </c>
       <c r="T128">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="U128">
         <v>354</v>
@@ -18918,7 +18918,7 @@
       </c>
       <c r="AI128">
         <f t="shared" si="76"/>
-        <v>28.57</v>
+        <v>30.95</v>
       </c>
       <c r="AJ128">
         <f t="shared" si="77"/>
@@ -19437,7 +19437,7 @@
         <v>68</v>
       </c>
       <c r="Z132">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AA132">
         <v>260</v>
@@ -19490,7 +19490,7 @@
       </c>
       <c r="AO132">
         <f t="shared" si="82"/>
-        <v>21.95</v>
+        <v>22.2</v>
       </c>
       <c r="AP132">
         <f t="shared" si="83"/>
@@ -19705,7 +19705,7 @@
         <v>509</v>
       </c>
       <c r="X134">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="Y134">
         <v>78</v>
@@ -19756,7 +19756,7 @@
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
-        <v>12.01</v>
+        <v>12.19</v>
       </c>
       <c r="AN134">
         <f t="shared" si="93"/>
@@ -19848,7 +19848,7 @@
         <v>97</v>
       </c>
       <c r="Z135">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AA135">
         <v>245</v>
@@ -19901,7 +19901,7 @@
       </c>
       <c r="AO135">
         <f t="shared" si="94"/>
-        <v>11.06</v>
+        <v>11.3</v>
       </c>
       <c r="AP135">
         <f t="shared" si="95"/>
@@ -19976,10 +19976,10 @@
         <v>194</v>
       </c>
       <c r="W136">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="X136">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="Y136">
         <v>59</v>
@@ -20026,11 +20026,11 @@
       </c>
       <c r="AL136">
         <f t="shared" ref="AL136:AL137" si="103">ROUND((W136-I136)/I136*100,2)</f>
-        <v>19.95</v>
+        <v>20.190000000000001</v>
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>6.58</v>
+        <v>6.76</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20104,7 +20104,7 @@
         <v>213</v>
       </c>
       <c r="T137">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="U137">
         <v>380</v>
@@ -20151,7 +20151,7 @@
       </c>
       <c r="AI137">
         <f t="shared" si="100"/>
-        <v>-11.11</v>
+        <v>-8.89</v>
       </c>
       <c r="AJ137">
         <f t="shared" si="101"/>
@@ -20259,7 +20259,7 @@
         <v>79</v>
       </c>
       <c r="Z138">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AA138">
         <v>229</v>
@@ -20312,7 +20312,7 @@
       </c>
       <c r="AO138">
         <f t="shared" ref="AO138:AO139" si="118">ROUND((Z138-L138)/L138*100,2)</f>
-        <v>11.19</v>
+        <v>11.44</v>
       </c>
       <c r="AP138">
         <f t="shared" ref="AP138:AP139" si="119">ROUND((AA138-M138)/M138*100,2)</f>
@@ -20381,7 +20381,7 @@
         <v>55</v>
       </c>
       <c r="U139">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="V139">
         <v>210</v>
@@ -20429,7 +20429,7 @@
       </c>
       <c r="AJ139">
         <f t="shared" si="113"/>
-        <v>14.07</v>
+        <v>14.37</v>
       </c>
       <c r="AK139">
         <f t="shared" si="114"/>
@@ -20649,7 +20649,7 @@
         <v>116</v>
       </c>
       <c r="S141">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="T141">
         <v>50</v>
@@ -20695,7 +20695,7 @@
       </c>
       <c r="AH141">
         <f t="shared" si="123"/>
-        <v>9.19</v>
+        <v>9.73</v>
       </c>
       <c r="AI141">
         <f t="shared" si="124"/>
@@ -20792,13 +20792,13 @@
         <v>44</v>
       </c>
       <c r="U142">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="V142">
         <v>186</v>
       </c>
       <c r="W142">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="X142">
         <v>593</v>
@@ -20807,7 +20807,7 @@
         <v>79</v>
       </c>
       <c r="Z142">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AA142">
         <v>209</v>
@@ -20840,7 +20840,7 @@
       </c>
       <c r="AJ142">
         <f t="shared" ref="AJ142:AJ143" si="137">ROUND((U142-G142)/G142*100,2)</f>
-        <v>10.78</v>
+        <v>11.38</v>
       </c>
       <c r="AK142">
         <f t="shared" ref="AK142:AK143" si="138">ROUND((V142-H142)/H142*100,2)</f>
@@ -20848,7 +20848,7 @@
       </c>
       <c r="AL142">
         <f t="shared" ref="AL142:AL143" si="139">ROUND((W142-I142)/I142*100,2)</f>
-        <v>7.08</v>
+        <v>7.31</v>
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
@@ -20860,7 +20860,7 @@
       </c>
       <c r="AO142">
         <f t="shared" ref="AO142:AO143" si="142">ROUND((Z142-L142)/L142*100,2)</f>
-        <v>11.66</v>
+        <v>11.91</v>
       </c>
       <c r="AP142">
         <f t="shared" ref="AP142:AP143" si="143">ROUND((AA142-M142)/M142*100,2)</f>
@@ -20938,13 +20938,13 @@
         <v>405</v>
       </c>
       <c r="X143">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="Y143">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z143">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="AA143">
         <v>223</v>
@@ -20989,15 +20989,15 @@
       </c>
       <c r="AM143">
         <f t="shared" si="140"/>
-        <v>7.71</v>
+        <v>8.06</v>
       </c>
       <c r="AN143">
         <f t="shared" si="141"/>
-        <v>-15.49</v>
+        <v>-14.08</v>
       </c>
       <c r="AO143">
         <f t="shared" si="142"/>
-        <v>2.71</v>
+        <v>2.96</v>
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
@@ -21054,13 +21054,13 @@
         <v>99</v>
       </c>
       <c r="Q144">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="R144">
         <v>108</v>
       </c>
       <c r="S144">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="T144">
         <v>42</v>
@@ -21072,19 +21072,19 @@
         <v>227</v>
       </c>
       <c r="W144">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="X144">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="Y144">
         <v>75</v>
       </c>
       <c r="Z144">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="AA144">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AC144">
         <v>2022</v>
@@ -21098,7 +21098,7 @@
       </c>
       <c r="AF144">
         <f t="shared" ref="AF144:AF145" si="145">ROUND((Q144-C144)/C144*100,2)</f>
-        <v>11.21</v>
+        <v>12.07</v>
       </c>
       <c r="AG144">
         <f t="shared" ref="AG144:AG145" si="146">ROUND((R144-D144)/D144*100,2)</f>
@@ -21106,7 +21106,7 @@
       </c>
       <c r="AH144">
         <f t="shared" ref="AH144:AH145" si="147">ROUND((S144-E144)/E144*100,2)</f>
-        <v>7.33</v>
+        <v>7.85</v>
       </c>
       <c r="AI144">
         <f t="shared" ref="AI144:AI145" si="148">ROUND((T144-F144)/F144*100,2)</f>
@@ -21122,11 +21122,11 @@
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
-        <v>10.88</v>
+        <v>11.81</v>
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
-        <v>7.12</v>
+        <v>7.47</v>
       </c>
       <c r="AN144">
         <f t="shared" ref="AN144:AN145" si="153">ROUND((Y144-K144)/K144*100,2)</f>
@@ -21134,11 +21134,11 @@
       </c>
       <c r="AO144">
         <f t="shared" ref="AO144:AO145" si="154">ROUND((Z144-L144)/L144*100,2)</f>
-        <v>2.42</v>
+        <v>2.9</v>
       </c>
       <c r="AP144">
         <f t="shared" ref="AP144:AP145" si="155">ROUND((AA144-M144)/M144*100,2)</f>
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="145" spans="1:42" x14ac:dyDescent="0.25">
@@ -21203,22 +21203,22 @@
         <v>34</v>
       </c>
       <c r="U145">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="V145">
         <v>231</v>
       </c>
       <c r="W145">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="X145">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="Y145">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z145">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AA145">
         <v>248</v>
@@ -21251,7 +21251,7 @@
       </c>
       <c r="AJ145">
         <f t="shared" si="149"/>
-        <v>27.94</v>
+        <v>28.24</v>
       </c>
       <c r="AK145">
         <f t="shared" si="150"/>
@@ -21259,19 +21259,19 @@
       </c>
       <c r="AL145">
         <f t="shared" si="151"/>
-        <v>8.76</v>
+        <v>10.14</v>
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>13.29</v>
+        <v>13.81</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
-        <v>2.74</v>
+        <v>4.1100000000000003</v>
       </c>
       <c r="AO145">
         <f t="shared" si="154"/>
-        <v>2.63</v>
+        <v>2.87</v>
       </c>
       <c r="AP145">
         <f t="shared" si="155"/>
@@ -21325,40 +21325,40 @@
         <v>40</v>
       </c>
       <c r="P146">
+        <v>128</v>
+      </c>
+      <c r="Q146">
         <v>134</v>
-      </c>
-      <c r="Q146">
-        <v>131</v>
       </c>
       <c r="R146">
         <v>104</v>
       </c>
       <c r="S146">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="T146">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="U146">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="V146">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="W146">
-        <v>456</v>
+        <v>490</v>
       </c>
       <c r="X146">
-        <v>611</v>
+        <v>647</v>
       </c>
       <c r="Y146">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="Z146">
-        <v>474</v>
+        <v>498</v>
       </c>
       <c r="AA146">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="AC146">
         <v>2022</v>
@@ -21367,52 +21367,52 @@
         <v>40</v>
       </c>
       <c r="AE146">
-        <f t="shared" ref="AE146" si="156">ROUND((P146-B146)/B146*100,2)</f>
-        <v>28.85</v>
+        <f t="shared" ref="AE146:AE147" si="156">ROUND((P146-B146)/B146*100,2)</f>
+        <v>23.08</v>
       </c>
       <c r="AF146">
-        <f t="shared" ref="AF146" si="157">ROUND((Q146-C146)/C146*100,2)</f>
-        <v>11.97</v>
+        <f t="shared" ref="AF146:AF147" si="157">ROUND((Q146-C146)/C146*100,2)</f>
+        <v>14.53</v>
       </c>
       <c r="AG146">
-        <f t="shared" ref="AG146" si="158">ROUND((R146-D146)/D146*100,2)</f>
+        <f t="shared" ref="AG146:AG147" si="158">ROUND((R146-D146)/D146*100,2)</f>
         <v>9.4700000000000006</v>
       </c>
       <c r="AH146">
-        <f t="shared" ref="AH146" si="159">ROUND((S146-E146)/E146*100,2)</f>
-        <v>29.32</v>
+        <f t="shared" ref="AH146:AH147" si="159">ROUND((S146-E146)/E146*100,2)</f>
+        <v>26.18</v>
       </c>
       <c r="AI146">
-        <f t="shared" ref="AI146" si="160">ROUND((T146-F146)/F146*100,2)</f>
-        <v>4.4400000000000004</v>
+        <f t="shared" ref="AI146:AI147" si="160">ROUND((T146-F146)/F146*100,2)</f>
+        <v>11.11</v>
       </c>
       <c r="AJ146">
-        <f t="shared" ref="AJ146" si="161">ROUND((U146-G146)/G146*100,2)</f>
-        <v>31.98</v>
+        <f t="shared" ref="AJ146:AJ147" si="161">ROUND((U146-G146)/G146*100,2)</f>
+        <v>29.36</v>
       </c>
       <c r="AK146">
-        <f t="shared" ref="AK146" si="162">ROUND((V146-H146)/H146*100,2)</f>
-        <v>3.66</v>
+        <f t="shared" ref="AK146:AK147" si="162">ROUND((V146-H146)/H146*100,2)</f>
+        <v>12.57</v>
       </c>
       <c r="AL146">
-        <f t="shared" ref="AL146" si="163">ROUND((W146-I146)/I146*100,2)</f>
-        <v>4.1100000000000003</v>
+        <f t="shared" ref="AL146:AL147" si="163">ROUND((W146-I146)/I146*100,2)</f>
+        <v>11.87</v>
       </c>
       <c r="AM146">
-        <f t="shared" ref="AM146" si="164">ROUND((X146-J146)/J146*100,2)</f>
-        <v>5.53</v>
+        <f t="shared" ref="AM146:AM147" si="164">ROUND((X146-J146)/J146*100,2)</f>
+        <v>11.74</v>
       </c>
       <c r="AN146">
-        <f t="shared" ref="AN146" si="165">ROUND((Y146-K146)/K146*100,2)</f>
-        <v>9.4600000000000009</v>
+        <f t="shared" ref="AN146:AN147" si="165">ROUND((Y146-K146)/K146*100,2)</f>
+        <v>14.86</v>
       </c>
       <c r="AO146">
-        <f t="shared" ref="AO146" si="166">ROUND((Z146-L146)/L146*100,2)</f>
-        <v>11.53</v>
+        <f t="shared" ref="AO146:AO147" si="166">ROUND((Z146-L146)/L146*100,2)</f>
+        <v>17.18</v>
       </c>
       <c r="AP146">
-        <f t="shared" ref="AP146" si="167">ROUND((AA146-M146)/M146*100,2)</f>
-        <v>1.8</v>
+        <f t="shared" ref="AP146:AP147" si="167">ROUND((AA146-M146)/M146*100,2)</f>
+        <v>-1.8</v>
       </c>
     </row>
     <row r="147" spans="1:42" x14ac:dyDescent="0.25">
@@ -21454,6 +21454,102 @@
       </c>
       <c r="M147">
         <v>224</v>
+      </c>
+      <c r="N147">
+        <v>2022</v>
+      </c>
+      <c r="O147">
+        <v>41</v>
+      </c>
+      <c r="P147">
+        <v>101</v>
+      </c>
+      <c r="Q147">
+        <v>121</v>
+      </c>
+      <c r="R147">
+        <v>107</v>
+      </c>
+      <c r="S147">
+        <v>238</v>
+      </c>
+      <c r="T147">
+        <v>56</v>
+      </c>
+      <c r="U147">
+        <v>464</v>
+      </c>
+      <c r="V147">
+        <v>218</v>
+      </c>
+      <c r="W147">
+        <v>501</v>
+      </c>
+      <c r="X147">
+        <v>672</v>
+      </c>
+      <c r="Y147">
+        <v>87</v>
+      </c>
+      <c r="Z147">
+        <v>470</v>
+      </c>
+      <c r="AA147">
+        <v>247</v>
+      </c>
+      <c r="AC147">
+        <v>2022</v>
+      </c>
+      <c r="AD147">
+        <v>41</v>
+      </c>
+      <c r="AE147">
+        <f t="shared" si="156"/>
+        <v>-3.81</v>
+      </c>
+      <c r="AF147">
+        <f t="shared" si="157"/>
+        <v>2.54</v>
+      </c>
+      <c r="AG147">
+        <f t="shared" si="158"/>
+        <v>13.83</v>
+      </c>
+      <c r="AH147">
+        <f t="shared" si="159"/>
+        <v>22.68</v>
+      </c>
+      <c r="AI147">
+        <f t="shared" si="160"/>
+        <v>19.149999999999999</v>
+      </c>
+      <c r="AJ147">
+        <f t="shared" si="161"/>
+        <v>32.950000000000003</v>
+      </c>
+      <c r="AK147">
+        <f t="shared" si="162"/>
+        <v>13.54</v>
+      </c>
+      <c r="AL147">
+        <f t="shared" si="163"/>
+        <v>14.12</v>
+      </c>
+      <c r="AM147">
+        <f t="shared" si="164"/>
+        <v>15.86</v>
+      </c>
+      <c r="AN147">
+        <f t="shared" si="165"/>
+        <v>16</v>
+      </c>
+      <c r="AO147">
+        <f t="shared" si="166"/>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="AP147">
+        <f t="shared" si="167"/>
+        <v>10.27</v>
       </c>
     </row>
     <row r="148" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update weekly excess mortality data and plots
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53CB49A-023F-44BA-87EA-29FC7483204C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83585A5-6FE5-4420-A29C-3179C4617B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2085" yWindow="1380" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1575" yWindow="555" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AK146" sqref="AK146"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AG141" sqref="AG141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17376,7 +17376,7 @@
         <v>516</v>
       </c>
       <c r="X117">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="Y117">
         <v>113</v>
@@ -17427,7 +17427,7 @@
       </c>
       <c r="AM117">
         <f t="shared" si="32"/>
-        <v>1.66</v>
+        <v>1.81</v>
       </c>
       <c r="AN117">
         <f t="shared" si="33"/>
@@ -17513,7 +17513,7 @@
         <v>530</v>
       </c>
       <c r="X118">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="Y118">
         <v>82</v>
@@ -17564,7 +17564,7 @@
       </c>
       <c r="AM118">
         <f t="shared" si="32"/>
-        <v>11.4</v>
+        <v>11.25</v>
       </c>
       <c r="AN118">
         <f t="shared" si="33"/>
@@ -17647,7 +17647,7 @@
         <v>237</v>
       </c>
       <c r="W119">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="X119">
         <v>723</v>
@@ -17697,7 +17697,7 @@
       </c>
       <c r="AL119">
         <f t="shared" si="31"/>
-        <v>19.66</v>
+        <v>19.87</v>
       </c>
       <c r="AM119">
         <f t="shared" si="32"/>
@@ -17933,7 +17933,7 @@
         <v>503</v>
       </c>
       <c r="AA121">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AC121">
         <v>2022</v>
@@ -17987,7 +17987,7 @@
       </c>
       <c r="AP121">
         <f t="shared" si="35"/>
-        <v>28.27</v>
+        <v>28.69</v>
       </c>
     </row>
     <row r="122" spans="1:42" x14ac:dyDescent="0.25">
@@ -19294,13 +19294,13 @@
         <v>444</v>
       </c>
       <c r="X131">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="Y131">
         <v>93</v>
       </c>
       <c r="Z131">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="AA131">
         <v>211</v>
@@ -19345,7 +19345,7 @@
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>26.57</v>
+        <v>26.93</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
@@ -19353,7 +19353,7 @@
       </c>
       <c r="AO131">
         <f t="shared" si="82"/>
-        <v>9.18</v>
+        <v>9.42</v>
       </c>
       <c r="AP131">
         <f t="shared" si="83"/>
@@ -19836,10 +19836,10 @@
         <v>403</v>
       </c>
       <c r="V135">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="W135">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="X135">
         <v>639</v>
@@ -19885,11 +19885,11 @@
       </c>
       <c r="AK135">
         <f t="shared" si="90"/>
-        <v>3.76</v>
+        <v>4.84</v>
       </c>
       <c r="AL135">
         <f t="shared" si="91"/>
-        <v>18.93</v>
+        <v>19.16</v>
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
@@ -19979,7 +19979,7 @@
         <v>512</v>
       </c>
       <c r="X136">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Y136">
         <v>59</v>
@@ -20030,7 +20030,7 @@
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>6.76</v>
+        <v>6.94</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20250,7 +20250,7 @@
         <v>175</v>
       </c>
       <c r="W138">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="X138">
         <v>596</v>
@@ -20300,7 +20300,7 @@
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>4.9400000000000004</v>
+        <v>5.18</v>
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
@@ -20387,10 +20387,10 @@
         <v>210</v>
       </c>
       <c r="W139">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="X139">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="Y139">
         <v>70</v>
@@ -20437,11 +20437,11 @@
       </c>
       <c r="AL139">
         <f t="shared" si="115"/>
-        <v>18.440000000000001</v>
+        <v>18.68</v>
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>9.6199999999999992</v>
+        <v>9.98</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20524,16 +20524,16 @@
         <v>207</v>
       </c>
       <c r="W140">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="X140">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Y140">
         <v>84</v>
       </c>
       <c r="Z140">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AA140">
         <v>230</v>
@@ -20574,11 +20574,11 @@
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>4.9800000000000004</v>
+        <v>5.21</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
-        <v>7.61</v>
+        <v>7.79</v>
       </c>
       <c r="AN140">
         <f t="shared" ref="AN140:AN141" si="129">ROUND((Y140-K140)/K140*100,2)</f>
@@ -20586,7 +20586,7 @@
       </c>
       <c r="AO140">
         <f t="shared" ref="AO140:AO141" si="130">ROUND((Z140-L140)/L140*100,2)</f>
-        <v>22.31</v>
+        <v>22.56</v>
       </c>
       <c r="AP140">
         <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
@@ -20655,7 +20655,7 @@
         <v>50</v>
       </c>
       <c r="U141">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="V141">
         <v>188</v>
@@ -20664,7 +20664,7 @@
         <v>412</v>
       </c>
       <c r="X141">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="Y141">
         <v>72</v>
@@ -20673,7 +20673,7 @@
         <v>477</v>
       </c>
       <c r="AA141">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AC141">
         <v>2022</v>
@@ -20703,7 +20703,7 @@
       </c>
       <c r="AJ141">
         <f t="shared" si="125"/>
-        <v>18.670000000000002</v>
+        <v>18.98</v>
       </c>
       <c r="AK141">
         <f t="shared" si="126"/>
@@ -20715,7 +20715,7 @@
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>8.35</v>
+        <v>8.7100000000000009</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
@@ -20727,7 +20727,7 @@
       </c>
       <c r="AP141">
         <f t="shared" si="131"/>
-        <v>12.8</v>
+        <v>13.27</v>
       </c>
     </row>
     <row r="142" spans="1:42" x14ac:dyDescent="0.25">
@@ -20798,7 +20798,7 @@
         <v>186</v>
       </c>
       <c r="W142">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="X142">
         <v>593</v>
@@ -20848,7 +20848,7 @@
       </c>
       <c r="AL142">
         <f t="shared" ref="AL142:AL143" si="139">ROUND((W142-I142)/I142*100,2)</f>
-        <v>7.31</v>
+        <v>7.78</v>
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
@@ -20938,7 +20938,7 @@
         <v>405</v>
       </c>
       <c r="X143">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="Y143">
         <v>61</v>
@@ -20947,7 +20947,7 @@
         <v>418</v>
       </c>
       <c r="AA143">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AC143">
         <v>2022</v>
@@ -20989,7 +20989,7 @@
       </c>
       <c r="AM143">
         <f t="shared" si="140"/>
-        <v>8.06</v>
+        <v>8.24</v>
       </c>
       <c r="AN143">
         <f t="shared" si="141"/>
@@ -21001,7 +21001,7 @@
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
-        <v>3.24</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="144" spans="1:42" x14ac:dyDescent="0.25">
@@ -21057,7 +21057,7 @@
         <v>130</v>
       </c>
       <c r="R144">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="S144">
         <v>206</v>
@@ -21066,16 +21066,16 @@
         <v>42</v>
       </c>
       <c r="U144">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="V144">
         <v>227</v>
       </c>
       <c r="W144">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="X144">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="Y144">
         <v>75</v>
@@ -21084,7 +21084,7 @@
         <v>426</v>
       </c>
       <c r="AA144">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AC144">
         <v>2022</v>
@@ -21102,7 +21102,7 @@
       </c>
       <c r="AG144">
         <f t="shared" ref="AG144:AG145" si="146">ROUND((R144-D144)/D144*100,2)</f>
-        <v>12.5</v>
+        <v>13.54</v>
       </c>
       <c r="AH144">
         <f t="shared" ref="AH144:AH145" si="147">ROUND((S144-E144)/E144*100,2)</f>
@@ -21114,7 +21114,7 @@
       </c>
       <c r="AJ144">
         <f t="shared" ref="AJ144:AJ145" si="149">ROUND((U144-G144)/G144*100,2)</f>
-        <v>10.91</v>
+        <v>11.21</v>
       </c>
       <c r="AK144">
         <f t="shared" ref="AK144:AK145" si="150">ROUND((V144-H144)/H144*100,2)</f>
@@ -21122,11 +21122,11 @@
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
-        <v>11.81</v>
+        <v>12.27</v>
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
-        <v>7.47</v>
+        <v>7.83</v>
       </c>
       <c r="AN144">
         <f t="shared" ref="AN144:AN145" si="153">ROUND((Y144-K144)/K144*100,2)</f>
@@ -21138,7 +21138,7 @@
       </c>
       <c r="AP144">
         <f t="shared" ref="AP144:AP145" si="155">ROUND((AA144-M144)/M144*100,2)</f>
-        <v>0.92</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="145" spans="1:42" x14ac:dyDescent="0.25">
@@ -21197,7 +21197,7 @@
         <v>119</v>
       </c>
       <c r="S145">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="T145">
         <v>34</v>
@@ -21209,10 +21209,10 @@
         <v>231</v>
       </c>
       <c r="W145">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="X145">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="Y145">
         <v>76</v>
@@ -21243,7 +21243,7 @@
       </c>
       <c r="AH145">
         <f t="shared" si="147"/>
-        <v>16.149999999999999</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="AI145">
         <f t="shared" si="148"/>
@@ -21259,11 +21259,11 @@
       </c>
       <c r="AL145">
         <f t="shared" si="151"/>
-        <v>10.14</v>
+        <v>10.6</v>
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>13.81</v>
+        <v>14.34</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
@@ -21325,7 +21325,7 @@
         <v>40</v>
       </c>
       <c r="P146">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="Q146">
         <v>134</v>
@@ -21334,31 +21334,31 @@
         <v>104</v>
       </c>
       <c r="S146">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="T146">
         <v>50</v>
       </c>
       <c r="U146">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="V146">
         <v>215</v>
       </c>
       <c r="W146">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="X146">
-        <v>647</v>
+        <v>658</v>
       </c>
       <c r="Y146">
         <v>85</v>
       </c>
       <c r="Z146">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="AA146">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AC146">
         <v>2022</v>
@@ -21368,7 +21368,7 @@
       </c>
       <c r="AE146">
         <f t="shared" ref="AE146:AE147" si="156">ROUND((P146-B146)/B146*100,2)</f>
-        <v>23.08</v>
+        <v>24.04</v>
       </c>
       <c r="AF146">
         <f t="shared" ref="AF146:AF147" si="157">ROUND((Q146-C146)/C146*100,2)</f>
@@ -21380,7 +21380,7 @@
       </c>
       <c r="AH146">
         <f t="shared" ref="AH146:AH147" si="159">ROUND((S146-E146)/E146*100,2)</f>
-        <v>26.18</v>
+        <v>27.75</v>
       </c>
       <c r="AI146">
         <f t="shared" ref="AI146:AI147" si="160">ROUND((T146-F146)/F146*100,2)</f>
@@ -21388,7 +21388,7 @@
       </c>
       <c r="AJ146">
         <f t="shared" ref="AJ146:AJ147" si="161">ROUND((U146-G146)/G146*100,2)</f>
-        <v>29.36</v>
+        <v>29.94</v>
       </c>
       <c r="AK146">
         <f t="shared" ref="AK146:AK147" si="162">ROUND((V146-H146)/H146*100,2)</f>
@@ -21396,11 +21396,11 @@
       </c>
       <c r="AL146">
         <f t="shared" ref="AL146:AL147" si="163">ROUND((W146-I146)/I146*100,2)</f>
-        <v>11.87</v>
+        <v>13.01</v>
       </c>
       <c r="AM146">
         <f t="shared" ref="AM146:AM147" si="164">ROUND((X146-J146)/J146*100,2)</f>
-        <v>11.74</v>
+        <v>13.64</v>
       </c>
       <c r="AN146">
         <f t="shared" ref="AN146:AN147" si="165">ROUND((Y146-K146)/K146*100,2)</f>
@@ -21408,11 +21408,11 @@
       </c>
       <c r="AO146">
         <f t="shared" ref="AO146:AO147" si="166">ROUND((Z146-L146)/L146*100,2)</f>
-        <v>17.18</v>
+        <v>17.649999999999999</v>
       </c>
       <c r="AP146">
         <f t="shared" ref="AP146:AP147" si="167">ROUND((AA146-M146)/M146*100,2)</f>
-        <v>-1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:42" x14ac:dyDescent="0.25">
@@ -21462,40 +21462,40 @@
         <v>41</v>
       </c>
       <c r="P147">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="Q147">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="R147">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S147">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="T147">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="U147">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="V147">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="W147">
-        <v>501</v>
+        <v>468</v>
       </c>
       <c r="X147">
-        <v>672</v>
+        <v>680</v>
       </c>
       <c r="Y147">
         <v>87</v>
       </c>
       <c r="Z147">
-        <v>470</v>
+        <v>480</v>
       </c>
       <c r="AA147">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="AC147">
         <v>2022</v>
@@ -21505,39 +21505,39 @@
       </c>
       <c r="AE147">
         <f t="shared" si="156"/>
-        <v>-3.81</v>
+        <v>0.95</v>
       </c>
       <c r="AF147">
         <f t="shared" si="157"/>
-        <v>2.54</v>
+        <v>5.08</v>
       </c>
       <c r="AG147">
         <f t="shared" si="158"/>
-        <v>13.83</v>
+        <v>12.77</v>
       </c>
       <c r="AH147">
         <f t="shared" si="159"/>
-        <v>22.68</v>
+        <v>19.07</v>
       </c>
       <c r="AI147">
         <f t="shared" si="160"/>
-        <v>19.149999999999999</v>
+        <v>4.26</v>
       </c>
       <c r="AJ147">
         <f t="shared" si="161"/>
-        <v>32.950000000000003</v>
+        <v>31.23</v>
       </c>
       <c r="AK147">
         <f t="shared" si="162"/>
-        <v>13.54</v>
+        <v>10.42</v>
       </c>
       <c r="AL147">
         <f t="shared" si="163"/>
-        <v>14.12</v>
+        <v>6.61</v>
       </c>
       <c r="AM147">
         <f t="shared" si="164"/>
-        <v>15.86</v>
+        <v>17.239999999999998</v>
       </c>
       <c r="AN147">
         <f t="shared" si="165"/>
@@ -21545,11 +21545,11 @@
       </c>
       <c r="AO147">
         <f t="shared" si="166"/>
-        <v>9.3000000000000007</v>
+        <v>11.63</v>
       </c>
       <c r="AP147">
         <f t="shared" si="167"/>
-        <v>10.27</v>
+        <v>13.84</v>
       </c>
     </row>
     <row r="148" spans="1:42" x14ac:dyDescent="0.25">
@@ -21591,6 +21591,102 @@
       </c>
       <c r="M148">
         <v>227</v>
+      </c>
+      <c r="N148">
+        <v>2022</v>
+      </c>
+      <c r="O148">
+        <v>42</v>
+      </c>
+      <c r="P148">
+        <v>116</v>
+      </c>
+      <c r="Q148">
+        <v>161</v>
+      </c>
+      <c r="R148">
+        <v>109</v>
+      </c>
+      <c r="S148">
+        <v>255</v>
+      </c>
+      <c r="T148">
+        <v>65</v>
+      </c>
+      <c r="U148">
+        <v>429</v>
+      </c>
+      <c r="V148">
+        <v>249</v>
+      </c>
+      <c r="W148">
+        <v>455</v>
+      </c>
+      <c r="X148">
+        <v>634</v>
+      </c>
+      <c r="Y148">
+        <v>79</v>
+      </c>
+      <c r="Z148">
+        <v>527</v>
+      </c>
+      <c r="AA148">
+        <v>240</v>
+      </c>
+      <c r="AC148">
+        <v>2022</v>
+      </c>
+      <c r="AD148">
+        <v>42</v>
+      </c>
+      <c r="AE148">
+        <f t="shared" ref="AE148" si="168">ROUND((P148-B148)/B148*100,2)</f>
+        <v>10.48</v>
+      </c>
+      <c r="AF148">
+        <f t="shared" ref="AF148" si="169">ROUND((Q148-C148)/C148*100,2)</f>
+        <v>31.97</v>
+      </c>
+      <c r="AG148">
+        <f t="shared" ref="AG148" si="170">ROUND((R148-D148)/D148*100,2)</f>
+        <v>14.74</v>
+      </c>
+      <c r="AH148">
+        <f t="shared" ref="AH148" si="171">ROUND((S148-E148)/E148*100,2)</f>
+        <v>30.1</v>
+      </c>
+      <c r="AI148">
+        <f t="shared" ref="AI148" si="172">ROUND((T148-F148)/F148*100,2)</f>
+        <v>38.299999999999997</v>
+      </c>
+      <c r="AJ148">
+        <f t="shared" ref="AJ148" si="173">ROUND((U148-G148)/G148*100,2)</f>
+        <v>21.88</v>
+      </c>
+      <c r="AK148">
+        <f t="shared" ref="AK148" si="174">ROUND((V148-H148)/H148*100,2)</f>
+        <v>27.69</v>
+      </c>
+      <c r="AL148">
+        <f t="shared" ref="AL148" si="175">ROUND((W148-I148)/I148*100,2)</f>
+        <v>3.17</v>
+      </c>
+      <c r="AM148">
+        <f t="shared" ref="AM148" si="176">ROUND((X148-J148)/J148*100,2)</f>
+        <v>7.28</v>
+      </c>
+      <c r="AN148">
+        <f t="shared" ref="AN148" si="177">ROUND((Y148-K148)/K148*100,2)</f>
+        <v>3.95</v>
+      </c>
+      <c r="AO148">
+        <f t="shared" ref="AO148" si="178">ROUND((Z148-L148)/L148*100,2)</f>
+        <v>21.99</v>
+      </c>
+      <c r="AP148">
+        <f t="shared" ref="AP148" si="179">ROUND((AA148-M148)/M148*100,2)</f>
+        <v>5.73</v>
       </c>
     </row>
     <row r="149" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excess mortality analyses - Week 44
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83585A5-6FE5-4420-A29C-3179C4617B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476C52E-253A-4FCF-9EB8-9F51542224A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="555" windowWidth="26715" windowHeight="14820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AG141" sqref="AG141"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH150" sqref="AH150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17650,7 +17650,7 @@
         <v>567</v>
       </c>
       <c r="X119">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="Y119">
         <v>97</v>
@@ -17701,7 +17701,7 @@
       </c>
       <c r="AM119">
         <f t="shared" si="32"/>
-        <v>14.22</v>
+        <v>14.38</v>
       </c>
       <c r="AN119">
         <f t="shared" si="33"/>
@@ -18609,7 +18609,7 @@
         <v>455</v>
       </c>
       <c r="X126">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="Y126">
         <v>66</v>
@@ -18660,7 +18660,7 @@
       </c>
       <c r="AM126">
         <f t="shared" si="68"/>
-        <v>0.35</v>
+        <v>0.53</v>
       </c>
       <c r="AN126">
         <f t="shared" si="69"/>
@@ -18743,7 +18743,7 @@
         <v>171</v>
       </c>
       <c r="W127">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="X127">
         <v>590</v>
@@ -18793,7 +18793,7 @@
       </c>
       <c r="AL127">
         <f t="shared" ref="AL127:AL132" si="79">ROUND((W127-I127)/I127*100,2)</f>
-        <v>-0.92</v>
+        <v>-0.69</v>
       </c>
       <c r="AM127">
         <f t="shared" ref="AM127:AM132" si="80">ROUND((X127-J127)/J127*100,2)</f>
@@ -19422,7 +19422,7 @@
         <v>52</v>
       </c>
       <c r="U132">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="V132">
         <v>194</v>
@@ -19470,7 +19470,7 @@
       </c>
       <c r="AJ132">
         <f t="shared" si="77"/>
-        <v>10.68</v>
+        <v>10.98</v>
       </c>
       <c r="AK132">
         <f t="shared" si="78"/>
@@ -19577,7 +19577,7 @@
         <v>446</v>
       </c>
       <c r="AA133">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AC133">
         <v>2022</v>
@@ -19631,7 +19631,7 @@
       </c>
       <c r="AP133">
         <f t="shared" ref="AP133:AP135" si="95">ROUND((AA133-M133)/M133*100,2)</f>
-        <v>-4.1500000000000004</v>
+        <v>-3.69</v>
       </c>
     </row>
     <row r="134" spans="1:42" x14ac:dyDescent="0.25">
@@ -19827,7 +19827,7 @@
         <v>128</v>
       </c>
       <c r="S135">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="T135">
         <v>59</v>
@@ -19842,7 +19842,7 @@
         <v>510</v>
       </c>
       <c r="X135">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="Y135">
         <v>97</v>
@@ -19873,7 +19873,7 @@
       </c>
       <c r="AH135">
         <f t="shared" si="87"/>
-        <v>11.35</v>
+        <v>11.89</v>
       </c>
       <c r="AI135">
         <f t="shared" si="88"/>
@@ -19893,7 +19893,7 @@
       </c>
       <c r="AM135">
         <f t="shared" si="92"/>
-        <v>13.9</v>
+        <v>14.08</v>
       </c>
       <c r="AN135">
         <f t="shared" si="93"/>
@@ -19979,7 +19979,7 @@
         <v>512</v>
       </c>
       <c r="X136">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Y136">
         <v>59</v>
@@ -20030,7 +20030,7 @@
       </c>
       <c r="AM136">
         <f t="shared" ref="AM136:AM137" si="104">ROUND((X136-J136)/J136*100,2)</f>
-        <v>6.94</v>
+        <v>7.12</v>
       </c>
       <c r="AN136">
         <f t="shared" ref="AN136:AN137" si="105">ROUND((Y136-K136)/K136*100,2)</f>
@@ -20238,22 +20238,22 @@
         <v>119</v>
       </c>
       <c r="S138">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="T138">
         <v>50</v>
       </c>
       <c r="U138">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="V138">
         <v>175</v>
       </c>
       <c r="W138">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="X138">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="Y138">
         <v>79</v>
@@ -20284,7 +20284,7 @@
       </c>
       <c r="AH138">
         <f t="shared" ref="AH138:AH139" si="111">ROUND((S138-E138)/E138*100,2)</f>
-        <v>15.3</v>
+        <v>15.85</v>
       </c>
       <c r="AI138">
         <f t="shared" ref="AI138:AI139" si="112">ROUND((T138-F138)/F138*100,2)</f>
@@ -20292,7 +20292,7 @@
       </c>
       <c r="AJ138">
         <f t="shared" ref="AJ138:AJ139" si="113">ROUND((U138-G138)/G138*100,2)</f>
-        <v>17.96</v>
+        <v>18.260000000000002</v>
       </c>
       <c r="AK138">
         <f t="shared" ref="AK138:AK139" si="114">ROUND((V138-H138)/H138*100,2)</f>
@@ -20300,11 +20300,11 @@
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>5.18</v>
+        <v>5.41</v>
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
-        <v>7.39</v>
+        <v>7.75</v>
       </c>
       <c r="AN138">
         <f t="shared" ref="AN138:AN139" si="117">ROUND((Y138-K138)/K138*100,2)</f>
@@ -20384,13 +20384,13 @@
         <v>382</v>
       </c>
       <c r="V139">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="W139">
         <v>502</v>
       </c>
       <c r="X139">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="Y139">
         <v>70</v>
@@ -20399,7 +20399,7 @@
         <v>474</v>
       </c>
       <c r="AA139">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AC139">
         <v>2022</v>
@@ -20433,7 +20433,7 @@
       </c>
       <c r="AK139">
         <f t="shared" si="114"/>
-        <v>15.38</v>
+        <v>15.93</v>
       </c>
       <c r="AL139">
         <f t="shared" si="115"/>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>9.98</v>
+        <v>10.34</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20453,7 +20453,7 @@
       </c>
       <c r="AP139">
         <f t="shared" si="119"/>
-        <v>-3.3</v>
+        <v>-2.83</v>
       </c>
     </row>
     <row r="140" spans="1:42" x14ac:dyDescent="0.25">
@@ -20527,7 +20527,7 @@
         <v>444</v>
       </c>
       <c r="X140">
-        <v>595</v>
+        <v>597</v>
       </c>
       <c r="Y140">
         <v>84</v>
@@ -20578,7 +20578,7 @@
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
-        <v>7.79</v>
+        <v>8.15</v>
       </c>
       <c r="AN140">
         <f t="shared" ref="AN140:AN141" si="129">ROUND((Y140-K140)/K140*100,2)</f>
@@ -20655,7 +20655,7 @@
         <v>50</v>
       </c>
       <c r="U141">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="V141">
         <v>188</v>
@@ -20703,7 +20703,7 @@
       </c>
       <c r="AJ141">
         <f t="shared" si="125"/>
-        <v>18.98</v>
+        <v>19.28</v>
       </c>
       <c r="AK141">
         <f t="shared" si="126"/>
@@ -20801,7 +20801,7 @@
         <v>457</v>
       </c>
       <c r="X142">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="Y142">
         <v>79</v>
@@ -20852,7 +20852,7 @@
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
-        <v>6.85</v>
+        <v>7.03</v>
       </c>
       <c r="AN142">
         <f t="shared" ref="AN142:AN143" si="141">ROUND((Y142-K142)/K142*100,2)</f>
@@ -20914,7 +20914,7 @@
         <v>37</v>
       </c>
       <c r="P143">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q143">
         <v>110</v>
@@ -20932,13 +20932,13 @@
         <v>374</v>
       </c>
       <c r="V143">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="W143">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="X143">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="Y143">
         <v>61</v>
@@ -20947,7 +20947,7 @@
         <v>418</v>
       </c>
       <c r="AA143">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AC143">
         <v>2022</v>
@@ -20957,7 +20957,7 @@
       </c>
       <c r="AE143">
         <f t="shared" si="132"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF143">
         <f t="shared" si="133"/>
@@ -20981,15 +20981,15 @@
       </c>
       <c r="AK143">
         <f t="shared" si="138"/>
-        <v>-7.65</v>
+        <v>-7.1</v>
       </c>
       <c r="AL143">
         <f t="shared" si="139"/>
-        <v>-4.93</v>
+        <v>-4.6900000000000004</v>
       </c>
       <c r="AM143">
         <f t="shared" si="140"/>
-        <v>8.24</v>
+        <v>8.42</v>
       </c>
       <c r="AN143">
         <f t="shared" si="141"/>
@@ -21001,7 +21001,7 @@
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
-        <v>3.7</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="144" spans="1:42" x14ac:dyDescent="0.25">
@@ -21072,7 +21072,7 @@
         <v>227</v>
       </c>
       <c r="W144">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="X144">
         <v>606</v>
@@ -21081,7 +21081,7 @@
         <v>75</v>
       </c>
       <c r="Z144">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AA144">
         <v>221</v>
@@ -21122,7 +21122,7 @@
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
-        <v>12.27</v>
+        <v>12.73</v>
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
@@ -21134,7 +21134,7 @@
       </c>
       <c r="AO144">
         <f t="shared" ref="AO144:AO145" si="154">ROUND((Z144-L144)/L144*100,2)</f>
-        <v>2.9</v>
+        <v>3.14</v>
       </c>
       <c r="AP144">
         <f t="shared" ref="AP144:AP145" si="155">ROUND((AA144-M144)/M144*100,2)</f>
@@ -21209,13 +21209,13 @@
         <v>231</v>
       </c>
       <c r="W145">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="X145">
-        <v>654</v>
+        <v>660</v>
       </c>
       <c r="Y145">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="Z145">
         <v>430</v>
@@ -21259,15 +21259,15 @@
       </c>
       <c r="AL145">
         <f t="shared" si="151"/>
-        <v>10.6</v>
+        <v>11.75</v>
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>14.34</v>
+        <v>15.38</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
-        <v>4.1100000000000003</v>
+        <v>5.48</v>
       </c>
       <c r="AO145">
         <f t="shared" si="154"/>
@@ -21334,7 +21334,7 @@
         <v>104</v>
       </c>
       <c r="S146">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="T146">
         <v>50</v>
@@ -21343,13 +21343,13 @@
         <v>447</v>
       </c>
       <c r="V146">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="W146">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="X146">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="Y146">
         <v>85</v>
@@ -21358,7 +21358,7 @@
         <v>500</v>
       </c>
       <c r="AA146">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AC146">
         <v>2022</v>
@@ -21380,7 +21380,7 @@
       </c>
       <c r="AH146">
         <f t="shared" ref="AH146:AH147" si="159">ROUND((S146-E146)/E146*100,2)</f>
-        <v>27.75</v>
+        <v>28.8</v>
       </c>
       <c r="AI146">
         <f t="shared" ref="AI146:AI147" si="160">ROUND((T146-F146)/F146*100,2)</f>
@@ -21392,15 +21392,15 @@
       </c>
       <c r="AK146">
         <f t="shared" ref="AK146:AK147" si="162">ROUND((V146-H146)/H146*100,2)</f>
-        <v>12.57</v>
+        <v>13.61</v>
       </c>
       <c r="AL146">
         <f t="shared" ref="AL146:AL147" si="163">ROUND((W146-I146)/I146*100,2)</f>
-        <v>13.01</v>
+        <v>14.16</v>
       </c>
       <c r="AM146">
         <f t="shared" ref="AM146:AM147" si="164">ROUND((X146-J146)/J146*100,2)</f>
-        <v>13.64</v>
+        <v>14.34</v>
       </c>
       <c r="AN146">
         <f t="shared" ref="AN146:AN147" si="165">ROUND((Y146-K146)/K146*100,2)</f>
@@ -21412,7 +21412,7 @@
       </c>
       <c r="AP146">
         <f t="shared" ref="AP146:AP147" si="167">ROUND((AA146-M146)/M146*100,2)</f>
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="147" spans="1:42" x14ac:dyDescent="0.25">
@@ -21471,31 +21471,31 @@
         <v>106</v>
       </c>
       <c r="S147">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="T147">
         <v>49</v>
       </c>
       <c r="U147">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="V147">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="W147">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="X147">
-        <v>680</v>
+        <v>689</v>
       </c>
       <c r="Y147">
         <v>87</v>
       </c>
       <c r="Z147">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="AA147">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AC147">
         <v>2022</v>
@@ -21517,7 +21517,7 @@
       </c>
       <c r="AH147">
         <f t="shared" si="159"/>
-        <v>19.07</v>
+        <v>19.59</v>
       </c>
       <c r="AI147">
         <f t="shared" si="160"/>
@@ -21525,19 +21525,19 @@
       </c>
       <c r="AJ147">
         <f t="shared" si="161"/>
-        <v>31.23</v>
+        <v>31.52</v>
       </c>
       <c r="AK147">
         <f t="shared" si="162"/>
-        <v>10.42</v>
+        <v>11.98</v>
       </c>
       <c r="AL147">
         <f t="shared" si="163"/>
-        <v>6.61</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="AM147">
         <f t="shared" si="164"/>
-        <v>17.239999999999998</v>
+        <v>18.79</v>
       </c>
       <c r="AN147">
         <f t="shared" si="165"/>
@@ -21545,11 +21545,11 @@
       </c>
       <c r="AO147">
         <f t="shared" si="166"/>
-        <v>11.63</v>
+        <v>12.56</v>
       </c>
       <c r="AP147">
         <f t="shared" si="167"/>
-        <v>13.84</v>
+        <v>14.73</v>
       </c>
     </row>
     <row r="148" spans="1:42" x14ac:dyDescent="0.25">
@@ -21599,40 +21599,40 @@
         <v>42</v>
       </c>
       <c r="P148">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="Q148">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="R148">
         <v>109</v>
       </c>
       <c r="S148">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="T148">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U148">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="V148">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="W148">
-        <v>455</v>
+        <v>496</v>
       </c>
       <c r="X148">
-        <v>634</v>
+        <v>657</v>
       </c>
       <c r="Y148">
         <v>79</v>
       </c>
       <c r="Z148">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="AA148">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="AC148">
         <v>2022</v>
@@ -21641,52 +21641,52 @@
         <v>42</v>
       </c>
       <c r="AE148">
-        <f t="shared" ref="AE148" si="168">ROUND((P148-B148)/B148*100,2)</f>
-        <v>10.48</v>
+        <f t="shared" ref="AE148:AE149" si="168">ROUND((P148-B148)/B148*100,2)</f>
+        <v>13.33</v>
       </c>
       <c r="AF148">
-        <f t="shared" ref="AF148" si="169">ROUND((Q148-C148)/C148*100,2)</f>
-        <v>31.97</v>
+        <f t="shared" ref="AF148:AF149" si="169">ROUND((Q148-C148)/C148*100,2)</f>
+        <v>22.95</v>
       </c>
       <c r="AG148">
-        <f t="shared" ref="AG148" si="170">ROUND((R148-D148)/D148*100,2)</f>
+        <f t="shared" ref="AG148:AG149" si="170">ROUND((R148-D148)/D148*100,2)</f>
         <v>14.74</v>
       </c>
       <c r="AH148">
-        <f t="shared" ref="AH148" si="171">ROUND((S148-E148)/E148*100,2)</f>
-        <v>30.1</v>
+        <f t="shared" ref="AH148:AH149" si="171">ROUND((S148-E148)/E148*100,2)</f>
+        <v>28.06</v>
       </c>
       <c r="AI148">
-        <f t="shared" ref="AI148" si="172">ROUND((T148-F148)/F148*100,2)</f>
-        <v>38.299999999999997</v>
+        <f t="shared" ref="AI148:AI149" si="172">ROUND((T148-F148)/F148*100,2)</f>
+        <v>34.04</v>
       </c>
       <c r="AJ148">
-        <f t="shared" ref="AJ148" si="173">ROUND((U148-G148)/G148*100,2)</f>
-        <v>21.88</v>
+        <f t="shared" ref="AJ148:AJ149" si="173">ROUND((U148-G148)/G148*100,2)</f>
+        <v>19.03</v>
       </c>
       <c r="AK148">
-        <f t="shared" ref="AK148" si="174">ROUND((V148-H148)/H148*100,2)</f>
-        <v>27.69</v>
+        <f t="shared" ref="AK148:AK149" si="174">ROUND((V148-H148)/H148*100,2)</f>
+        <v>21.54</v>
       </c>
       <c r="AL148">
-        <f t="shared" ref="AL148" si="175">ROUND((W148-I148)/I148*100,2)</f>
-        <v>3.17</v>
+        <f t="shared" ref="AL148:AL149" si="175">ROUND((W148-I148)/I148*100,2)</f>
+        <v>12.47</v>
       </c>
       <c r="AM148">
-        <f t="shared" ref="AM148" si="176">ROUND((X148-J148)/J148*100,2)</f>
-        <v>7.28</v>
+        <f t="shared" ref="AM148:AM149" si="176">ROUND((X148-J148)/J148*100,2)</f>
+        <v>11.17</v>
       </c>
       <c r="AN148">
-        <f t="shared" ref="AN148" si="177">ROUND((Y148-K148)/K148*100,2)</f>
+        <f t="shared" ref="AN148:AN149" si="177">ROUND((Y148-K148)/K148*100,2)</f>
         <v>3.95</v>
       </c>
       <c r="AO148">
-        <f t="shared" ref="AO148" si="178">ROUND((Z148-L148)/L148*100,2)</f>
-        <v>21.99</v>
+        <f t="shared" ref="AO148:AO149" si="178">ROUND((Z148-L148)/L148*100,2)</f>
+        <v>23.61</v>
       </c>
       <c r="AP148">
-        <f t="shared" ref="AP148" si="179">ROUND((AA148-M148)/M148*100,2)</f>
-        <v>5.73</v>
+        <f t="shared" ref="AP148:AP149" si="179">ROUND((AA148-M148)/M148*100,2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:42" x14ac:dyDescent="0.25">
@@ -21729,6 +21729,102 @@
       <c r="M149">
         <v>227</v>
       </c>
+      <c r="N149">
+        <v>2022</v>
+      </c>
+      <c r="O149">
+        <v>43</v>
+      </c>
+      <c r="P149">
+        <v>112</v>
+      </c>
+      <c r="Q149">
+        <v>135</v>
+      </c>
+      <c r="R149">
+        <v>141</v>
+      </c>
+      <c r="S149">
+        <v>224</v>
+      </c>
+      <c r="T149">
+        <v>41</v>
+      </c>
+      <c r="U149">
+        <v>443</v>
+      </c>
+      <c r="V149">
+        <v>214</v>
+      </c>
+      <c r="W149">
+        <v>510</v>
+      </c>
+      <c r="X149">
+        <v>636</v>
+      </c>
+      <c r="Y149">
+        <v>79</v>
+      </c>
+      <c r="Z149">
+        <v>497</v>
+      </c>
+      <c r="AA149">
+        <v>248</v>
+      </c>
+      <c r="AC149">
+        <v>2022</v>
+      </c>
+      <c r="AD149">
+        <v>43</v>
+      </c>
+      <c r="AE149">
+        <f t="shared" si="168"/>
+        <v>4.67</v>
+      </c>
+      <c r="AF149">
+        <f t="shared" si="169"/>
+        <v>9.76</v>
+      </c>
+      <c r="AG149">
+        <f t="shared" si="170"/>
+        <v>45.36</v>
+      </c>
+      <c r="AH149">
+        <f t="shared" si="171"/>
+        <v>14.29</v>
+      </c>
+      <c r="AI149">
+        <f t="shared" si="172"/>
+        <v>-14.58</v>
+      </c>
+      <c r="AJ149">
+        <f t="shared" si="173"/>
+        <v>25.85</v>
+      </c>
+      <c r="AK149">
+        <f t="shared" si="174"/>
+        <v>9.18</v>
+      </c>
+      <c r="AL149">
+        <f t="shared" si="175"/>
+        <v>14.61</v>
+      </c>
+      <c r="AM149">
+        <f t="shared" si="176"/>
+        <v>6.89</v>
+      </c>
+      <c r="AN149">
+        <f t="shared" si="177"/>
+        <v>1.28</v>
+      </c>
+      <c r="AO149">
+        <f t="shared" si="178"/>
+        <v>12.95</v>
+      </c>
+      <c r="AP149">
+        <f t="shared" si="179"/>
+        <v>9.25</v>
+      </c>
     </row>
     <row r="150" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
@@ -21769,6 +21865,102 @@
       </c>
       <c r="M150">
         <v>229</v>
+      </c>
+      <c r="N150">
+        <v>2022</v>
+      </c>
+      <c r="O150">
+        <v>44</v>
+      </c>
+      <c r="P150">
+        <v>108</v>
+      </c>
+      <c r="Q150">
+        <v>143</v>
+      </c>
+      <c r="R150">
+        <v>132</v>
+      </c>
+      <c r="S150">
+        <v>230</v>
+      </c>
+      <c r="T150">
+        <v>64</v>
+      </c>
+      <c r="U150">
+        <v>392</v>
+      </c>
+      <c r="V150">
+        <v>221</v>
+      </c>
+      <c r="W150">
+        <v>488</v>
+      </c>
+      <c r="X150">
+        <v>695</v>
+      </c>
+      <c r="Y150">
+        <v>89</v>
+      </c>
+      <c r="Z150">
+        <v>459</v>
+      </c>
+      <c r="AA150">
+        <v>222</v>
+      </c>
+      <c r="AC150">
+        <v>2022</v>
+      </c>
+      <c r="AD150">
+        <v>44</v>
+      </c>
+      <c r="AE150">
+        <f t="shared" ref="AE150" si="180">ROUND((P150-B150)/B150*100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="AF150">
+        <f t="shared" ref="AF150" si="181">ROUND((Q150-C150)/C150*100,2)</f>
+        <v>16.260000000000002</v>
+      </c>
+      <c r="AG150">
+        <f t="shared" ref="AG150" si="182">ROUND((R150-D150)/D150*100,2)</f>
+        <v>34.69</v>
+      </c>
+      <c r="AH150">
+        <f t="shared" ref="AH150" si="183">ROUND((S150-E150)/E150*100,2)</f>
+        <v>16.75</v>
+      </c>
+      <c r="AI150">
+        <f t="shared" ref="AI150" si="184">ROUND((T150-F150)/F150*100,2)</f>
+        <v>33.33</v>
+      </c>
+      <c r="AJ150">
+        <f t="shared" ref="AJ150" si="185">ROUND((U150-G150)/G150*100,2)</f>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="AK150">
+        <f t="shared" ref="AK150" si="186">ROUND((V150-H150)/H150*100,2)</f>
+        <v>12.76</v>
+      </c>
+      <c r="AL150">
+        <f t="shared" ref="AL150" si="187">ROUND((W150-I150)/I150*100,2)</f>
+        <v>8.93</v>
+      </c>
+      <c r="AM150">
+        <f t="shared" ref="AM150" si="188">ROUND((X150-J150)/J150*100,2)</f>
+        <v>15.83</v>
+      </c>
+      <c r="AN150">
+        <f t="shared" ref="AN150" si="189">ROUND((Y150-K150)/K150*100,2)</f>
+        <v>14.1</v>
+      </c>
+      <c r="AO150">
+        <f t="shared" ref="AO150" si="190">ROUND((Z150-L150)/L150*100,2)</f>
+        <v>2.68</v>
+      </c>
+      <c r="AP150">
+        <f t="shared" ref="AP150" si="191">ROUND((AA150-M150)/M150*100,2)</f>
+        <v>-3.06</v>
       </c>
     </row>
     <row r="151" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update excess mortality plots
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C476C52E-253A-4FCF-9EB8-9F51542224A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2579D23-100B-4FA6-9100-A00C61E117FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="excess_mortality_provinces" sheetId="1" r:id="rId1"/>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH150" sqref="AH150"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AJ120" sqref="AJ120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18463,7 +18463,7 @@
         <v>54</v>
       </c>
       <c r="U125">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="V125">
         <v>209</v>
@@ -18511,7 +18511,7 @@
       </c>
       <c r="AJ125">
         <f t="shared" ref="AJ125:AJ126" si="65">ROUND((U125-G125)/G125*100,2)</f>
-        <v>15.97</v>
+        <v>16.25</v>
       </c>
       <c r="AK125">
         <f t="shared" ref="AK125:AK126" si="66">ROUND((V125-H125)/H125*100,2)</f>
@@ -19142,7 +19142,7 @@
         <v>118</v>
       </c>
       <c r="S130">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="T130">
         <v>44</v>
@@ -19188,7 +19188,7 @@
       </c>
       <c r="AH130">
         <f t="shared" si="75"/>
-        <v>6.28</v>
+        <v>6.81</v>
       </c>
       <c r="AI130">
         <f t="shared" si="76"/>
@@ -19428,7 +19428,7 @@
         <v>194</v>
       </c>
       <c r="W132">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="X132">
         <v>573</v>
@@ -19478,7 +19478,7 @@
       </c>
       <c r="AL132">
         <f t="shared" si="79"/>
-        <v>12.41</v>
+        <v>12.65</v>
       </c>
       <c r="AM132">
         <f t="shared" si="80"/>
@@ -20366,7 +20366,7 @@
         <v>33</v>
       </c>
       <c r="P139">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="Q139">
         <v>124</v>
@@ -20409,7 +20409,7 @@
       </c>
       <c r="AE139">
         <f t="shared" si="108"/>
-        <v>17.350000000000001</v>
+        <v>18.37</v>
       </c>
       <c r="AF139">
         <f t="shared" si="109"/>
@@ -20536,7 +20536,7 @@
         <v>489</v>
       </c>
       <c r="AA140">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AC140">
         <v>2022</v>
@@ -20590,7 +20590,7 @@
       </c>
       <c r="AP140">
         <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
-        <v>8.49</v>
+        <v>8.9600000000000009</v>
       </c>
     </row>
     <row r="141" spans="1:42" x14ac:dyDescent="0.25">
@@ -20661,7 +20661,7 @@
         <v>188</v>
       </c>
       <c r="W141">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="X141">
         <v>599</v>
@@ -20711,7 +20711,7 @@
       </c>
       <c r="AL141">
         <f t="shared" si="127"/>
-        <v>-2.83</v>
+        <v>-2.59</v>
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
@@ -20777,7 +20777,7 @@
         <v>36</v>
       </c>
       <c r="P142">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q142">
         <v>122</v>
@@ -20801,13 +20801,13 @@
         <v>457</v>
       </c>
       <c r="X142">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Y142">
         <v>79</v>
       </c>
       <c r="Z142">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="AA142">
         <v>209</v>
@@ -20820,7 +20820,7 @@
       </c>
       <c r="AE142">
         <f t="shared" ref="AE142:AE143" si="132">ROUND((P142-B142)/B142*100,2)</f>
-        <v>24.49</v>
+        <v>25.51</v>
       </c>
       <c r="AF142">
         <f t="shared" ref="AF142:AF143" si="133">ROUND((Q142-C142)/C142*100,2)</f>
@@ -20852,7 +20852,7 @@
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
-        <v>7.03</v>
+        <v>7.21</v>
       </c>
       <c r="AN142">
         <f t="shared" ref="AN142:AN143" si="141">ROUND((Y142-K142)/K142*100,2)</f>
@@ -20860,7 +20860,7 @@
       </c>
       <c r="AO142">
         <f t="shared" ref="AO142:AO143" si="142">ROUND((Z142-L142)/L142*100,2)</f>
-        <v>11.91</v>
+        <v>12.16</v>
       </c>
       <c r="AP142">
         <f t="shared" ref="AP142:AP143" si="143">ROUND((AA142-M142)/M142*100,2)</f>
@@ -20938,7 +20938,7 @@
         <v>406</v>
       </c>
       <c r="X143">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="Y143">
         <v>61</v>
@@ -20989,7 +20989,7 @@
       </c>
       <c r="AM143">
         <f t="shared" si="140"/>
-        <v>8.42</v>
+        <v>8.7799999999999994</v>
       </c>
       <c r="AN143">
         <f t="shared" si="141"/>
@@ -21072,10 +21072,10 @@
         <v>227</v>
       </c>
       <c r="W144">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="X144">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Y144">
         <v>75</v>
@@ -21122,11 +21122,11 @@
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
-        <v>12.73</v>
+        <v>13.19</v>
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
-        <v>7.83</v>
+        <v>8.01</v>
       </c>
       <c r="AN144">
         <f t="shared" ref="AN144:AN145" si="153">ROUND((Y144-K144)/K144*100,2)</f>
@@ -21194,7 +21194,7 @@
         <v>122</v>
       </c>
       <c r="R145">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="S145">
         <v>224</v>
@@ -21218,7 +21218,7 @@
         <v>77</v>
       </c>
       <c r="Z145">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="AA145">
         <v>248</v>
@@ -21239,7 +21239,7 @@
       </c>
       <c r="AG145">
         <f t="shared" si="146"/>
-        <v>23.96</v>
+        <v>25</v>
       </c>
       <c r="AH145">
         <f t="shared" si="147"/>
@@ -21271,7 +21271,7 @@
       </c>
       <c r="AO145">
         <f t="shared" si="154"/>
-        <v>2.87</v>
+        <v>3.35</v>
       </c>
       <c r="AP145">
         <f t="shared" si="155"/>
@@ -21337,7 +21337,7 @@
         <v>246</v>
       </c>
       <c r="T146">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U146">
         <v>447</v>
@@ -21346,10 +21346,10 @@
         <v>217</v>
       </c>
       <c r="W146">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="X146">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="Y146">
         <v>85</v>
@@ -21384,7 +21384,7 @@
       </c>
       <c r="AI146">
         <f t="shared" ref="AI146:AI147" si="160">ROUND((T146-F146)/F146*100,2)</f>
-        <v>11.11</v>
+        <v>13.33</v>
       </c>
       <c r="AJ146">
         <f t="shared" ref="AJ146:AJ147" si="161">ROUND((U146-G146)/G146*100,2)</f>
@@ -21396,11 +21396,11 @@
       </c>
       <c r="AL146">
         <f t="shared" ref="AL146:AL147" si="163">ROUND((W146-I146)/I146*100,2)</f>
-        <v>14.16</v>
+        <v>14.38</v>
       </c>
       <c r="AM146">
         <f t="shared" ref="AM146:AM147" si="164">ROUND((X146-J146)/J146*100,2)</f>
-        <v>14.34</v>
+        <v>14.51</v>
       </c>
       <c r="AN146">
         <f t="shared" ref="AN146:AN147" si="165">ROUND((Y146-K146)/K146*100,2)</f>
@@ -21474,25 +21474,25 @@
         <v>232</v>
       </c>
       <c r="T147">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="U147">
         <v>459</v>
       </c>
       <c r="V147">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="W147">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="X147">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="Y147">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Z147">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="AA147">
         <v>257</v>
@@ -21521,7 +21521,7 @@
       </c>
       <c r="AI147">
         <f t="shared" si="160"/>
-        <v>4.26</v>
+        <v>6.38</v>
       </c>
       <c r="AJ147">
         <f t="shared" si="161"/>
@@ -21529,23 +21529,23 @@
       </c>
       <c r="AK147">
         <f t="shared" si="162"/>
-        <v>11.98</v>
+        <v>13.02</v>
       </c>
       <c r="AL147">
         <f t="shared" si="163"/>
-        <v>8.1999999999999993</v>
+        <v>8.43</v>
       </c>
       <c r="AM147">
         <f t="shared" si="164"/>
-        <v>18.79</v>
+        <v>18.97</v>
       </c>
       <c r="AN147">
         <f t="shared" si="165"/>
-        <v>16</v>
+        <v>17.329999999999998</v>
       </c>
       <c r="AO147">
         <f t="shared" si="166"/>
-        <v>12.56</v>
+        <v>13.02</v>
       </c>
       <c r="AP147">
         <f t="shared" si="167"/>
@@ -21608,7 +21608,7 @@
         <v>109</v>
       </c>
       <c r="S148">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="T148">
         <v>63</v>
@@ -21620,10 +21620,10 @@
         <v>237</v>
       </c>
       <c r="W148">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="X148">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="Y148">
         <v>79</v>
@@ -21632,7 +21632,7 @@
         <v>534</v>
       </c>
       <c r="AA148">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AC148">
         <v>2022</v>
@@ -21654,7 +21654,7 @@
       </c>
       <c r="AH148">
         <f t="shared" ref="AH148:AH149" si="171">ROUND((S148-E148)/E148*100,2)</f>
-        <v>28.06</v>
+        <v>28.57</v>
       </c>
       <c r="AI148">
         <f t="shared" ref="AI148:AI149" si="172">ROUND((T148-F148)/F148*100,2)</f>
@@ -21670,11 +21670,11 @@
       </c>
       <c r="AL148">
         <f t="shared" ref="AL148:AL149" si="175">ROUND((W148-I148)/I148*100,2)</f>
-        <v>12.47</v>
+        <v>13.15</v>
       </c>
       <c r="AM148">
         <f t="shared" ref="AM148:AM149" si="176">ROUND((X148-J148)/J148*100,2)</f>
-        <v>11.17</v>
+        <v>11.51</v>
       </c>
       <c r="AN148">
         <f t="shared" ref="AN148:AN149" si="177">ROUND((Y148-K148)/K148*100,2)</f>
@@ -21686,7 +21686,7 @@
       </c>
       <c r="AP148">
         <f t="shared" ref="AP148:AP149" si="179">ROUND((AA148-M148)/M148*100,2)</f>
-        <v>0</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="149" spans="1:42" x14ac:dyDescent="0.25">
@@ -21751,16 +21751,16 @@
         <v>41</v>
       </c>
       <c r="U149">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="V149">
         <v>214</v>
       </c>
       <c r="W149">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="X149">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="Y149">
         <v>79</v>
@@ -21769,7 +21769,7 @@
         <v>497</v>
       </c>
       <c r="AA149">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AC149">
         <v>2022</v>
@@ -21799,7 +21799,7 @@
       </c>
       <c r="AJ149">
         <f t="shared" si="173"/>
-        <v>25.85</v>
+        <v>26.14</v>
       </c>
       <c r="AK149">
         <f t="shared" si="174"/>
@@ -21807,11 +21807,11 @@
       </c>
       <c r="AL149">
         <f t="shared" si="175"/>
-        <v>14.61</v>
+        <v>15.28</v>
       </c>
       <c r="AM149">
         <f t="shared" si="176"/>
-        <v>6.89</v>
+        <v>7.56</v>
       </c>
       <c r="AN149">
         <f t="shared" si="177"/>
@@ -21823,7 +21823,7 @@
       </c>
       <c r="AP149">
         <f t="shared" si="179"/>
-        <v>9.25</v>
+        <v>9.69</v>
       </c>
     </row>
     <row r="150" spans="1:42" x14ac:dyDescent="0.25">
@@ -21876,37 +21876,37 @@
         <v>108</v>
       </c>
       <c r="Q150">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="R150">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="S150">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="T150">
         <v>64</v>
       </c>
       <c r="U150">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="V150">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="W150">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="X150">
-        <v>695</v>
+        <v>652</v>
       </c>
       <c r="Y150">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="Z150">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="AA150">
-        <v>222</v>
+        <v>241</v>
       </c>
       <c r="AC150">
         <v>2022</v>
@@ -21915,52 +21915,52 @@
         <v>44</v>
       </c>
       <c r="AE150">
-        <f t="shared" ref="AE150" si="180">ROUND((P150-B150)/B150*100,2)</f>
+        <f t="shared" ref="AE150:AE151" si="180">ROUND((P150-B150)/B150*100,2)</f>
         <v>0</v>
       </c>
       <c r="AF150">
-        <f t="shared" ref="AF150" si="181">ROUND((Q150-C150)/C150*100,2)</f>
-        <v>16.260000000000002</v>
+        <f t="shared" ref="AF150:AF151" si="181">ROUND((Q150-C150)/C150*100,2)</f>
+        <v>8.94</v>
       </c>
       <c r="AG150">
-        <f t="shared" ref="AG150" si="182">ROUND((R150-D150)/D150*100,2)</f>
-        <v>34.69</v>
+        <f t="shared" ref="AG150:AG151" si="182">ROUND((R150-D150)/D150*100,2)</f>
+        <v>35.71</v>
       </c>
       <c r="AH150">
-        <f t="shared" ref="AH150" si="183">ROUND((S150-E150)/E150*100,2)</f>
-        <v>16.75</v>
+        <f t="shared" ref="AH150:AH151" si="183">ROUND((S150-E150)/E150*100,2)</f>
+        <v>15.23</v>
       </c>
       <c r="AI150">
-        <f t="shared" ref="AI150" si="184">ROUND((T150-F150)/F150*100,2)</f>
+        <f t="shared" ref="AI150:AI151" si="184">ROUND((T150-F150)/F150*100,2)</f>
         <v>33.33</v>
       </c>
       <c r="AJ150">
-        <f t="shared" ref="AJ150" si="185">ROUND((U150-G150)/G150*100,2)</f>
-        <v>9.8000000000000007</v>
+        <f t="shared" ref="AJ150:AJ151" si="185">ROUND((U150-G150)/G150*100,2)</f>
+        <v>8.68</v>
       </c>
       <c r="AK150">
-        <f t="shared" ref="AK150" si="186">ROUND((V150-H150)/H150*100,2)</f>
-        <v>12.76</v>
+        <f t="shared" ref="AK150:AK151" si="186">ROUND((V150-H150)/H150*100,2)</f>
+        <v>18.88</v>
       </c>
       <c r="AL150">
-        <f t="shared" ref="AL150" si="187">ROUND((W150-I150)/I150*100,2)</f>
-        <v>8.93</v>
+        <f t="shared" ref="AL150:AL151" si="187">ROUND((W150-I150)/I150*100,2)</f>
+        <v>5.36</v>
       </c>
       <c r="AM150">
-        <f t="shared" ref="AM150" si="188">ROUND((X150-J150)/J150*100,2)</f>
-        <v>15.83</v>
+        <f t="shared" ref="AM150:AM151" si="188">ROUND((X150-J150)/J150*100,2)</f>
+        <v>8.67</v>
       </c>
       <c r="AN150">
-        <f t="shared" ref="AN150" si="189">ROUND((Y150-K150)/K150*100,2)</f>
-        <v>14.1</v>
+        <f t="shared" ref="AN150:AN151" si="189">ROUND((Y150-K150)/K150*100,2)</f>
+        <v>5.13</v>
       </c>
       <c r="AO150">
-        <f t="shared" ref="AO150" si="190">ROUND((Z150-L150)/L150*100,2)</f>
-        <v>2.68</v>
+        <f t="shared" ref="AO150:AO151" si="190">ROUND((Z150-L150)/L150*100,2)</f>
+        <v>1.34</v>
       </c>
       <c r="AP150">
-        <f t="shared" ref="AP150" si="191">ROUND((AA150-M150)/M150*100,2)</f>
-        <v>-3.06</v>
+        <f t="shared" ref="AP150:AP151" si="191">ROUND((AA150-M150)/M150*100,2)</f>
+        <v>5.24</v>
       </c>
     </row>
     <row r="151" spans="1:42" x14ac:dyDescent="0.25">
@@ -22002,6 +22002,102 @@
       </c>
       <c r="M151">
         <v>231</v>
+      </c>
+      <c r="N151">
+        <v>2022</v>
+      </c>
+      <c r="O151">
+        <v>45</v>
+      </c>
+      <c r="P151">
+        <v>117</v>
+      </c>
+      <c r="Q151">
+        <v>132</v>
+      </c>
+      <c r="R151">
+        <v>135</v>
+      </c>
+      <c r="S151">
+        <v>222</v>
+      </c>
+      <c r="T151">
+        <v>63</v>
+      </c>
+      <c r="U151">
+        <v>431</v>
+      </c>
+      <c r="V151">
+        <v>235</v>
+      </c>
+      <c r="W151">
+        <v>470</v>
+      </c>
+      <c r="X151">
+        <v>646</v>
+      </c>
+      <c r="Y151">
+        <v>76</v>
+      </c>
+      <c r="Z151">
+        <v>493</v>
+      </c>
+      <c r="AA151">
+        <v>261</v>
+      </c>
+      <c r="AC151">
+        <v>2022</v>
+      </c>
+      <c r="AD151">
+        <v>45</v>
+      </c>
+      <c r="AE151">
+        <f t="shared" si="180"/>
+        <v>6.36</v>
+      </c>
+      <c r="AF151">
+        <f t="shared" si="181"/>
+        <v>7.32</v>
+      </c>
+      <c r="AG151">
+        <f t="shared" si="182"/>
+        <v>36.36</v>
+      </c>
+      <c r="AH151">
+        <f t="shared" si="183"/>
+        <v>11.56</v>
+      </c>
+      <c r="AI151">
+        <f t="shared" si="184"/>
+        <v>31.25</v>
+      </c>
+      <c r="AJ151">
+        <f t="shared" si="185"/>
+        <v>20.39</v>
+      </c>
+      <c r="AK151">
+        <f t="shared" si="186"/>
+        <v>18.09</v>
+      </c>
+      <c r="AL151">
+        <f t="shared" si="187"/>
+        <v>4.21</v>
+      </c>
+      <c r="AM151">
+        <f t="shared" si="188"/>
+        <v>7.49</v>
+      </c>
+      <c r="AN151">
+        <f t="shared" si="189"/>
+        <v>-3.8</v>
+      </c>
+      <c r="AO151">
+        <f t="shared" si="190"/>
+        <v>10.79</v>
+      </c>
+      <c r="AP151">
+        <f t="shared" si="191"/>
+        <v>12.99</v>
       </c>
     </row>
     <row r="152" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update excess mortality graphs - Week 48 (2022)
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8F535-3B1B-4998-B87B-EF3F6AFD7D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2364383-A2E3-471E-908D-0501A8B46CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA99" sqref="AA99"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI155" sqref="AI155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19008,7 +19008,7 @@
         <v>196</v>
       </c>
       <c r="T129">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U129">
         <v>395</v>
@@ -19020,7 +19020,7 @@
         <v>438</v>
       </c>
       <c r="X129">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="Y129">
         <v>73</v>
@@ -19055,7 +19055,7 @@
       </c>
       <c r="AI129">
         <f t="shared" si="76"/>
-        <v>40.479999999999997</v>
+        <v>42.86</v>
       </c>
       <c r="AJ129">
         <f t="shared" si="77"/>
@@ -19071,7 +19071,7 @@
       </c>
       <c r="AM129">
         <f t="shared" si="80"/>
-        <v>6.08</v>
+        <v>6.26</v>
       </c>
       <c r="AN129">
         <f t="shared" si="81"/>
@@ -19154,10 +19154,10 @@
         <v>222</v>
       </c>
       <c r="W130">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="X130">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="Y130">
         <v>65</v>
@@ -19204,11 +19204,11 @@
       </c>
       <c r="AL130">
         <f t="shared" si="79"/>
-        <v>4.42</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="AM130">
         <f t="shared" si="80"/>
-        <v>8.93</v>
+        <v>9.11</v>
       </c>
       <c r="AN130">
         <f t="shared" si="81"/>
@@ -19294,7 +19294,7 @@
         <v>444</v>
       </c>
       <c r="X131">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="Y131">
         <v>93</v>
@@ -19345,7 +19345,7 @@
       </c>
       <c r="AM131">
         <f t="shared" si="80"/>
-        <v>27.11</v>
+        <v>27.29</v>
       </c>
       <c r="AN131">
         <f t="shared" si="81"/>
@@ -20113,7 +20113,7 @@
         <v>198</v>
       </c>
       <c r="W137">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="X137">
         <v>614</v>
@@ -20163,7 +20163,7 @@
       </c>
       <c r="AL137">
         <f t="shared" si="103"/>
-        <v>7.31</v>
+        <v>7.55</v>
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
@@ -20524,7 +20524,7 @@
         <v>207</v>
       </c>
       <c r="W140">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="X140">
         <v>597</v>
@@ -20536,7 +20536,7 @@
         <v>489</v>
       </c>
       <c r="AA140">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AC140">
         <v>2022</v>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>5.21</v>
+        <v>5.45</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
@@ -20590,7 +20590,7 @@
       </c>
       <c r="AP140">
         <f t="shared" ref="AP140:AP141" si="131">ROUND((AA140-M140)/M140*100,2)</f>
-        <v>8.9600000000000009</v>
+        <v>9.43</v>
       </c>
     </row>
     <row r="141" spans="1:42" x14ac:dyDescent="0.25">
@@ -20664,7 +20664,7 @@
         <v>413</v>
       </c>
       <c r="X141">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="Y141">
         <v>72</v>
@@ -20715,7 +20715,7 @@
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>8.7100000000000009</v>
+        <v>8.89</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
@@ -20780,7 +20780,7 @@
         <v>123</v>
       </c>
       <c r="Q142">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="R142">
         <v>91</v>
@@ -20801,7 +20801,7 @@
         <v>458</v>
       </c>
       <c r="X142">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="Y142">
         <v>80</v>
@@ -20824,7 +20824,7 @@
       </c>
       <c r="AF142">
         <f t="shared" ref="AF142:AF143" si="133">ROUND((Q142-C142)/C142*100,2)</f>
-        <v>7.96</v>
+        <v>8.85</v>
       </c>
       <c r="AG142">
         <f t="shared" ref="AG142:AG143" si="134">ROUND((R142-D142)/D142*100,2)</f>
@@ -20852,7 +20852,7 @@
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
-        <v>7.21</v>
+        <v>7.39</v>
       </c>
       <c r="AN142">
         <f t="shared" ref="AN142:AN143" si="141">ROUND((Y142-K142)/K142*100,2)</f>
@@ -20929,7 +20929,7 @@
         <v>46</v>
       </c>
       <c r="U143">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="V143">
         <v>170</v>
@@ -20944,7 +20944,7 @@
         <v>61</v>
       </c>
       <c r="Z143">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AA143">
         <v>225</v>
@@ -20977,7 +20977,7 @@
       </c>
       <c r="AJ143">
         <f t="shared" si="137"/>
-        <v>11.31</v>
+        <v>11.61</v>
       </c>
       <c r="AK143">
         <f t="shared" si="138"/>
@@ -20997,7 +20997,7 @@
       </c>
       <c r="AO143">
         <f t="shared" si="142"/>
-        <v>2.96</v>
+        <v>3.2</v>
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
@@ -21075,7 +21075,7 @@
         <v>489</v>
       </c>
       <c r="X144">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="Y144">
         <v>75</v>
@@ -21126,7 +21126,7 @@
       </c>
       <c r="AM144">
         <f t="shared" ref="AM144:AM145" si="152">ROUND((X144-J144)/J144*100,2)</f>
-        <v>8.01</v>
+        <v>8.36</v>
       </c>
       <c r="AN144">
         <f t="shared" ref="AN144:AN145" si="153">ROUND((Y144-K144)/K144*100,2)</f>
@@ -21212,7 +21212,7 @@
         <v>486</v>
       </c>
       <c r="X145">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="Y145">
         <v>77</v>
@@ -21263,7 +21263,7 @@
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>15.38</v>
+        <v>15.56</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
@@ -21340,7 +21340,7 @@
         <v>51</v>
       </c>
       <c r="U146">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="V146">
         <v>217</v>
@@ -21388,7 +21388,7 @@
       </c>
       <c r="AJ146">
         <f t="shared" ref="AJ146:AJ147" si="161">ROUND((U146-G146)/G146*100,2)</f>
-        <v>29.94</v>
+        <v>30.23</v>
       </c>
       <c r="AK146">
         <f t="shared" ref="AK146:AK147" si="162">ROUND((V146-H146)/H146*100,2)</f>
@@ -21477,25 +21477,25 @@
         <v>50</v>
       </c>
       <c r="U147">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="V147">
         <v>218</v>
       </c>
       <c r="W147">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="X147">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="Y147">
         <v>88</v>
       </c>
       <c r="Z147">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AA147">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AC147">
         <v>2022</v>
@@ -21525,7 +21525,7 @@
       </c>
       <c r="AJ147">
         <f t="shared" si="161"/>
-        <v>31.52</v>
+        <v>31.81</v>
       </c>
       <c r="AK147">
         <f t="shared" si="162"/>
@@ -21533,11 +21533,11 @@
       </c>
       <c r="AL147">
         <f t="shared" si="163"/>
-        <v>8.43</v>
+        <v>8.8800000000000008</v>
       </c>
       <c r="AM147">
         <f t="shared" si="164"/>
-        <v>18.97</v>
+        <v>19.309999999999999</v>
       </c>
       <c r="AN147">
         <f t="shared" si="165"/>
@@ -21545,11 +21545,11 @@
       </c>
       <c r="AO147">
         <f t="shared" si="166"/>
-        <v>13.02</v>
+        <v>13.26</v>
       </c>
       <c r="AP147">
         <f t="shared" si="167"/>
-        <v>14.73</v>
+        <v>15.18</v>
       </c>
     </row>
     <row r="148" spans="1:42" x14ac:dyDescent="0.25">
@@ -21614,16 +21614,16 @@
         <v>63</v>
       </c>
       <c r="U148">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="V148">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="W148">
         <v>500</v>
       </c>
       <c r="X148">
-        <v>661</v>
+        <v>663</v>
       </c>
       <c r="Y148">
         <v>79</v>
@@ -21662,11 +21662,11 @@
       </c>
       <c r="AJ148">
         <f t="shared" ref="AJ148:AJ149" si="173">ROUND((U148-G148)/G148*100,2)</f>
-        <v>19.03</v>
+        <v>19.32</v>
       </c>
       <c r="AK148">
         <f t="shared" ref="AK148:AK149" si="174">ROUND((V148-H148)/H148*100,2)</f>
-        <v>22.05</v>
+        <v>22.56</v>
       </c>
       <c r="AL148">
         <f t="shared" ref="AL148:AL149" si="175">ROUND((W148-I148)/I148*100,2)</f>
@@ -21674,7 +21674,7 @@
       </c>
       <c r="AM148">
         <f t="shared" ref="AM148:AM149" si="176">ROUND((X148-J148)/J148*100,2)</f>
-        <v>11.84</v>
+        <v>12.18</v>
       </c>
       <c r="AN148">
         <f t="shared" ref="AN148:AN149" si="177">ROUND((Y148-K148)/K148*100,2)</f>
@@ -21745,7 +21745,7 @@
         <v>141</v>
       </c>
       <c r="S149">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="T149">
         <v>41</v>
@@ -21766,7 +21766,7 @@
         <v>80</v>
       </c>
       <c r="Z149">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="AA149">
         <v>249</v>
@@ -21791,7 +21791,7 @@
       </c>
       <c r="AH149">
         <f t="shared" si="171"/>
-        <v>14.29</v>
+        <v>14.8</v>
       </c>
       <c r="AI149">
         <f t="shared" si="172"/>
@@ -21819,7 +21819,7 @@
       </c>
       <c r="AO149">
         <f t="shared" si="178"/>
-        <v>13.41</v>
+        <v>13.64</v>
       </c>
       <c r="AP149">
         <f t="shared" si="179"/>
@@ -21888,25 +21888,25 @@
         <v>64</v>
       </c>
       <c r="U150">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="V150">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="W150">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="X150">
-        <v>656</v>
+        <v>660</v>
       </c>
       <c r="Y150">
         <v>82</v>
       </c>
       <c r="Z150">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="AA150">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AC150">
         <v>2022</v>
@@ -21936,19 +21936,19 @@
       </c>
       <c r="AJ150">
         <f t="shared" ref="AJ150:AJ151" si="185">ROUND((U150-G150)/G150*100,2)</f>
-        <v>8.9600000000000009</v>
+        <v>9.52</v>
       </c>
       <c r="AK150">
         <f t="shared" ref="AK150:AK151" si="186">ROUND((V150-H150)/H150*100,2)</f>
-        <v>19.39</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="AL150">
         <f t="shared" ref="AL150:AL151" si="187">ROUND((W150-I150)/I150*100,2)</f>
-        <v>6.7</v>
+        <v>6.92</v>
       </c>
       <c r="AM150">
         <f t="shared" ref="AM150:AM151" si="188">ROUND((X150-J150)/J150*100,2)</f>
-        <v>9.33</v>
+        <v>10</v>
       </c>
       <c r="AN150">
         <f t="shared" ref="AN150:AN151" si="189">ROUND((Y150-K150)/K150*100,2)</f>
@@ -21956,11 +21956,11 @@
       </c>
       <c r="AO150">
         <f t="shared" ref="AO150:AO151" si="190">ROUND((Z150-L150)/L150*100,2)</f>
-        <v>2.91</v>
+        <v>3.36</v>
       </c>
       <c r="AP150">
         <f t="shared" ref="AP150:AP151" si="191">ROUND((AA150-M150)/M150*100,2)</f>
-        <v>5.24</v>
+        <v>5.68</v>
       </c>
     </row>
     <row r="151" spans="1:42" x14ac:dyDescent="0.25">
@@ -22013,37 +22013,37 @@
         <v>115</v>
       </c>
       <c r="Q151">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="R151">
         <v>124</v>
       </c>
       <c r="S151">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T151">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U151">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="V151">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="W151">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="X151">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="Y151">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Z151">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="AA151">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AC151">
         <v>2022</v>
@@ -22057,7 +22057,7 @@
       </c>
       <c r="AF151">
         <f t="shared" si="181"/>
-        <v>11.38</v>
+        <v>12.2</v>
       </c>
       <c r="AG151">
         <f t="shared" si="182"/>
@@ -22065,39 +22065,39 @@
       </c>
       <c r="AH151">
         <f t="shared" si="183"/>
-        <v>7.54</v>
+        <v>8.5399999999999991</v>
       </c>
       <c r="AI151">
         <f t="shared" si="184"/>
-        <v>29.17</v>
+        <v>31.25</v>
       </c>
       <c r="AJ151">
         <f t="shared" si="185"/>
-        <v>15.64</v>
+        <v>16.48</v>
       </c>
       <c r="AK151">
         <f t="shared" si="186"/>
-        <v>18.09</v>
+        <v>18.59</v>
       </c>
       <c r="AL151">
         <f t="shared" si="187"/>
-        <v>-2.88</v>
+        <v>-2.2200000000000002</v>
       </c>
       <c r="AM151">
         <f t="shared" si="188"/>
-        <v>1</v>
+        <v>1.83</v>
       </c>
       <c r="AN151">
         <f t="shared" si="189"/>
-        <v>-7.59</v>
+        <v>-6.33</v>
       </c>
       <c r="AO151">
         <f t="shared" si="190"/>
-        <v>6.52</v>
+        <v>7.19</v>
       </c>
       <c r="AP151">
         <f t="shared" si="191"/>
-        <v>6.06</v>
+        <v>6.49</v>
       </c>
     </row>
     <row r="152" spans="1:42" x14ac:dyDescent="0.25">
@@ -22147,40 +22147,40 @@
         <v>46</v>
       </c>
       <c r="P152">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q152">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="R152">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S152">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="T152">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U152">
-        <v>426</v>
+        <v>408</v>
       </c>
       <c r="V152">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="W152">
-        <v>498</v>
+        <v>467</v>
       </c>
       <c r="X152">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="Y152">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Z152">
-        <v>512</v>
+        <v>486</v>
       </c>
       <c r="AA152">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="AC152">
         <v>2022</v>
@@ -22189,52 +22189,52 @@
         <v>46</v>
       </c>
       <c r="AE152">
-        <f t="shared" ref="AE152" si="192">ROUND((P152-B152)/B152*100,2)</f>
-        <v>-3.6</v>
+        <f t="shared" ref="AE152:AE153" si="192">ROUND((P152-B152)/B152*100,2)</f>
+        <v>-1.8</v>
       </c>
       <c r="AF152">
-        <f t="shared" ref="AF152" si="193">ROUND((Q152-C152)/C152*100,2)</f>
-        <v>21.95</v>
+        <f t="shared" ref="AF152:AF153" si="193">ROUND((Q152-C152)/C152*100,2)</f>
+        <v>14.63</v>
       </c>
       <c r="AG152">
-        <f t="shared" ref="AG152" si="194">ROUND((R152-D152)/D152*100,2)</f>
-        <v>-6</v>
+        <f t="shared" ref="AG152:AG153" si="194">ROUND((R152-D152)/D152*100,2)</f>
+        <v>-7</v>
       </c>
       <c r="AH152">
-        <f t="shared" ref="AH152" si="195">ROUND((S152-E152)/E152*100,2)</f>
-        <v>14.57</v>
+        <f t="shared" ref="AH152:AH153" si="195">ROUND((S152-E152)/E152*100,2)</f>
+        <v>11.56</v>
       </c>
       <c r="AI152">
-        <f t="shared" ref="AI152" si="196">ROUND((T152-F152)/F152*100,2)</f>
-        <v>16.329999999999998</v>
+        <f t="shared" ref="AI152:AI153" si="196">ROUND((T152-F152)/F152*100,2)</f>
+        <v>18.37</v>
       </c>
       <c r="AJ152">
-        <f t="shared" ref="AJ152" si="197">ROUND((U152-G152)/G152*100,2)</f>
-        <v>17.36</v>
+        <f t="shared" ref="AJ152:AJ153" si="197">ROUND((U152-G152)/G152*100,2)</f>
+        <v>12.4</v>
       </c>
       <c r="AK152">
-        <f t="shared" ref="AK152" si="198">ROUND((V152-H152)/H152*100,2)</f>
-        <v>20</v>
+        <f t="shared" ref="AK152:AK153" si="198">ROUND((V152-H152)/H152*100,2)</f>
+        <v>16</v>
       </c>
       <c r="AL152">
-        <f t="shared" ref="AL152" si="199">ROUND((W152-I152)/I152*100,2)</f>
-        <v>9.2100000000000009</v>
+        <f t="shared" ref="AL152:AL153" si="199">ROUND((W152-I152)/I152*100,2)</f>
+        <v>2.41</v>
       </c>
       <c r="AM152">
-        <f t="shared" ref="AM152" si="200">ROUND((X152-J152)/J152*100,2)</f>
-        <v>7.25</v>
+        <f t="shared" ref="AM152:AM153" si="200">ROUND((X152-J152)/J152*100,2)</f>
+        <v>6.92</v>
       </c>
       <c r="AN152">
-        <f t="shared" ref="AN152" si="201">ROUND((Y152-K152)/K152*100,2)</f>
-        <v>5.13</v>
+        <f t="shared" ref="AN152:AN153" si="201">ROUND((Y152-K152)/K152*100,2)</f>
+        <v>1.28</v>
       </c>
       <c r="AO152">
-        <f t="shared" ref="AO152" si="202">ROUND((Z152-L152)/L152*100,2)</f>
-        <v>13.27</v>
+        <f t="shared" ref="AO152:AO153" si="202">ROUND((Z152-L152)/L152*100,2)</f>
+        <v>7.52</v>
       </c>
       <c r="AP152">
-        <f t="shared" ref="AP152" si="203">ROUND((AA152-M152)/M152*100,2)</f>
-        <v>8.9</v>
+        <f t="shared" ref="AP152:AP153" si="203">ROUND((AA152-M152)/M152*100,2)</f>
+        <v>3.81</v>
       </c>
     </row>
     <row r="153" spans="1:42" x14ac:dyDescent="0.25">
@@ -22277,6 +22277,102 @@
       <c r="M153">
         <v>237</v>
       </c>
+      <c r="N153">
+        <v>2022</v>
+      </c>
+      <c r="O153">
+        <v>47</v>
+      </c>
+      <c r="P153">
+        <v>123</v>
+      </c>
+      <c r="Q153">
+        <v>141</v>
+      </c>
+      <c r="R153">
+        <v>123</v>
+      </c>
+      <c r="S153">
+        <v>219</v>
+      </c>
+      <c r="T153">
+        <v>61</v>
+      </c>
+      <c r="U153">
+        <v>429</v>
+      </c>
+      <c r="V153">
+        <v>249</v>
+      </c>
+      <c r="W153">
+        <v>484</v>
+      </c>
+      <c r="X153">
+        <v>669</v>
+      </c>
+      <c r="Y153">
+        <v>104</v>
+      </c>
+      <c r="Z153">
+        <v>496</v>
+      </c>
+      <c r="AA153">
+        <v>267</v>
+      </c>
+      <c r="AC153">
+        <v>2022</v>
+      </c>
+      <c r="AD153">
+        <v>47</v>
+      </c>
+      <c r="AE153">
+        <f t="shared" si="192"/>
+        <v>9.82</v>
+      </c>
+      <c r="AF153">
+        <f t="shared" si="193"/>
+        <v>12.8</v>
+      </c>
+      <c r="AG153">
+        <f t="shared" si="194"/>
+        <v>19.420000000000002</v>
+      </c>
+      <c r="AH153">
+        <f t="shared" si="195"/>
+        <v>7.88</v>
+      </c>
+      <c r="AI153">
+        <f t="shared" si="196"/>
+        <v>24.49</v>
+      </c>
+      <c r="AJ153">
+        <f t="shared" si="197"/>
+        <v>16.260000000000002</v>
+      </c>
+      <c r="AK153">
+        <f t="shared" si="198"/>
+        <v>23.88</v>
+      </c>
+      <c r="AL153">
+        <f t="shared" si="199"/>
+        <v>3.86</v>
+      </c>
+      <c r="AM153">
+        <f t="shared" si="200"/>
+        <v>9.14</v>
+      </c>
+      <c r="AN153">
+        <f t="shared" si="201"/>
+        <v>31.65</v>
+      </c>
+      <c r="AO153">
+        <f t="shared" si="202"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="AP153">
+        <f t="shared" si="203"/>
+        <v>12.66</v>
+      </c>
     </row>
     <row r="154" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
@@ -22317,6 +22413,102 @@
       </c>
       <c r="M154">
         <v>239</v>
+      </c>
+      <c r="N154">
+        <v>2022</v>
+      </c>
+      <c r="O154">
+        <v>48</v>
+      </c>
+      <c r="P154">
+        <v>128</v>
+      </c>
+      <c r="Q154">
+        <v>154</v>
+      </c>
+      <c r="R154">
+        <v>121</v>
+      </c>
+      <c r="S154">
+        <v>216</v>
+      </c>
+      <c r="T154">
+        <v>62</v>
+      </c>
+      <c r="U154">
+        <v>406</v>
+      </c>
+      <c r="V154">
+        <v>222</v>
+      </c>
+      <c r="W154">
+        <v>534</v>
+      </c>
+      <c r="X154">
+        <v>700</v>
+      </c>
+      <c r="Y154">
+        <v>75</v>
+      </c>
+      <c r="Z154">
+        <v>535</v>
+      </c>
+      <c r="AA154">
+        <v>251</v>
+      </c>
+      <c r="AC154">
+        <v>2022</v>
+      </c>
+      <c r="AD154">
+        <v>48</v>
+      </c>
+      <c r="AE154">
+        <f t="shared" ref="AE154" si="204">ROUND((P154-B154)/B154*100,2)</f>
+        <v>13.27</v>
+      </c>
+      <c r="AF154">
+        <f t="shared" ref="AF154" si="205">ROUND((Q154-C154)/C154*100,2)</f>
+        <v>22.22</v>
+      </c>
+      <c r="AG154">
+        <f t="shared" ref="AG154" si="206">ROUND((R154-D154)/D154*100,2)</f>
+        <v>15.24</v>
+      </c>
+      <c r="AH154">
+        <f t="shared" ref="AH154" si="207">ROUND((S154-E154)/E154*100,2)</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="AI154">
+        <f t="shared" ref="AI154" si="208">ROUND((T154-F154)/F154*100,2)</f>
+        <v>29.17</v>
+      </c>
+      <c r="AJ154">
+        <f t="shared" ref="AJ154" si="209">ROUND((U154-G154)/G154*100,2)</f>
+        <v>8.56</v>
+      </c>
+      <c r="AK154">
+        <f t="shared" ref="AK154" si="210">ROUND((V154-H154)/H154*100,2)</f>
+        <v>7.77</v>
+      </c>
+      <c r="AL154">
+        <f t="shared" ref="AL154" si="211">ROUND((W154-I154)/I154*100,2)</f>
+        <v>13.62</v>
+      </c>
+      <c r="AM154">
+        <f t="shared" ref="AM154" si="212">ROUND((X154-J154)/J154*100,2)</f>
+        <v>11.82</v>
+      </c>
+      <c r="AN154">
+        <f t="shared" ref="AN154" si="213">ROUND((Y154-K154)/K154*100,2)</f>
+        <v>-6.25</v>
+      </c>
+      <c r="AO154">
+        <f t="shared" ref="AO154" si="214">ROUND((Z154-L154)/L154*100,2)</f>
+        <v>15.8</v>
+      </c>
+      <c r="AP154">
+        <f t="shared" ref="AP154" si="215">ROUND((AA154-M154)/M154*100,2)</f>
+        <v>5.0199999999999996</v>
       </c>
     </row>
     <row r="155" spans="1:42" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update cases per ggd/per week per agegroup 2023-01-06
</commit_message>
<xml_diff>
--- a/data-misc/excess_mortality/excess_mortality_provinces.xlsx
+++ b/data-misc/excess_mortality/excess_mortality_provinces.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Documents\covid-19\data-misc\excess_mortality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2364383-A2E3-471E-908D-0501A8B46CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719DA419-8B57-4B36-BA2C-1DFE9F290400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI155" sqref="AI155"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG156" sqref="AG156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16828,7 +16828,7 @@
         <v>516</v>
       </c>
       <c r="X113">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="Y113">
         <v>103</v>
@@ -16879,7 +16879,7 @@
       </c>
       <c r="AM113">
         <f t="shared" si="32"/>
-        <v>-0.86</v>
+        <v>-0.72</v>
       </c>
       <c r="AN113">
         <f t="shared" si="33"/>
@@ -17796,7 +17796,7 @@
         <v>529</v>
       </c>
       <c r="AA120">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AC120">
         <v>2022</v>
@@ -17850,7 +17850,7 @@
       </c>
       <c r="AP120">
         <f t="shared" si="35"/>
-        <v>11.89</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="121" spans="1:42" x14ac:dyDescent="0.25">
@@ -18320,7 +18320,7 @@
         <v>110</v>
       </c>
       <c r="S124">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="T124">
         <v>54</v>
@@ -18366,7 +18366,7 @@
       </c>
       <c r="AH124">
         <f t="shared" si="51"/>
-        <v>4.9800000000000004</v>
+        <v>5.47</v>
       </c>
       <c r="AI124">
         <f t="shared" si="52"/>
@@ -19565,7 +19565,7 @@
         <v>197</v>
       </c>
       <c r="W133">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="X133">
         <v>605</v>
@@ -19615,7 +19615,7 @@
       </c>
       <c r="AL133">
         <f t="shared" ref="AL133:AL135" si="91">ROUND((W133-I133)/I133*100,2)</f>
-        <v>10.51</v>
+        <v>10.75</v>
       </c>
       <c r="AM133">
         <f t="shared" ref="AM133:AM135" si="92">ROUND((X133-J133)/J133*100,2)</f>
@@ -19702,7 +19702,7 @@
         <v>217</v>
       </c>
       <c r="W134">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="X134">
         <v>626</v>
@@ -19752,7 +19752,7 @@
       </c>
       <c r="AL134">
         <f t="shared" si="91"/>
-        <v>18.649999999999999</v>
+        <v>18.88</v>
       </c>
       <c r="AM134">
         <f t="shared" si="92"/>
@@ -19833,7 +19833,7 @@
         <v>59</v>
       </c>
       <c r="U135">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="V135">
         <v>195</v>
@@ -19881,7 +19881,7 @@
       </c>
       <c r="AJ135">
         <f t="shared" si="89"/>
-        <v>19.23</v>
+        <v>19.53</v>
       </c>
       <c r="AK135">
         <f t="shared" si="90"/>
@@ -20116,7 +20116,7 @@
         <v>456</v>
       </c>
       <c r="X137">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="Y137">
         <v>65</v>
@@ -20167,7 +20167,7 @@
       </c>
       <c r="AM137">
         <f t="shared" si="104"/>
-        <v>9.84</v>
+        <v>10.02</v>
       </c>
       <c r="AN137">
         <f t="shared" si="105"/>
@@ -20250,7 +20250,7 @@
         <v>175</v>
       </c>
       <c r="W138">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="X138">
         <v>598</v>
@@ -20300,7 +20300,7 @@
       </c>
       <c r="AL138">
         <f t="shared" ref="AL138:AL139" si="115">ROUND((W138-I138)/I138*100,2)</f>
-        <v>5.41</v>
+        <v>5.65</v>
       </c>
       <c r="AM138">
         <f t="shared" ref="AM138:AM139" si="116">ROUND((X138-J138)/J138*100,2)</f>
@@ -20390,7 +20390,7 @@
         <v>502</v>
       </c>
       <c r="X139">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="Y139">
         <v>70</v>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="AM139">
         <f t="shared" si="116"/>
-        <v>10.34</v>
+        <v>10.53</v>
       </c>
       <c r="AN139">
         <f t="shared" si="117"/>
@@ -20524,7 +20524,7 @@
         <v>207</v>
       </c>
       <c r="W140">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="X140">
         <v>597</v>
@@ -20574,7 +20574,7 @@
       </c>
       <c r="AL140">
         <f t="shared" ref="AL140:AL141" si="127">ROUND((W140-I140)/I140*100,2)</f>
-        <v>5.45</v>
+        <v>6.16</v>
       </c>
       <c r="AM140">
         <f t="shared" ref="AM140:AM141" si="128">ROUND((X140-J140)/J140*100,2)</f>
@@ -20664,7 +20664,7 @@
         <v>413</v>
       </c>
       <c r="X141">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="Y141">
         <v>72</v>
@@ -20715,7 +20715,7 @@
       </c>
       <c r="AM141">
         <f t="shared" si="128"/>
-        <v>8.89</v>
+        <v>9.07</v>
       </c>
       <c r="AN141">
         <f t="shared" si="129"/>
@@ -20801,10 +20801,10 @@
         <v>458</v>
       </c>
       <c r="X142">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="Y142">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z142">
         <v>452</v>
@@ -20852,11 +20852,11 @@
       </c>
       <c r="AM142">
         <f t="shared" ref="AM142:AM143" si="140">ROUND((X142-J142)/J142*100,2)</f>
-        <v>7.39</v>
+        <v>7.57</v>
       </c>
       <c r="AN142">
         <f t="shared" ref="AN142:AN143" si="141">ROUND((Y142-K142)/K142*100,2)</f>
-        <v>14.29</v>
+        <v>15.71</v>
       </c>
       <c r="AO142">
         <f t="shared" ref="AO142:AO143" si="142">ROUND((Z142-L142)/L142*100,2)</f>
@@ -20917,7 +20917,7 @@
         <v>111</v>
       </c>
       <c r="Q143">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="R143">
         <v>86</v>
@@ -20926,10 +20926,10 @@
         <v>193</v>
       </c>
       <c r="T143">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="U143">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="V143">
         <v>170</v>
@@ -20944,7 +20944,7 @@
         <v>61</v>
       </c>
       <c r="Z143">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AA143">
         <v>225</v>
@@ -20961,7 +20961,7 @@
       </c>
       <c r="AF143">
         <f t="shared" si="133"/>
-        <v>-2.65</v>
+        <v>-1.77</v>
       </c>
       <c r="AG143">
         <f t="shared" si="134"/>
@@ -20973,11 +20973,11 @@
       </c>
       <c r="AI143">
         <f t="shared" si="136"/>
-        <v>6.98</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="AJ143">
         <f t="shared" si="137"/>
-        <v>11.61</v>
+        <v>11.9</v>
       </c>
       <c r="AK143">
         <f t="shared" si="138"/>
@@ -20997,7 +20997,7 @@
       </c>
       <c r="AO143">
         <f t="shared" si="142"/>
-        <v>3.2</v>
+        <v>3.45</v>
       </c>
       <c r="AP143">
         <f t="shared" si="143"/>
@@ -21057,7 +21057,7 @@
         <v>130</v>
       </c>
       <c r="R144">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="S144">
         <v>206</v>
@@ -21069,7 +21069,7 @@
         <v>377</v>
       </c>
       <c r="V144">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="W144">
         <v>489</v>
@@ -21102,7 +21102,7 @@
       </c>
       <c r="AG144">
         <f t="shared" ref="AG144:AG145" si="146">ROUND((R144-D144)/D144*100,2)</f>
-        <v>14.58</v>
+        <v>15.63</v>
       </c>
       <c r="AH144">
         <f t="shared" ref="AH144:AH145" si="147">ROUND((S144-E144)/E144*100,2)</f>
@@ -21118,7 +21118,7 @@
       </c>
       <c r="AK144">
         <f t="shared" ref="AK144:AK145" si="150">ROUND((V144-H144)/H144*100,2)</f>
-        <v>22.04</v>
+        <v>22.58</v>
       </c>
       <c r="AL144">
         <f t="shared" ref="AL144:AL145" si="151">ROUND((W144-I144)/I144*100,2)</f>
@@ -21209,16 +21209,16 @@
         <v>231</v>
       </c>
       <c r="W145">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="X145">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="Y145">
         <v>77</v>
       </c>
       <c r="Z145">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="AA145">
         <v>248</v>
@@ -21259,11 +21259,11 @@
       </c>
       <c r="AL145">
         <f t="shared" si="151"/>
-        <v>11.98</v>
+        <v>12.21</v>
       </c>
       <c r="AM145">
         <f t="shared" si="152"/>
-        <v>15.56</v>
+        <v>15.73</v>
       </c>
       <c r="AN145">
         <f t="shared" si="153"/>
@@ -21271,7 +21271,7 @@
       </c>
       <c r="AO145">
         <f t="shared" si="154"/>
-        <v>3.59</v>
+        <v>4.07</v>
       </c>
       <c r="AP145">
         <f t="shared" si="155"/>
@@ -21328,13 +21328,13 @@
         <v>129</v>
       </c>
       <c r="Q146">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="R146">
         <v>104</v>
       </c>
       <c r="S146">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="T146">
         <v>51</v>
@@ -21355,7 +21355,7 @@
         <v>85</v>
       </c>
       <c r="Z146">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AA146">
         <v>224</v>
@@ -21372,7 +21372,7 @@
       </c>
       <c r="AF146">
         <f t="shared" ref="AF146:AF147" si="157">ROUND((Q146-C146)/C146*100,2)</f>
-        <v>14.53</v>
+        <v>15.38</v>
       </c>
       <c r="AG146">
         <f t="shared" ref="AG146:AG147" si="158">ROUND((R146-D146)/D146*100,2)</f>
@@ -21380,7 +21380,7 @@
       </c>
       <c r="AH146">
         <f t="shared" ref="AH146:AH147" si="159">ROUND((S146-E146)/E146*100,2)</f>
-        <v>28.8</v>
+        <v>29.32</v>
       </c>
       <c r="AI146">
         <f t="shared" ref="AI146:AI147" si="160">ROUND((T146-F146)/F146*100,2)</f>
@@ -21408,7 +21408,7 @@
       </c>
       <c r="AO146">
         <f t="shared" ref="AO146:AO147" si="166">ROUND((Z146-L146)/L146*100,2)</f>
-        <v>17.649999999999999</v>
+        <v>17.88</v>
       </c>
       <c r="AP146">
         <f t="shared" ref="AP146:AP147" si="167">ROUND((AA146-M146)/M146*100,2)</f>
@@ -21474,7 +21474,7 @@
         <v>232</v>
       </c>
       <c r="T147">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U147">
         <v>460</v>
@@ -21483,16 +21483,16 @@
         <v>218</v>
       </c>
       <c r="W147">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="X147">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="Y147">
         <v>88</v>
       </c>
       <c r="Z147">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="AA147">
         <v>258</v>
@@ -21521,7 +21521,7 @@
       </c>
       <c r="AI147">
         <f t="shared" si="160"/>
-        <v>6.38</v>
+        <v>8.51</v>
       </c>
       <c r="AJ147">
         <f t="shared" si="161"/>
@@ -21533,11 +21533,11 @@
       </c>
       <c r="AL147">
         <f t="shared" si="163"/>
-        <v>8.8800000000000008</v>
+        <v>9.34</v>
       </c>
       <c r="AM147">
         <f t="shared" si="164"/>
-        <v>19.309999999999999</v>
+        <v>19.66</v>
       </c>
       <c r="AN147">
         <f t="shared" si="165"/>
@@ -21545,7 +21545,7 @@
       </c>
       <c r="AO147">
         <f t="shared" si="166"/>
-        <v>13.26</v>
+        <v>13.72</v>
       </c>
       <c r="AP147">
         <f t="shared" si="167"/>
@@ -21605,7 +21605,7 @@
         <v>150</v>
       </c>
       <c r="R148">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="S148">
         <v>252</v>
@@ -21614,16 +21614,16 @@
         <v>63</v>
       </c>
       <c r="U148">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="V148">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="W148">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="X148">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="Y148">
         <v>79</v>
@@ -21650,7 +21650,7 @@
       </c>
       <c r="AG148">
         <f t="shared" ref="AG148:AG149" si="170">ROUND((R148-D148)/D148*100,2)</f>
-        <v>14.74</v>
+        <v>15.79</v>
       </c>
       <c r="AH148">
         <f t="shared" ref="AH148:AH149" si="171">ROUND((S148-E148)/E148*100,2)</f>
@@ -21662,19 +21662,19 @@
       </c>
       <c r="AJ148">
         <f t="shared" ref="AJ148:AJ149" si="173">ROUND((U148-G148)/G148*100,2)</f>
-        <v>19.32</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="AK148">
         <f t="shared" ref="AK148:AK149" si="174">ROUND((V148-H148)/H148*100,2)</f>
-        <v>22.56</v>
+        <v>23.08</v>
       </c>
       <c r="AL148">
         <f t="shared" ref="AL148:AL149" si="175">ROUND((W148-I148)/I148*100,2)</f>
-        <v>13.38</v>
+        <v>13.83</v>
       </c>
       <c r="AM148">
         <f t="shared" ref="AM148:AM149" si="176">ROUND((X148-J148)/J148*100,2)</f>
-        <v>12.18</v>
+        <v>12.35</v>
       </c>
       <c r="AN148">
         <f t="shared" ref="AN148:AN149" si="177">ROUND((Y148-K148)/K148*100,2)</f>
@@ -21754,13 +21754,13 @@
         <v>444</v>
       </c>
       <c r="V149">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="W149">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="X149">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="Y149">
         <v>80</v>
@@ -21803,15 +21803,15 @@
       </c>
       <c r="AK149">
         <f t="shared" si="174"/>
-        <v>9.18</v>
+        <v>9.69</v>
       </c>
       <c r="AL149">
         <f t="shared" si="175"/>
-        <v>15.73</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="AM149">
         <f t="shared" si="176"/>
-        <v>7.73</v>
+        <v>8.24</v>
       </c>
       <c r="AN149">
         <f t="shared" si="177"/>
@@ -21888,22 +21888,22 @@
         <v>64</v>
       </c>
       <c r="U150">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="V150">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="W150">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="X150">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="Y150">
         <v>82</v>
       </c>
       <c r="Z150">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AA150">
         <v>242</v>
@@ -21936,19 +21936,19 @@
       </c>
       <c r="AJ150">
         <f t="shared" ref="AJ150:AJ151" si="185">ROUND((U150-G150)/G150*100,2)</f>
-        <v>9.52</v>
+        <v>10.08</v>
       </c>
       <c r="AK150">
         <f t="shared" ref="AK150:AK151" si="186">ROUND((V150-H150)/H150*100,2)</f>
-        <v>19.899999999999999</v>
+        <v>20.41</v>
       </c>
       <c r="AL150">
         <f t="shared" ref="AL150:AL151" si="187">ROUND((W150-I150)/I150*100,2)</f>
-        <v>6.92</v>
+        <v>7.37</v>
       </c>
       <c r="AM150">
         <f t="shared" ref="AM150:AM151" si="188">ROUND((X150-J150)/J150*100,2)</f>
-        <v>10</v>
+        <v>10.17</v>
       </c>
       <c r="AN150">
         <f t="shared" ref="AN150:AN151" si="189">ROUND((Y150-K150)/K150*100,2)</f>
@@ -21956,7 +21956,7 @@
       </c>
       <c r="AO150">
         <f t="shared" ref="AO150:AO151" si="190">ROUND((Z150-L150)/L150*100,2)</f>
-        <v>3.36</v>
+        <v>3.58</v>
       </c>
       <c r="AP150">
         <f t="shared" ref="AP150:AP151" si="191">ROUND((AA150-M150)/M150*100,2)</f>
@@ -22016,7 +22016,7 @@
         <v>138</v>
       </c>
       <c r="R151">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="S151">
         <v>216</v>
@@ -22025,25 +22025,25 @@
         <v>63</v>
       </c>
       <c r="U151">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="V151">
         <v>236</v>
       </c>
       <c r="W151">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="X151">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="Y151">
         <v>74</v>
       </c>
       <c r="Z151">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA151">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AC151">
         <v>2022</v>
@@ -22061,7 +22061,7 @@
       </c>
       <c r="AG151">
         <f t="shared" si="182"/>
-        <v>25.25</v>
+        <v>26.26</v>
       </c>
       <c r="AH151">
         <f t="shared" si="183"/>
@@ -22073,7 +22073,7 @@
       </c>
       <c r="AJ151">
         <f t="shared" si="185"/>
-        <v>16.48</v>
+        <v>17.04</v>
       </c>
       <c r="AK151">
         <f t="shared" si="186"/>
@@ -22081,11 +22081,11 @@
       </c>
       <c r="AL151">
         <f t="shared" si="187"/>
-        <v>-2.2200000000000002</v>
+        <v>-2</v>
       </c>
       <c r="AM151">
         <f t="shared" si="188"/>
-        <v>1.83</v>
+        <v>2.5</v>
       </c>
       <c r="AN151">
         <f t="shared" si="189"/>
@@ -22093,11 +22093,11 @@
       </c>
       <c r="AO151">
         <f t="shared" si="190"/>
-        <v>7.19</v>
+        <v>7.42</v>
       </c>
       <c r="AP151">
         <f t="shared" si="191"/>
-        <v>6.49</v>
+        <v>6.93</v>
       </c>
     </row>
     <row r="152" spans="1:42" x14ac:dyDescent="0.25">
@@ -22165,19 +22165,19 @@
         <v>408</v>
       </c>
       <c r="V152">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="W152">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="X152">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="Y152">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z152">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AA152">
         <v>245</v>
@@ -22214,23 +22214,23 @@
       </c>
       <c r="AK152">
         <f t="shared" ref="AK152:AK153" si="198">ROUND((V152-H152)/H152*100,2)</f>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AL152">
         <f t="shared" ref="AL152:AL153" si="199">ROUND((W152-I152)/I152*100,2)</f>
-        <v>2.41</v>
+        <v>3.51</v>
       </c>
       <c r="AM152">
         <f t="shared" ref="AM152:AM153" si="200">ROUND((X152-J152)/J152*100,2)</f>
-        <v>6.92</v>
+        <v>7.58</v>
       </c>
       <c r="AN152">
         <f t="shared" ref="AN152:AN153" si="201">ROUND((Y152-K152)/K152*100,2)</f>
-        <v>1.28</v>
+        <v>2.56</v>
       </c>
       <c r="AO152">
         <f t="shared" ref="AO152:AO153" si="202">ROUND((Z152-L152)/L152*100,2)</f>
-        <v>7.52</v>
+        <v>7.74</v>
       </c>
       <c r="AP152">
         <f t="shared" ref="AP152:AP153" si="203">ROUND((AA152-M152)/M152*100,2)</f>
@@ -22290,34 +22290,34 @@
         <v>141</v>
       </c>
       <c r="R153">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="S153">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="T153">
         <v>61</v>
       </c>
       <c r="U153">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="V153">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="W153">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="X153">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="Y153">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="Z153">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="AA153">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="AC153">
         <v>2022</v>
@@ -22335,11 +22335,11 @@
       </c>
       <c r="AG153">
         <f t="shared" si="194"/>
-        <v>19.420000000000002</v>
+        <v>20.39</v>
       </c>
       <c r="AH153">
         <f t="shared" si="195"/>
-        <v>7.88</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="AI153">
         <f t="shared" si="196"/>
@@ -22347,31 +22347,31 @@
       </c>
       <c r="AJ153">
         <f t="shared" si="197"/>
-        <v>16.260000000000002</v>
+        <v>16.8</v>
       </c>
       <c r="AK153">
         <f t="shared" si="198"/>
-        <v>23.88</v>
+        <v>24.38</v>
       </c>
       <c r="AL153">
         <f t="shared" si="199"/>
-        <v>3.86</v>
+        <v>5.36</v>
       </c>
       <c r="AM153">
         <f t="shared" si="200"/>
-        <v>9.14</v>
+        <v>10.6</v>
       </c>
       <c r="AN153">
         <f t="shared" si="201"/>
-        <v>31.65</v>
+        <v>32.909999999999997</v>
       </c>
       <c r="AO153">
         <f t="shared" si="202"/>
-        <v>8.3000000000000007</v>
+        <v>9.39</v>
       </c>
       <c r="AP153">
         <f t="shared" si="203"/>
-        <v>12.66</v>
+        <v>14.35</v>
       </c>
     </row>
     <row r="154" spans="1:42" x14ac:dyDescent="0.25">
@@ -22424,37 +22424,37 @@
         <v>128</v>
       </c>
       <c r="Q154">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="R154">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S154">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="T154">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="U154">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="V154">
-        <v>222</v>
+        <v>249</v>
       </c>
       <c r="W154">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="X154">
-        <v>700</v>
+        <v>681</v>
       </c>
       <c r="Y154">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="Z154">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="AA154">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="AC154">
         <v>2022</v>
@@ -22463,52 +22463,52 @@
         <v>48</v>
       </c>
       <c r="AE154">
-        <f t="shared" ref="AE154" si="204">ROUND((P154-B154)/B154*100,2)</f>
+        <f t="shared" ref="AE154:AE155" si="204">ROUND((P154-B154)/B154*100,2)</f>
         <v>13.27</v>
       </c>
       <c r="AF154">
-        <f t="shared" ref="AF154" si="205">ROUND((Q154-C154)/C154*100,2)</f>
-        <v>22.22</v>
+        <f t="shared" ref="AF154:AF155" si="205">ROUND((Q154-C154)/C154*100,2)</f>
+        <v>24.6</v>
       </c>
       <c r="AG154">
-        <f t="shared" ref="AG154" si="206">ROUND((R154-D154)/D154*100,2)</f>
-        <v>15.24</v>
+        <f t="shared" ref="AG154:AG155" si="206">ROUND((R154-D154)/D154*100,2)</f>
+        <v>13.33</v>
       </c>
       <c r="AH154">
-        <f t="shared" ref="AH154" si="207">ROUND((S154-E154)/E154*100,2)</f>
-        <v>4.8499999999999996</v>
+        <f t="shared" ref="AH154:AH155" si="207">ROUND((S154-E154)/E154*100,2)</f>
+        <v>7.77</v>
       </c>
       <c r="AI154">
-        <f t="shared" ref="AI154" si="208">ROUND((T154-F154)/F154*100,2)</f>
-        <v>29.17</v>
+        <f t="shared" ref="AI154:AI155" si="208">ROUND((T154-F154)/F154*100,2)</f>
+        <v>31.25</v>
       </c>
       <c r="AJ154">
-        <f t="shared" ref="AJ154" si="209">ROUND((U154-G154)/G154*100,2)</f>
-        <v>8.56</v>
+        <f t="shared" ref="AJ154:AJ155" si="209">ROUND((U154-G154)/G154*100,2)</f>
+        <v>10.43</v>
       </c>
       <c r="AK154">
-        <f t="shared" ref="AK154" si="210">ROUND((V154-H154)/H154*100,2)</f>
-        <v>7.77</v>
+        <f t="shared" ref="AK154:AK155" si="210">ROUND((V154-H154)/H154*100,2)</f>
+        <v>20.87</v>
       </c>
       <c r="AL154">
-        <f t="shared" ref="AL154" si="211">ROUND((W154-I154)/I154*100,2)</f>
-        <v>13.62</v>
+        <f t="shared" ref="AL154:AL155" si="211">ROUND((W154-I154)/I154*100,2)</f>
+        <v>12.98</v>
       </c>
       <c r="AM154">
-        <f t="shared" ref="AM154" si="212">ROUND((X154-J154)/J154*100,2)</f>
-        <v>11.82</v>
+        <f t="shared" ref="AM154:AM155" si="212">ROUND((X154-J154)/J154*100,2)</f>
+        <v>8.7899999999999991</v>
       </c>
       <c r="AN154">
-        <f t="shared" ref="AN154" si="213">ROUND((Y154-K154)/K154*100,2)</f>
-        <v>-6.25</v>
+        <f t="shared" ref="AN154:AN155" si="213">ROUND((Y154-K154)/K154*100,2)</f>
+        <v>-10</v>
       </c>
       <c r="AO154">
-        <f t="shared" ref="AO154" si="214">ROUND((Z154-L154)/L154*100,2)</f>
-        <v>15.8</v>
+        <f t="shared" ref="AO154:AO155" si="214">ROUND((Z154-L154)/L154*100,2)</f>
+        <v>14.07</v>
       </c>
       <c r="AP154">
-        <f t="shared" ref="AP154" si="215">ROUND((AA154-M154)/M154*100,2)</f>
-        <v>5.0199999999999996</v>
+        <f t="shared" ref="AP154:AP155" si="215">ROUND((AA154-M154)/M154*100,2)</f>
+        <v>8.7899999999999991</v>
       </c>
     </row>
     <row r="155" spans="1:42" x14ac:dyDescent="0.25">
@@ -22551,6 +22551,102 @@
       <c r="M155">
         <v>241</v>
       </c>
+      <c r="N155">
+        <v>2022</v>
+      </c>
+      <c r="O155">
+        <v>49</v>
+      </c>
+      <c r="P155">
+        <v>132</v>
+      </c>
+      <c r="Q155">
+        <v>153</v>
+      </c>
+      <c r="R155">
+        <v>111</v>
+      </c>
+      <c r="S155">
+        <v>258</v>
+      </c>
+      <c r="T155">
+        <v>64</v>
+      </c>
+      <c r="U155">
+        <v>423</v>
+      </c>
+      <c r="V155">
+        <v>246</v>
+      </c>
+      <c r="W155">
+        <v>527</v>
+      </c>
+      <c r="X155">
+        <v>732</v>
+      </c>
+      <c r="Y155">
+        <v>109</v>
+      </c>
+      <c r="Z155">
+        <v>548</v>
+      </c>
+      <c r="AA155">
+        <v>291</v>
+      </c>
+      <c r="AC155">
+        <v>2022</v>
+      </c>
+      <c r="AD155">
+        <v>49</v>
+      </c>
+      <c r="AE155">
+        <f t="shared" si="204"/>
+        <v>14.78</v>
+      </c>
+      <c r="AF155">
+        <f t="shared" si="205"/>
+        <v>23.39</v>
+      </c>
+      <c r="AG155">
+        <f t="shared" si="206"/>
+        <v>5.71</v>
+      </c>
+      <c r="AH155">
+        <f t="shared" si="207"/>
+        <v>24.64</v>
+      </c>
+      <c r="AI155">
+        <f t="shared" si="208"/>
+        <v>30.61</v>
+      </c>
+      <c r="AJ155">
+        <f t="shared" si="209"/>
+        <v>12.5</v>
+      </c>
+      <c r="AK155">
+        <f t="shared" si="210"/>
+        <v>18.27</v>
+      </c>
+      <c r="AL155">
+        <f t="shared" si="211"/>
+        <v>10.71</v>
+      </c>
+      <c r="AM155">
+        <f t="shared" si="212"/>
+        <v>15.82</v>
+      </c>
+      <c r="AN155">
+        <f t="shared" si="213"/>
+        <v>37.97</v>
+      </c>
+      <c r="AO155">
+        <f t="shared" si="214"/>
+        <v>17.34</v>
+      </c>
+      <c r="AP155">
+        <f t="shared" si="215"/>
+        <v>20.75</v>
+      </c>
     </row>
     <row r="156" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
@@ -22592,6 +22688,102 @@
       <c r="M156">
         <v>244</v>
       </c>
+      <c r="N156">
+        <v>2022</v>
+      </c>
+      <c r="O156">
+        <v>50</v>
+      </c>
+      <c r="P156">
+        <v>129</v>
+      </c>
+      <c r="Q156">
+        <v>174</v>
+      </c>
+      <c r="R156">
+        <v>147</v>
+      </c>
+      <c r="S156">
+        <v>280</v>
+      </c>
+      <c r="T156">
+        <v>70</v>
+      </c>
+      <c r="U156">
+        <v>501</v>
+      </c>
+      <c r="V156">
+        <v>262</v>
+      </c>
+      <c r="W156">
+        <v>560</v>
+      </c>
+      <c r="X156">
+        <v>803</v>
+      </c>
+      <c r="Y156">
+        <v>106</v>
+      </c>
+      <c r="Z156">
+        <v>617</v>
+      </c>
+      <c r="AA156">
+        <v>314</v>
+      </c>
+      <c r="AC156">
+        <v>2022</v>
+      </c>
+      <c r="AD156">
+        <v>50</v>
+      </c>
+      <c r="AE156">
+        <f t="shared" ref="AE156:AE158" si="216">ROUND((P156-B156)/B156*100,2)</f>
+        <v>11.21</v>
+      </c>
+      <c r="AF156">
+        <f t="shared" ref="AF156:AF158" si="217">ROUND((Q156-C156)/C156*100,2)</f>
+        <v>37.01</v>
+      </c>
+      <c r="AG156">
+        <f t="shared" ref="AG156:AG158" si="218">ROUND((R156-D156)/D156*100,2)</f>
+        <v>37.380000000000003</v>
+      </c>
+      <c r="AH156">
+        <f t="shared" ref="AH156:AH158" si="219">ROUND((S156-E156)/E156*100,2)</f>
+        <v>30.84</v>
+      </c>
+      <c r="AI156">
+        <f t="shared" ref="AI156:AI158" si="220">ROUND((T156-F156)/F156*100,2)</f>
+        <v>37.25</v>
+      </c>
+      <c r="AJ156">
+        <f t="shared" ref="AJ156:AJ158" si="221">ROUND((U156-G156)/G156*100,2)</f>
+        <v>29.46</v>
+      </c>
+      <c r="AK156">
+        <f t="shared" ref="AK156:AK158" si="222">ROUND((V156-H156)/H156*100,2)</f>
+        <v>24.76</v>
+      </c>
+      <c r="AL156">
+        <f t="shared" ref="AL156:AL158" si="223">ROUND((W156-I156)/I156*100,2)</f>
+        <v>14.29</v>
+      </c>
+      <c r="AM156">
+        <f t="shared" ref="AM156:AM158" si="224">ROUND((X156-J156)/J156*100,2)</f>
+        <v>23.92</v>
+      </c>
+      <c r="AN156">
+        <f t="shared" ref="AN156:AN158" si="225">ROUND((Y156-K156)/K156*100,2)</f>
+        <v>32.5</v>
+      </c>
+      <c r="AO156">
+        <f t="shared" ref="AO156:AO158" si="226">ROUND((Z156-L156)/L156*100,2)</f>
+        <v>31.28</v>
+      </c>
+      <c r="AP156">
+        <f t="shared" ref="AP156:AP158" si="227">ROUND((AA156-M156)/M156*100,2)</f>
+        <v>28.69</v>
+      </c>
     </row>
     <row r="157" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -22633,6 +22825,102 @@
       <c r="M157">
         <v>248</v>
       </c>
+      <c r="N157">
+        <v>2022</v>
+      </c>
+      <c r="O157">
+        <v>51</v>
+      </c>
+      <c r="P157">
+        <v>162</v>
+      </c>
+      <c r="Q157">
+        <v>173</v>
+      </c>
+      <c r="R157">
+        <v>156</v>
+      </c>
+      <c r="S157">
+        <v>298</v>
+      </c>
+      <c r="T157">
+        <v>69</v>
+      </c>
+      <c r="U157">
+        <v>516</v>
+      </c>
+      <c r="V157">
+        <v>304</v>
+      </c>
+      <c r="W157">
+        <v>600</v>
+      </c>
+      <c r="X157">
+        <v>789</v>
+      </c>
+      <c r="Y157">
+        <v>111</v>
+      </c>
+      <c r="Z157">
+        <v>635</v>
+      </c>
+      <c r="AA157">
+        <v>313</v>
+      </c>
+      <c r="AC157">
+        <v>2022</v>
+      </c>
+      <c r="AD157">
+        <v>51</v>
+      </c>
+      <c r="AE157">
+        <f t="shared" si="216"/>
+        <v>37.29</v>
+      </c>
+      <c r="AF157">
+        <f t="shared" si="217"/>
+        <v>33.08</v>
+      </c>
+      <c r="AG157">
+        <f t="shared" si="218"/>
+        <v>44.44</v>
+      </c>
+      <c r="AH157">
+        <f t="shared" si="219"/>
+        <v>34.840000000000003</v>
+      </c>
+      <c r="AI157">
+        <f t="shared" si="220"/>
+        <v>30.19</v>
+      </c>
+      <c r="AJ157">
+        <f t="shared" si="221"/>
+        <v>30.96</v>
+      </c>
+      <c r="AK157">
+        <f t="shared" si="222"/>
+        <v>42.06</v>
+      </c>
+      <c r="AL157">
+        <f t="shared" si="223"/>
+        <v>20</v>
+      </c>
+      <c r="AM157">
+        <f t="shared" si="224"/>
+        <v>18.829999999999998</v>
+      </c>
+      <c r="AN157">
+        <f t="shared" si="225"/>
+        <v>35.369999999999997</v>
+      </c>
+      <c r="AO157">
+        <f t="shared" si="226"/>
+        <v>33.119999999999997</v>
+      </c>
+      <c r="AP157">
+        <f t="shared" si="227"/>
+        <v>26.21</v>
+      </c>
     </row>
     <row r="158" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -22673,6 +22961,102 @@
       </c>
       <c r="M158">
         <v>252</v>
+      </c>
+      <c r="N158">
+        <v>2022</v>
+      </c>
+      <c r="O158">
+        <v>52</v>
+      </c>
+      <c r="P158">
+        <v>155</v>
+      </c>
+      <c r="Q158">
+        <v>139</v>
+      </c>
+      <c r="R158">
+        <v>142</v>
+      </c>
+      <c r="S158">
+        <v>280</v>
+      </c>
+      <c r="T158">
+        <v>72</v>
+      </c>
+      <c r="U158">
+        <v>533</v>
+      </c>
+      <c r="V158">
+        <v>273</v>
+      </c>
+      <c r="W158">
+        <v>552</v>
+      </c>
+      <c r="X158">
+        <v>720</v>
+      </c>
+      <c r="Y158">
+        <v>100</v>
+      </c>
+      <c r="Z158">
+        <v>537</v>
+      </c>
+      <c r="AA158">
+        <v>319</v>
+      </c>
+      <c r="AC158">
+        <v>2022</v>
+      </c>
+      <c r="AD158">
+        <v>52</v>
+      </c>
+      <c r="AE158">
+        <f t="shared" si="216"/>
+        <v>30.25</v>
+      </c>
+      <c r="AF158">
+        <f t="shared" si="217"/>
+        <v>5.3</v>
+      </c>
+      <c r="AG158">
+        <f t="shared" si="218"/>
+        <v>29.09</v>
+      </c>
+      <c r="AH158">
+        <f t="shared" si="219"/>
+        <v>24.44</v>
+      </c>
+      <c r="AI158">
+        <f t="shared" si="220"/>
+        <v>33.33</v>
+      </c>
+      <c r="AJ158">
+        <f t="shared" si="221"/>
+        <v>31.93</v>
+      </c>
+      <c r="AK158">
+        <f t="shared" si="222"/>
+        <v>26.98</v>
+      </c>
+      <c r="AL158">
+        <f t="shared" si="223"/>
+        <v>8.66</v>
+      </c>
+      <c r="AM158">
+        <f t="shared" si="224"/>
+        <v>5.73</v>
+      </c>
+      <c r="AN158">
+        <f t="shared" si="225"/>
+        <v>20.48</v>
+      </c>
+      <c r="AO158">
+        <f t="shared" si="226"/>
+        <v>10.72</v>
+      </c>
+      <c r="AP158">
+        <f t="shared" si="227"/>
+        <v>26.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>